<commit_message>
Rubric, Interpolated vectors on the action groups/sequences
</commit_message>
<xml_diff>
--- a/Rubric/GAM_Project_Rubric_EpisodePrototype.xlsx
+++ b/Rubric/GAM_Project_Rubric_EpisodePrototype.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Connor\Source\Repos\Game200-Project\Rubric\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Connor\Source\Repos\Game200-project\Rubric\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,6 @@
     <sheet name="Instructor Grade" sheetId="9" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -4319,87 +4318,6 @@
     <xf numFmtId="0" fontId="27" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4427,16 +4345,94 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4446,15 +4442,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4478,14 +4465,20 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -4500,6 +4493,42 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4528,36 +4557,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="22" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="22" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -14580,47 +14579,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="145" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="146"/>
-      <c r="C1" s="146"/>
-      <c r="D1" s="147"/>
+      <c r="A1" s="118" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="120"/>
       <c r="E1" s="16"/>
-      <c r="F1" s="145" t="s">
+      <c r="F1" s="118" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="146"/>
-      <c r="H1" s="146"/>
-      <c r="I1" s="147"/>
+      <c r="G1" s="119"/>
+      <c r="H1" s="119"/>
+      <c r="I1" s="120"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
       <c r="L1" s="35"/>
     </row>
     <row r="2" spans="1:12" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="148"/>
-      <c r="B2" s="149"/>
-      <c r="C2" s="149"/>
-      <c r="D2" s="150"/>
+      <c r="A2" s="121"/>
+      <c r="B2" s="122"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="123"/>
       <c r="E2" s="16"/>
-      <c r="F2" s="148"/>
-      <c r="G2" s="149"/>
-      <c r="H2" s="149"/>
-      <c r="I2" s="150"/>
+      <c r="F2" s="121"/>
+      <c r="G2" s="122"/>
+      <c r="H2" s="122"/>
+      <c r="I2" s="123"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
       <c r="L2" s="35"/>
     </row>
     <row r="3" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="151"/>
-      <c r="B3" s="152"/>
-      <c r="C3" s="152"/>
-      <c r="D3" s="153"/>
+      <c r="A3" s="124"/>
+      <c r="B3" s="125"/>
+      <c r="C3" s="125"/>
+      <c r="D3" s="126"/>
       <c r="E3" s="16"/>
-      <c r="F3" s="151"/>
-      <c r="G3" s="152"/>
-      <c r="H3" s="152"/>
-      <c r="I3" s="153"/>
+      <c r="F3" s="124"/>
+      <c r="G3" s="125"/>
+      <c r="H3" s="125"/>
+      <c r="I3" s="126"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
       <c r="L3" s="35"/>
@@ -14640,35 +14639,35 @@
       <c r="L4" s="35"/>
     </row>
     <row r="5" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="145" t="s">
+      <c r="A5" s="118" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="146"/>
-      <c r="C5" s="146"/>
-      <c r="D5" s="147"/>
+      <c r="B5" s="119"/>
+      <c r="C5" s="119"/>
+      <c r="D5" s="120"/>
       <c r="E5" s="16"/>
-      <c r="F5" s="145" t="s">
+      <c r="F5" s="118" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="146"/>
-      <c r="H5" s="146"/>
-      <c r="I5" s="147"/>
+      <c r="G5" s="119"/>
+      <c r="H5" s="119"/>
+      <c r="I5" s="120"/>
       <c r="J5" s="6"/>
       <c r="K5" s="30"/>
       <c r="L5" s="35"/>
     </row>
     <row r="6" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="142"/>
-      <c r="B6" s="143"/>
-      <c r="C6" s="143"/>
-      <c r="D6" s="144"/>
+      <c r="A6" s="130"/>
+      <c r="B6" s="131"/>
+      <c r="C6" s="131"/>
+      <c r="D6" s="132"/>
       <c r="E6" s="16"/>
-      <c r="F6" s="142"/>
-      <c r="G6" s="143"/>
-      <c r="H6" s="143"/>
-      <c r="I6" s="144"/>
+      <c r="F6" s="130"/>
+      <c r="G6" s="131"/>
+      <c r="H6" s="131"/>
+      <c r="I6" s="132"/>
       <c r="J6" s="6"/>
-      <c r="K6" s="139" t="s">
+      <c r="K6" s="127" t="s">
         <v>29</v>
       </c>
       <c r="L6" s="35"/>
@@ -14679,42 +14678,42 @@
       <c r="C7" s="5"/>
       <c r="D7" s="37"/>
       <c r="E7" s="16"/>
-      <c r="F7" s="142"/>
-      <c r="G7" s="143"/>
-      <c r="H7" s="143"/>
-      <c r="I7" s="144"/>
+      <c r="F7" s="130"/>
+      <c r="G7" s="131"/>
+      <c r="H7" s="131"/>
+      <c r="I7" s="132"/>
       <c r="J7" s="6"/>
-      <c r="K7" s="140"/>
+      <c r="K7" s="128"/>
       <c r="L7" s="35"/>
     </row>
     <row r="8" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="145" t="s">
+      <c r="A8" s="118" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="146"/>
-      <c r="C8" s="146"/>
-      <c r="D8" s="147"/>
+      <c r="B8" s="119"/>
+      <c r="C8" s="119"/>
+      <c r="D8" s="120"/>
       <c r="E8" s="16"/>
-      <c r="F8" s="142"/>
-      <c r="G8" s="143"/>
-      <c r="H8" s="143"/>
-      <c r="I8" s="144"/>
+      <c r="F8" s="130"/>
+      <c r="G8" s="131"/>
+      <c r="H8" s="131"/>
+      <c r="I8" s="132"/>
       <c r="J8" s="6"/>
-      <c r="K8" s="140"/>
+      <c r="K8" s="128"/>
       <c r="L8" s="35"/>
     </row>
     <row r="9" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="142"/>
-      <c r="B9" s="143"/>
-      <c r="C9" s="143"/>
-      <c r="D9" s="144"/>
+      <c r="A9" s="130"/>
+      <c r="B9" s="131"/>
+      <c r="C9" s="131"/>
+      <c r="D9" s="132"/>
       <c r="E9" s="16"/>
-      <c r="F9" s="142"/>
-      <c r="G9" s="143"/>
-      <c r="H9" s="143"/>
-      <c r="I9" s="144"/>
+      <c r="F9" s="130"/>
+      <c r="G9" s="131"/>
+      <c r="H9" s="131"/>
+      <c r="I9" s="132"/>
       <c r="J9" s="6"/>
-      <c r="K9" s="141"/>
+      <c r="K9" s="129"/>
       <c r="L9" s="35"/>
     </row>
     <row r="10" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -14732,17 +14731,17 @@
       <c r="L10" s="35"/>
     </row>
     <row r="11" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="145" t="s">
+      <c r="A11" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="146"/>
-      <c r="C11" s="146"/>
-      <c r="D11" s="147"/>
+      <c r="B11" s="119"/>
+      <c r="C11" s="119"/>
+      <c r="D11" s="120"/>
       <c r="E11" s="16"/>
-      <c r="F11" s="145" t="s">
+      <c r="F11" s="118" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="147"/>
+      <c r="G11" s="120"/>
       <c r="H11" s="2" t="s">
         <v>7</v>
       </c>
@@ -14781,7 +14780,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="6"/>
-      <c r="K12" s="139" t="s">
+      <c r="K12" s="127" t="s">
         <v>8</v>
       </c>
       <c r="L12" s="35"/>
@@ -14805,7 +14804,7 @@
         <v>0</v>
       </c>
       <c r="J13" s="47"/>
-      <c r="K13" s="140"/>
+      <c r="K13" s="128"/>
       <c r="L13" s="48"/>
     </row>
     <row r="14" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -14826,7 +14825,7 @@
         <v>0</v>
       </c>
       <c r="J14" s="12"/>
-      <c r="K14" s="141"/>
+      <c r="K14" s="129"/>
       <c r="L14" s="52"/>
     </row>
     <row r="15" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -14868,10 +14867,10 @@
       <c r="C17" s="45"/>
       <c r="D17" s="46"/>
       <c r="E17" s="6"/>
-      <c r="F17" s="145" t="s">
+      <c r="F17" s="118" t="s">
         <v>17</v>
       </c>
-      <c r="G17" s="147"/>
+      <c r="G17" s="120"/>
       <c r="H17" s="2"/>
       <c r="I17" s="38">
         <v>0.75</v>
@@ -14889,16 +14888,16 @@
       <c r="F18" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="123" t="s">
+      <c r="G18" s="133" t="s">
         <v>20</v>
       </c>
-      <c r="H18" s="125"/>
+      <c r="H18" s="134"/>
       <c r="I18" s="43">
         <f>IF(LEFT(G18,6)="Entire",0,IF(LEFT(G18,6)="Custom",-0.05,-0.1))</f>
         <v>0</v>
       </c>
       <c r="J18" s="54"/>
-      <c r="K18" s="139" t="s">
+      <c r="K18" s="127" t="s">
         <v>18</v>
       </c>
       <c r="L18" s="35"/>
@@ -14912,16 +14911,16 @@
       <c r="F19" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="G19" s="129" t="s">
+      <c r="G19" s="135" t="s">
         <v>22</v>
       </c>
-      <c r="H19" s="131"/>
+      <c r="H19" s="136"/>
       <c r="I19" s="51">
         <f>IF(G19="2D Graphics and 2D Gameplay",IF(I11=0.15,-0.05,0),IF(G19="3D Graphics but 2D Gameplay",IF(I11=0.15,-0.02,-0.3),IF(I11=0.15,0,-0.3)))</f>
         <v>0</v>
       </c>
       <c r="J19" s="6"/>
-      <c r="K19" s="141"/>
+      <c r="K19" s="129"/>
       <c r="L19" s="35"/>
     </row>
     <row r="20" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -14949,7 +14948,7 @@
       <c r="C21" s="45"/>
       <c r="D21" s="46"/>
       <c r="E21" s="6"/>
-      <c r="F21" s="136" t="s">
+      <c r="F21" s="151" t="s">
         <v>23</v>
       </c>
       <c r="G21" s="55"/>
@@ -14965,17 +14964,17 @@
       <c r="C22" s="45"/>
       <c r="D22" s="46"/>
       <c r="E22" s="6"/>
-      <c r="F22" s="137"/>
+      <c r="F22" s="152"/>
       <c r="G22" s="55"/>
       <c r="H22" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="I22" s="118">
+      <c r="I22" s="137">
         <f>I20+I15</f>
         <v>0.85</v>
       </c>
       <c r="J22" s="6"/>
-      <c r="K22" s="120" t="s">
+      <c r="K22" s="139" t="s">
         <v>26</v>
       </c>
       <c r="L22" s="35"/>
@@ -14986,14 +14985,14 @@
       <c r="C23" s="45"/>
       <c r="D23" s="46"/>
       <c r="E23" s="6"/>
-      <c r="F23" s="137"/>
+      <c r="F23" s="152"/>
       <c r="G23" s="55"/>
       <c r="H23" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="I23" s="119"/>
+      <c r="I23" s="138"/>
       <c r="J23" s="6"/>
-      <c r="K23" s="121"/>
+      <c r="K23" s="140"/>
       <c r="L23" s="35"/>
     </row>
     <row r="24" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -15002,7 +15001,7 @@
       <c r="C24" s="45"/>
       <c r="D24" s="46"/>
       <c r="E24" s="6"/>
-      <c r="F24" s="138"/>
+      <c r="F24" s="153"/>
       <c r="G24" s="55"/>
       <c r="H24" s="55"/>
       <c r="I24" s="55"/>
@@ -15030,12 +15029,12 @@
       <c r="C26" s="45"/>
       <c r="D26" s="46"/>
       <c r="E26" s="16"/>
-      <c r="F26" s="122" t="s">
+      <c r="F26" s="141" t="s">
         <v>27</v>
       </c>
-      <c r="G26" s="122"/>
-      <c r="H26" s="122"/>
-      <c r="I26" s="122"/>
+      <c r="G26" s="141"/>
+      <c r="H26" s="141"/>
+      <c r="I26" s="141"/>
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
       <c r="L26" s="35"/>
@@ -15046,12 +15045,12 @@
       <c r="C27" s="45"/>
       <c r="D27" s="46"/>
       <c r="E27" s="16"/>
-      <c r="F27" s="123" t="s">
+      <c r="F27" s="133" t="s">
         <v>28</v>
       </c>
-      <c r="G27" s="124"/>
-      <c r="H27" s="124"/>
-      <c r="I27" s="125"/>
+      <c r="G27" s="142"/>
+      <c r="H27" s="142"/>
+      <c r="I27" s="134"/>
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
       <c r="L27" s="35"/>
@@ -15062,10 +15061,10 @@
       <c r="C28" s="45"/>
       <c r="D28" s="46"/>
       <c r="E28" s="16"/>
-      <c r="F28" s="126"/>
-      <c r="G28" s="127"/>
-      <c r="H28" s="127"/>
-      <c r="I28" s="128"/>
+      <c r="F28" s="143"/>
+      <c r="G28" s="144"/>
+      <c r="H28" s="144"/>
+      <c r="I28" s="145"/>
       <c r="J28" s="6"/>
       <c r="K28" s="6"/>
       <c r="L28" s="35"/>
@@ -15076,10 +15075,10 @@
       <c r="C29" s="45"/>
       <c r="D29" s="46"/>
       <c r="E29" s="16"/>
-      <c r="F29" s="126"/>
-      <c r="G29" s="127"/>
-      <c r="H29" s="127"/>
-      <c r="I29" s="128"/>
+      <c r="F29" s="143"/>
+      <c r="G29" s="144"/>
+      <c r="H29" s="144"/>
+      <c r="I29" s="145"/>
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
       <c r="L29" s="35"/>
@@ -15090,26 +15089,26 @@
       <c r="C30" s="45"/>
       <c r="D30" s="46"/>
       <c r="E30" s="16"/>
-      <c r="F30" s="126"/>
-      <c r="G30" s="127"/>
-      <c r="H30" s="127"/>
-      <c r="I30" s="128"/>
+      <c r="F30" s="143"/>
+      <c r="G30" s="144"/>
+      <c r="H30" s="144"/>
+      <c r="I30" s="145"/>
       <c r="J30" s="6"/>
       <c r="K30" s="6"/>
       <c r="L30" s="35"/>
     </row>
     <row r="31" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="132" t="s">
+      <c r="A31" s="147" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="133"/>
-      <c r="C31" s="134"/>
-      <c r="D31" s="135"/>
+      <c r="B31" s="148"/>
+      <c r="C31" s="149"/>
+      <c r="D31" s="150"/>
       <c r="E31" s="6"/>
-      <c r="F31" s="129"/>
-      <c r="G31" s="130"/>
-      <c r="H31" s="130"/>
-      <c r="I31" s="131"/>
+      <c r="F31" s="135"/>
+      <c r="G31" s="146"/>
+      <c r="H31" s="146"/>
+      <c r="I31" s="136"/>
       <c r="J31" s="6"/>
       <c r="K31" s="6"/>
       <c r="L31" s="35"/>
@@ -15130,12 +15129,13 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="A2:D3"/>
-    <mergeCell ref="F2:I3"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="F27:I31"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="F21:F24"/>
     <mergeCell ref="K12:K14"/>
     <mergeCell ref="K18:K19"/>
     <mergeCell ref="A6:D6"/>
@@ -15151,13 +15151,12 @@
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="G19:H19"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="F27:I31"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="F21:F24"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="A2:D3"/>
+    <mergeCell ref="F2:I3"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="F5:I5"/>
   </mergeCells>
   <dataValidations count="9">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A6:D6">
@@ -15214,65 +15213,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="179" t="s">
+      <c r="A1" s="189" t="s">
         <v>707</v>
       </c>
       <c r="B1" s="75"/>
-      <c r="C1" s="194" t="s">
+      <c r="C1" s="179" t="s">
         <v>690</v>
       </c>
-      <c r="D1" s="195"/>
-      <c r="E1" s="194" t="s">
+      <c r="D1" s="180"/>
+      <c r="E1" s="179" t="s">
         <v>691</v>
       </c>
-      <c r="F1" s="195"/>
-      <c r="G1" s="194" t="s">
+      <c r="F1" s="180"/>
+      <c r="G1" s="179" t="s">
         <v>692</v>
       </c>
-      <c r="H1" s="195"/>
+      <c r="H1" s="180"/>
     </row>
     <row r="2" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="180"/>
+      <c r="A2" s="190"/>
       <c r="B2" s="75"/>
-      <c r="C2" s="196" t="s">
+      <c r="C2" s="181" t="s">
         <v>689</v>
       </c>
-      <c r="D2" s="197"/>
-      <c r="E2" s="196" t="s">
+      <c r="D2" s="182"/>
+      <c r="E2" s="181" t="s">
         <v>689</v>
       </c>
-      <c r="F2" s="197"/>
-      <c r="G2" s="196" t="s">
+      <c r="F2" s="182"/>
+      <c r="G2" s="181" t="s">
         <v>689</v>
       </c>
-      <c r="H2" s="197"/>
-      <c r="J2" s="182" t="s">
+      <c r="H2" s="182"/>
+      <c r="J2" s="192" t="s">
         <v>708</v>
       </c>
-      <c r="K2" s="183"/>
-      <c r="L2" s="184"/>
+      <c r="K2" s="193"/>
+      <c r="L2" s="194"/>
     </row>
     <row r="3" spans="1:12" ht="22.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="181"/>
+      <c r="A3" s="191"/>
       <c r="B3" s="76"/>
-      <c r="C3" s="192">
+      <c r="C3" s="183">
         <f>MAX(0,MIN(1,IF((A6+C6+L6) &lt;= 0.95, ROUND(A6+C6+L6,2), FLOOR((0.95+(A6+C6+L6-0.95)/5),2))))</f>
         <v>0.85</v>
       </c>
-      <c r="D3" s="193"/>
-      <c r="E3" s="192">
+      <c r="D3" s="184"/>
+      <c r="E3" s="183">
         <f>MAX(0,MIN(1,IF((A6+E6+L6) &lt;= 0.95, ROUND(A6+E6+L6,2), FLOOR((0.95+(A6+E6+L6-0.95)/5),2))))</f>
         <v>0.85</v>
       </c>
-      <c r="F3" s="193"/>
-      <c r="G3" s="192">
+      <c r="F3" s="184"/>
+      <c r="G3" s="183">
         <f>MAX(0,MIN(1,IF((A6+G6+L6) &lt;= 0.95, ROUND(A6+G6+L6,2), FLOOR((0.95+(A6+G6+L6-0.95)/5),2))))</f>
         <v>0.85</v>
       </c>
-      <c r="H3" s="193"/>
-      <c r="J3" s="185"/>
-      <c r="K3" s="186"/>
-      <c r="L3" s="187"/>
+      <c r="H3" s="184"/>
+      <c r="J3" s="195"/>
+      <c r="K3" s="196"/>
+      <c r="L3" s="197"/>
     </row>
     <row r="4" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
@@ -15292,18 +15291,18 @@
         <v>693</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="145" t="s">
+      <c r="C5" s="118" t="s">
         <v>694</v>
       </c>
-      <c r="D5" s="147"/>
-      <c r="E5" s="145" t="s">
+      <c r="D5" s="120"/>
+      <c r="E5" s="118" t="s">
         <v>695</v>
       </c>
-      <c r="F5" s="147"/>
-      <c r="G5" s="145" t="s">
+      <c r="F5" s="120"/>
+      <c r="G5" s="118" t="s">
         <v>696</v>
       </c>
-      <c r="H5" s="147"/>
+      <c r="H5" s="120"/>
       <c r="J5" s="77" t="s">
         <v>709</v>
       </c>
@@ -15318,24 +15317,24 @@
         <v>0.85</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="189">
+      <c r="C6" s="186">
         <f>D15+D24+D33+D42+D51+D60</f>
         <v>0</v>
       </c>
-      <c r="D6" s="190"/>
-      <c r="E6" s="189">
+      <c r="D6" s="187"/>
+      <c r="E6" s="186">
         <f>F15+F24+F33+F42+F51+F60</f>
         <v>0</v>
       </c>
-      <c r="F6" s="190"/>
-      <c r="G6" s="189">
+      <c r="F6" s="187"/>
+      <c r="G6" s="186">
         <f>H15+H24+H33+H42+H51+H60</f>
         <v>0</v>
       </c>
-      <c r="H6" s="190"/>
+      <c r="H6" s="187"/>
       <c r="J6" s="92">
         <f>ABS('Student Grade'!$F$15+'Student Grade'!$D$24+'Student Grade'!$H$33+'Student Grade'!$F$42+'Student Grade'!$F$51+'Student Grade'!$F$60-$F$15-$D$24-$D$33-$H$42-$F$51-$F$60)</f>
-        <v>9.0000000000000011E-2</v>
+        <v>0.08</v>
       </c>
       <c r="K6" s="3"/>
       <c r="L6" s="90">
@@ -15346,18 +15345,18 @@
     <row r="7" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="11"/>
-      <c r="C7" s="191" t="s">
+      <c r="C7" s="188" t="s">
         <v>697</v>
       </c>
-      <c r="D7" s="191"/>
-      <c r="E7" s="191" t="s">
+      <c r="D7" s="188"/>
+      <c r="E7" s="188" t="s">
         <v>698</v>
       </c>
-      <c r="F7" s="191"/>
-      <c r="G7" s="191" t="s">
+      <c r="F7" s="188"/>
+      <c r="G7" s="188" t="s">
         <v>699</v>
       </c>
-      <c r="H7" s="191"/>
+      <c r="H7" s="188"/>
       <c r="J7" s="91"/>
       <c r="K7" s="3"/>
       <c r="L7" s="89"/>
@@ -15531,7 +15530,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J12" s="139" t="s">
+      <c r="J12" s="127" t="s">
         <v>722</v>
       </c>
       <c r="K12" s="31"/>
@@ -15569,7 +15568,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J13" s="140"/>
+      <c r="J13" s="128"/>
       <c r="K13" s="31"/>
       <c r="L13" s="104" t="s">
         <v>715</v>
@@ -15605,7 +15604,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J14" s="140"/>
+      <c r="J14" s="128"/>
       <c r="K14" s="105"/>
       <c r="L14" s="104" t="s">
         <v>716</v>
@@ -15635,7 +15634,7 @@
         <f>SUM(H9:H14)</f>
         <v>0</v>
       </c>
-      <c r="J15" s="140"/>
+      <c r="J15" s="128"/>
       <c r="K15" s="105"/>
       <c r="L15" s="104" t="s">
         <v>717</v>
@@ -15644,19 +15643,19 @@
     <row r="16" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="11"/>
-      <c r="C16" s="188" t="s">
+      <c r="C16" s="185" t="s">
         <v>697</v>
       </c>
-      <c r="D16" s="188"/>
-      <c r="E16" s="188" t="s">
+      <c r="D16" s="185"/>
+      <c r="E16" s="185" t="s">
         <v>698</v>
       </c>
-      <c r="F16" s="188"/>
-      <c r="G16" s="188" t="s">
+      <c r="F16" s="185"/>
+      <c r="G16" s="185" t="s">
         <v>699</v>
       </c>
-      <c r="H16" s="188"/>
-      <c r="J16" s="140"/>
+      <c r="H16" s="185"/>
+      <c r="J16" s="128"/>
       <c r="K16" s="105"/>
       <c r="L16" s="104" t="s">
         <v>718</v>
@@ -15687,7 +15686,7 @@
       <c r="H17" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="J17" s="140"/>
+      <c r="J17" s="128"/>
       <c r="K17" s="105"/>
       <c r="L17" s="104" t="s">
         <v>719</v>
@@ -15723,7 +15722,7 @@
         <f t="shared" ref="H18:H23" si="5">B18*G18</f>
         <v>0</v>
       </c>
-      <c r="J18" s="140"/>
+      <c r="J18" s="128"/>
       <c r="K18" s="105"/>
       <c r="L18" s="104" t="s">
         <v>720</v>
@@ -15759,7 +15758,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J19" s="141"/>
+      <c r="J19" s="129"/>
       <c r="K19" s="105"/>
       <c r="L19" s="103" t="s">
         <v>721</v>
@@ -15917,18 +15916,18 @@
     <row r="25" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="11"/>
-      <c r="C25" s="188" t="s">
+      <c r="C25" s="185" t="s">
         <v>697</v>
       </c>
-      <c r="D25" s="188"/>
-      <c r="E25" s="188" t="s">
+      <c r="D25" s="185"/>
+      <c r="E25" s="185" t="s">
         <v>698</v>
       </c>
-      <c r="F25" s="188"/>
-      <c r="G25" s="188" t="s">
+      <c r="F25" s="185"/>
+      <c r="G25" s="185" t="s">
         <v>699</v>
       </c>
-      <c r="H25" s="188"/>
+      <c r="H25" s="185"/>
     </row>
     <row r="26" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
@@ -16170,18 +16169,18 @@
     <row r="34" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3"/>
       <c r="B34" s="11"/>
-      <c r="C34" s="188" t="s">
+      <c r="C34" s="185" t="s">
         <v>697</v>
       </c>
-      <c r="D34" s="188"/>
-      <c r="E34" s="188" t="s">
+      <c r="D34" s="185"/>
+      <c r="E34" s="185" t="s">
         <v>698</v>
       </c>
-      <c r="F34" s="188"/>
-      <c r="G34" s="188" t="s">
+      <c r="F34" s="185"/>
+      <c r="G34" s="185" t="s">
         <v>699</v>
       </c>
-      <c r="H34" s="188"/>
+      <c r="H34" s="185"/>
     </row>
     <row r="35" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
@@ -16423,18 +16422,18 @@
     <row r="43" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3"/>
       <c r="B43" s="11"/>
-      <c r="C43" s="188" t="s">
+      <c r="C43" s="185" t="s">
         <v>697</v>
       </c>
-      <c r="D43" s="188"/>
-      <c r="E43" s="188" t="s">
+      <c r="D43" s="185"/>
+      <c r="E43" s="185" t="s">
         <v>698</v>
       </c>
-      <c r="F43" s="188"/>
-      <c r="G43" s="188" t="s">
+      <c r="F43" s="185"/>
+      <c r="G43" s="185" t="s">
         <v>699</v>
       </c>
-      <c r="H43" s="188"/>
+      <c r="H43" s="185"/>
     </row>
     <row r="44" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
@@ -16676,18 +16675,18 @@
     <row r="52" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="3"/>
       <c r="B52" s="11"/>
-      <c r="C52" s="188" t="s">
+      <c r="C52" s="185" t="s">
         <v>697</v>
       </c>
-      <c r="D52" s="188"/>
-      <c r="E52" s="188" t="s">
+      <c r="D52" s="185"/>
+      <c r="E52" s="185" t="s">
         <v>698</v>
       </c>
-      <c r="F52" s="188"/>
-      <c r="G52" s="188" t="s">
+      <c r="F52" s="185"/>
+      <c r="G52" s="185" t="s">
         <v>699</v>
       </c>
-      <c r="H52" s="188"/>
+      <c r="H52" s="185"/>
     </row>
     <row r="53" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
@@ -16928,27 +16927,6 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
     <mergeCell ref="C52:D52"/>
     <mergeCell ref="E52:F52"/>
     <mergeCell ref="G52:H52"/>
@@ -16965,6 +16943,27 @@
     <mergeCell ref="E43:F43"/>
     <mergeCell ref="G43:H43"/>
     <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -16991,54 +16990,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="158" t="s">
+      <c r="A1" s="157" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="159"/>
-      <c r="C1" s="159"/>
-      <c r="D1" s="159"/>
-      <c r="E1" s="159"/>
-      <c r="F1" s="160"/>
+      <c r="B1" s="158"/>
+      <c r="C1" s="158"/>
+      <c r="D1" s="158"/>
+      <c r="E1" s="158"/>
+      <c r="F1" s="159"/>
     </row>
     <row r="2" spans="1:6" ht="43.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="161" t="s">
+      <c r="A2" s="154" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="162"/>
-      <c r="C2" s="162"/>
-      <c r="D2" s="162"/>
-      <c r="E2" s="162"/>
-      <c r="F2" s="163"/>
+      <c r="B2" s="155"/>
+      <c r="C2" s="155"/>
+      <c r="D2" s="155"/>
+      <c r="E2" s="155"/>
+      <c r="F2" s="156"/>
     </row>
     <row r="3" spans="1:6" ht="43.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="164" t="s">
+      <c r="A3" s="160" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="165"/>
-      <c r="C3" s="165"/>
-      <c r="D3" s="165"/>
-      <c r="E3" s="165"/>
-      <c r="F3" s="166"/>
+      <c r="B3" s="161"/>
+      <c r="C3" s="161"/>
+      <c r="D3" s="161"/>
+      <c r="E3" s="161"/>
+      <c r="F3" s="162"/>
     </row>
     <row r="4" spans="1:6" ht="28.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="161" t="s">
+      <c r="A4" s="154" t="s">
         <v>726</v>
       </c>
-      <c r="B4" s="162"/>
-      <c r="C4" s="162"/>
-      <c r="D4" s="162"/>
-      <c r="E4" s="162"/>
-      <c r="F4" s="163"/>
+      <c r="B4" s="155"/>
+      <c r="C4" s="155"/>
+      <c r="D4" s="155"/>
+      <c r="E4" s="155"/>
+      <c r="F4" s="156"/>
     </row>
     <row r="5" spans="1:6" ht="28.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="167" t="s">
+      <c r="A5" s="163" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="168"/>
-      <c r="C5" s="168"/>
-      <c r="D5" s="168"/>
-      <c r="E5" s="168"/>
-      <c r="F5" s="169"/>
+      <c r="B5" s="164"/>
+      <c r="C5" s="164"/>
+      <c r="D5" s="164"/>
+      <c r="E5" s="164"/>
+      <c r="F5" s="165"/>
     </row>
     <row r="6" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6"/>
@@ -17067,10 +17066,10 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="164" t="s">
+      <c r="A8" s="160" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="165"/>
+      <c r="B8" s="161"/>
       <c r="C8" s="17">
         <v>0</v>
       </c>
@@ -17086,10 +17085,10 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="154" t="s">
+      <c r="A9" s="167" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="155"/>
+      <c r="B9" s="168"/>
       <c r="C9" s="12">
         <v>0</v>
       </c>
@@ -17105,10 +17104,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="171" t="s">
+      <c r="A10" s="169" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="171"/>
+      <c r="B10" s="169"/>
       <c r="C10" s="12">
         <v>0</v>
       </c>
@@ -17124,10 +17123,10 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="171" t="s">
+      <c r="A11" s="169" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="171"/>
+      <c r="B11" s="169"/>
       <c r="C11" s="12">
         <v>0</v>
       </c>
@@ -17143,10 +17142,10 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="171" t="s">
+      <c r="A12" s="169" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="171"/>
+      <c r="B12" s="169"/>
       <c r="C12" s="12">
         <v>0</v>
       </c>
@@ -17162,10 +17161,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="154" t="s">
+      <c r="A13" s="167" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="155"/>
+      <c r="B13" s="168"/>
       <c r="C13" s="12">
         <v>0</v>
       </c>
@@ -17181,10 +17180,10 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="154" t="s">
+      <c r="A14" s="167" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="155"/>
+      <c r="B14" s="168"/>
       <c r="C14" s="12">
         <v>0</v>
       </c>
@@ -17200,10 +17199,10 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="156" t="s">
+      <c r="A15" s="170" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="157"/>
+      <c r="B15" s="171"/>
       <c r="C15" s="19">
         <v>0</v>
       </c>
@@ -17220,11 +17219,11 @@
     </row>
     <row r="16" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
-      <c r="B16" s="170" t="s">
+      <c r="B16" s="166" t="s">
         <v>50</v>
       </c>
-      <c r="C16" s="170"/>
-      <c r="D16" s="170"/>
+      <c r="C16" s="166"/>
+      <c r="D16" s="166"/>
       <c r="E16" s="108">
         <f>SUM(E8:E15)</f>
         <v>0</v>
@@ -17243,88 +17242,93 @@
       <c r="A18" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="158" t="s">
+      <c r="B18" s="157" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="159"/>
-      <c r="D18" s="159"/>
-      <c r="E18" s="159"/>
-      <c r="F18" s="160"/>
+      <c r="C18" s="158"/>
+      <c r="D18" s="158"/>
+      <c r="E18" s="158"/>
+      <c r="F18" s="159"/>
     </row>
     <row r="19" spans="1:6" ht="28.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="64" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="161" t="s">
+      <c r="B19" s="154" t="s">
         <v>69</v>
       </c>
-      <c r="C19" s="162"/>
-      <c r="D19" s="162"/>
-      <c r="E19" s="162"/>
-      <c r="F19" s="163"/>
+      <c r="C19" s="155"/>
+      <c r="D19" s="155"/>
+      <c r="E19" s="155"/>
+      <c r="F19" s="156"/>
     </row>
     <row r="20" spans="1:6" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="64" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="161" t="s">
+      <c r="B20" s="154" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="162"/>
-      <c r="D20" s="162"/>
-      <c r="E20" s="162"/>
-      <c r="F20" s="163"/>
+      <c r="C20" s="155"/>
+      <c r="D20" s="155"/>
+      <c r="E20" s="155"/>
+      <c r="F20" s="156"/>
     </row>
     <row r="21" spans="1:6" ht="28.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="161" t="s">
+      <c r="B21" s="154" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="162"/>
-      <c r="D21" s="162"/>
-      <c r="E21" s="162"/>
-      <c r="F21" s="163"/>
+      <c r="C21" s="155"/>
+      <c r="D21" s="155"/>
+      <c r="E21" s="155"/>
+      <c r="F21" s="156"/>
     </row>
     <row r="22" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="64" t="s">
         <v>60</v>
       </c>
-      <c r="B22" s="161" t="s">
+      <c r="B22" s="154" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="162"/>
-      <c r="D22" s="162"/>
-      <c r="E22" s="162"/>
-      <c r="F22" s="163"/>
+      <c r="C22" s="155"/>
+      <c r="D22" s="155"/>
+      <c r="E22" s="155"/>
+      <c r="F22" s="156"/>
     </row>
     <row r="23" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="161" t="s">
+      <c r="B23" s="154" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="162"/>
-      <c r="D23" s="162"/>
-      <c r="E23" s="162"/>
-      <c r="F23" s="163"/>
+      <c r="C23" s="155"/>
+      <c r="D23" s="155"/>
+      <c r="E23" s="155"/>
+      <c r="F23" s="156"/>
     </row>
     <row r="24" spans="1:6" ht="43.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="64" t="s">
         <v>56</v>
       </c>
-      <c r="B24" s="161" t="s">
+      <c r="B24" s="154" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="162"/>
-      <c r="D24" s="162"/>
-      <c r="E24" s="162"/>
-      <c r="F24" s="163"/>
+      <c r="C24" s="155"/>
+      <c r="D24" s="155"/>
+      <c r="E24" s="155"/>
+      <c r="F24" s="156"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B19:F19"/>
     <mergeCell ref="B24:F24"/>
     <mergeCell ref="B20:F20"/>
     <mergeCell ref="A1:F1"/>
@@ -17341,11 +17345,6 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B19:F19"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -17356,8 +17355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" topLeftCell="A115" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -17382,7 +17381,7 @@
       </c>
       <c r="D1" s="7" t="str">
         <f>""&amp;COUNTIF(D$10:D$250,$A$2)&amp;" "&amp;$A$2</f>
-        <v>29 Untested</v>
+        <v>3 Untested</v>
       </c>
       <c r="E1" s="7" t="str">
         <f>""&amp;COUNTIF(E$10:E$250,$A$2)&amp;" "&amp;$A$2</f>
@@ -17399,7 +17398,7 @@
       <c r="B2" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="174" t="s">
+      <c r="C2" s="172" t="s">
         <v>882</v>
       </c>
       <c r="D2" s="66">
@@ -17422,10 +17421,10 @@
       <c r="B3" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="175"/>
+      <c r="C3" s="173"/>
       <c r="D3" s="66">
         <f>SUMPRODUCT(($A$10:$A$250="Basic")*(D$10:D$250="Missing"))+0.5*SUMPRODUCT(($A$10:$A$250="Basic")*(D$10:D$250="Partial"))</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E3" s="66">
         <f>SUMPRODUCT(($A$10:$A$250="Basic")*(E$10:E$250="Missing"))+0.5*SUMPRODUCT(($A$10:$A$250="Basic")*(E$10:E$250="Partial"))</f>
@@ -17443,7 +17442,7 @@
       <c r="B4" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="175"/>
+      <c r="C4" s="173"/>
       <c r="D4" s="66">
         <f>SUMPRODUCT(($A$10:$A$250="Intermediate")*(D$10:D$250="Missing"))+0.5*SUMPRODUCT(($A$10:$A$250="Intermediate")*(D$10:D$250="Partial"))</f>
         <v>7</v>
@@ -17464,7 +17463,7 @@
       <c r="B5" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="175"/>
+      <c r="C5" s="173"/>
       <c r="D5" s="66">
         <f>SUMPRODUCT(($A$10:$A$250="Intermediate")*(D$10:D$250="Completed"))+SUMPRODUCT(($A$10:$A$250="Intermediate")*(D$10:D$250="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$250="Intermediate")*(D$10:D$250="Partial"))</f>
         <v>9</v>
@@ -17485,7 +17484,7 @@
       <c r="B6" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="175"/>
+      <c r="C6" s="173"/>
       <c r="D6" s="66">
         <f>SUMPRODUCT(($A$10:$A$250="Advanced")*(D$10:D$250="Missing"))+0.5*SUMPRODUCT(($A$10:$A$250="Advanced")*(D$10:D$250="Partial"))</f>
         <v>3</v>
@@ -17506,7 +17505,7 @@
       <c r="B7" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="175"/>
+      <c r="C7" s="173"/>
       <c r="D7" s="66">
         <f>SUMPRODUCT(($A$10:$A$250="Advanced")*(D$10:D$250="Completed"))+SUMPRODUCT(($A$10:$A$250="Advanced")*(D$10:D$250="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$250="Advanced")*(D$10:D$250="Partial"))</f>
         <v>3</v>
@@ -17527,7 +17526,7 @@
       <c r="B8" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="175"/>
+      <c r="C8" s="173"/>
       <c r="D8" s="66">
         <f>SUMPRODUCT(($A$10:$A$250="Professional")*(D$10:D$250="Completed"))+SUMPRODUCT(($A$10:$A$250="Professional")*(D$10:D$250="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$250="Professional")*(D$10:D$250="Partial"))</f>
         <v>0</v>
@@ -17542,11 +17541,11 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="177" t="s">
+      <c r="A9" s="175" t="s">
         <v>88</v>
       </c>
-      <c r="B9" s="178"/>
-      <c r="C9" s="176"/>
+      <c r="B9" s="176"/>
+      <c r="C9" s="174"/>
       <c r="D9" s="66">
         <f>SUMPRODUCT(($A$10:$A$250="Innovative")*(D$10:D$250="Completed"))+SUMPRODUCT(($A$10:$A$250="Innovative")*(D$10:D$250="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$250="Innovative")*(D$10:D$250="Partial"))</f>
         <v>0</v>
@@ -17561,10 +17560,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="172" t="s">
+      <c r="A10" s="177" t="s">
         <v>725</v>
       </c>
-      <c r="B10" s="173"/>
+      <c r="B10" s="178"/>
       <c r="C10" s="8" t="s">
         <v>869</v>
       </c>
@@ -17687,10 +17686,10 @@
       <c r="F16" s="60"/>
     </row>
     <row r="17" spans="1:6" ht="28.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="172" t="s">
+      <c r="A17" s="177" t="s">
         <v>740</v>
       </c>
-      <c r="B17" s="173"/>
+      <c r="B17" s="178"/>
       <c r="C17" s="8" t="s">
         <v>871</v>
       </c>
@@ -17905,10 +17904,10 @@
       <c r="F28" s="60"/>
     </row>
     <row r="29" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="172" t="s">
+      <c r="A29" s="177" t="s">
         <v>741</v>
       </c>
-      <c r="B29" s="173"/>
+      <c r="B29" s="178"/>
       <c r="C29" s="8" t="s">
         <v>872</v>
       </c>
@@ -17933,7 +17932,7 @@
         <v>750</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="E30" s="8" t="s">
         <v>74</v>
@@ -17951,7 +17950,7 @@
         <v>752</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>74</v>
@@ -17969,7 +17968,7 @@
         <v>753</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>74</v>
@@ -17987,7 +17986,7 @@
         <v>786</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="E33" s="8" t="s">
         <v>74</v>
@@ -18005,7 +18004,7 @@
         <v>765</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="E34" s="8" t="s">
         <v>74</v>
@@ -18023,7 +18022,7 @@
         <v>762</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="E35" s="8" t="s">
         <v>74</v>
@@ -18041,7 +18040,7 @@
         <v>757</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="E36" s="8" t="s">
         <v>74</v>
@@ -18059,7 +18058,7 @@
         <v>768</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="E37" s="8" t="s">
         <v>74</v>
@@ -18077,7 +18076,7 @@
         <v>769</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="E38" s="8" t="s">
         <v>74</v>
@@ -18095,7 +18094,7 @@
         <v>789</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="E39" s="8" t="s">
         <v>74</v>
@@ -18113,7 +18112,7 @@
         <v>764</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="E40" s="8" t="s">
         <v>74</v>
@@ -18131,7 +18130,7 @@
         <v>766</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="E41" s="8" t="s">
         <v>74</v>
@@ -18149,7 +18148,7 @@
         <v>770</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="E42" s="8" t="s">
         <v>74</v>
@@ -18167,7 +18166,7 @@
         <v>881</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="E43" s="8" t="s">
         <v>74</v>
@@ -18185,7 +18184,7 @@
         <v>791</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="E44" s="8" t="s">
         <v>74</v>
@@ -18203,7 +18202,7 @@
         <v>784</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="E45" s="8" t="s">
         <v>74</v>
@@ -18221,7 +18220,7 @@
         <v>772</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="E46" s="8" t="s">
         <v>74</v>
@@ -18239,7 +18238,7 @@
         <v>779</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="E47" s="8" t="s">
         <v>74</v>
@@ -18257,7 +18256,7 @@
         <v>797</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="E48" s="8" t="s">
         <v>74</v>
@@ -18275,7 +18274,7 @@
         <v>793</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="E49" s="8" t="s">
         <v>74</v>
@@ -18293,7 +18292,7 @@
         <v>785</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="E50" s="8" t="s">
         <v>74</v>
@@ -18311,7 +18310,7 @@
         <v>775</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="E51" s="8" t="s">
         <v>74</v>
@@ -18329,7 +18328,7 @@
         <v>777</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="E52" s="8" t="s">
         <v>74</v>
@@ -18347,7 +18346,7 @@
         <v>781</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="E53" s="8" t="s">
         <v>74</v>
@@ -18365,7 +18364,7 @@
         <v>799</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="E54" s="8" t="s">
         <v>74</v>
@@ -18383,7 +18382,7 @@
         <v>795</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="E55" s="8" t="s">
         <v>74</v>
@@ -18391,10 +18390,10 @@
       <c r="F55" s="60"/>
     </row>
     <row r="56" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="172" t="s">
+      <c r="A56" s="177" t="s">
         <v>114</v>
       </c>
-      <c r="B56" s="173"/>
+      <c r="B56" s="178"/>
       <c r="C56" s="8" t="s">
         <v>89</v>
       </c>
@@ -18491,7 +18490,7 @@
         <v>878</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E61" s="8" t="s">
         <v>74</v>
@@ -18625,10 +18624,10 @@
       <c r="F68" s="60"/>
     </row>
     <row r="69" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="172" t="s">
+      <c r="A69" s="177" t="s">
         <v>136</v>
       </c>
-      <c r="B69" s="173"/>
+      <c r="B69" s="178"/>
       <c r="C69" s="8" t="s">
         <v>89</v>
       </c>
@@ -18789,10 +18788,10 @@
       <c r="F77" s="60"/>
     </row>
     <row r="78" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="172" t="s">
+      <c r="A78" s="177" t="s">
         <v>153</v>
       </c>
-      <c r="B78" s="173"/>
+      <c r="B78" s="178"/>
       <c r="C78" s="8" t="s">
         <v>89</v>
       </c>
@@ -18897,10 +18896,10 @@
       <c r="F83" s="60"/>
     </row>
     <row r="84" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="172" t="s">
+      <c r="A84" s="177" t="s">
         <v>164</v>
       </c>
-      <c r="B84" s="173"/>
+      <c r="B84" s="178"/>
       <c r="C84" s="8" t="s">
         <v>89</v>
       </c>
@@ -19131,10 +19130,10 @@
       <c r="F96" s="60"/>
     </row>
     <row r="97" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A97" s="172" t="s">
+      <c r="A97" s="177" t="s">
         <v>188</v>
       </c>
-      <c r="B97" s="173"/>
+      <c r="B97" s="178"/>
       <c r="C97" s="8" t="s">
         <v>89</v>
       </c>
@@ -19221,10 +19220,10 @@
       <c r="F101" s="60"/>
     </row>
     <row r="102" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A102" s="172" t="s">
+      <c r="A102" s="177" t="s">
         <v>195</v>
       </c>
-      <c r="B102" s="173"/>
+      <c r="B102" s="178"/>
       <c r="C102" s="8" t="s">
         <v>89</v>
       </c>
@@ -19367,10 +19366,10 @@
       <c r="F109" s="60"/>
     </row>
     <row r="110" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A110" s="172" t="s">
+      <c r="A110" s="177" t="s">
         <v>206</v>
       </c>
-      <c r="B110" s="173"/>
+      <c r="B110" s="178"/>
       <c r="C110" s="8" t="s">
         <v>89</v>
       </c>
@@ -19439,10 +19438,10 @@
       <c r="F113" s="60"/>
     </row>
     <row r="114" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A114" s="172" t="s">
+      <c r="A114" s="177" t="s">
         <v>213</v>
       </c>
-      <c r="B114" s="173"/>
+      <c r="B114" s="178"/>
       <c r="C114" s="8" t="s">
         <v>89</v>
       </c>
@@ -19511,10 +19510,10 @@
       <c r="F117" s="60"/>
     </row>
     <row r="118" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A118" s="172" t="s">
+      <c r="A118" s="177" t="s">
         <v>220</v>
       </c>
-      <c r="B118" s="173"/>
+      <c r="B118" s="178"/>
       <c r="C118" s="8" t="s">
         <v>824</v>
       </c>
@@ -19674,11 +19673,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C2:C9"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A56:B56"/>
     <mergeCell ref="A110:B110"/>
     <mergeCell ref="A114:B114"/>
     <mergeCell ref="A118:B118"/>
@@ -19688,6 +19682,11 @@
     <mergeCell ref="A84:B84"/>
     <mergeCell ref="A97:B97"/>
     <mergeCell ref="A102:B102"/>
+    <mergeCell ref="C2:C9"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A56:B56"/>
   </mergeCells>
   <conditionalFormatting sqref="A10 A33:A37 A39:A41 A109:A251 A95:A107 A56:A92 A14:A31">
     <cfRule type="beginsWith" dxfId="740" priority="292" stopIfTrue="1" operator="beginsWith" text="Innovative">
@@ -20671,7 +20670,7 @@
       <c r="B2" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="174" t="s">
+      <c r="C2" s="172" t="s">
         <v>863</v>
       </c>
       <c r="D2" s="66">
@@ -20694,7 +20693,7 @@
       <c r="B3" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="175"/>
+      <c r="C3" s="173"/>
       <c r="D3" s="66">
         <f>SUMPRODUCT(($A$10:$A$241="Basic")*(D$10:D$241="Missing"))+0.5*SUMPRODUCT(($A$10:$A$241="Basic")*(D$10:D$241="Partial"))</f>
         <v>0</v>
@@ -20715,7 +20714,7 @@
       <c r="B4" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="175"/>
+      <c r="C4" s="173"/>
       <c r="D4" s="66">
         <f>SUMPRODUCT(($A$10:$A$241="Intermediate")*(D$10:D$241="Missing"))+0.5*SUMPRODUCT(($A$10:$A$241="Intermediate")*(D$10:D$241="Partial"))</f>
         <v>0</v>
@@ -20736,7 +20735,7 @@
       <c r="B5" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="175"/>
+      <c r="C5" s="173"/>
       <c r="D5" s="66">
         <f>SUMPRODUCT(($A$10:$A$241="Intermediate")*(D$10:D$241="Completed"))+SUMPRODUCT(($A$10:$A$241="Intermediate")*(D$10:D$241="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$241="Intermediate")*(D$10:D$241="Partial"))</f>
         <v>0</v>
@@ -20757,7 +20756,7 @@
       <c r="B6" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="175"/>
+      <c r="C6" s="173"/>
       <c r="D6" s="66">
         <f>SUMPRODUCT(($A$10:$A$241="Advanced")*(D$10:D$241="Missing"))+0.5*SUMPRODUCT(($A$10:$A$241="Advanced")*(D$10:D$241="Partial"))</f>
         <v>0</v>
@@ -20778,7 +20777,7 @@
       <c r="B7" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="175"/>
+      <c r="C7" s="173"/>
       <c r="D7" s="66">
         <f>SUMPRODUCT(($A$10:$A$241="Advanced")*(D$10:D$241="Completed"))+SUMPRODUCT(($A$10:$A$241="Advanced")*(D$10:D$241="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$241="Advanced")*(D$10:D$241="Partial"))</f>
         <v>0</v>
@@ -20799,7 +20798,7 @@
       <c r="B8" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="175"/>
+      <c r="C8" s="173"/>
       <c r="D8" s="66">
         <f>SUMPRODUCT(($A$10:$A$241="Professional")*(D$10:D$241="Completed"))+SUMPRODUCT(($A$10:$A$241="Professional")*(D$10:D$241="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$241="Professional")*(D$10:D$241="Partial"))</f>
         <v>0</v>
@@ -20814,11 +20813,11 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="177" t="s">
+      <c r="A9" s="175" t="s">
         <v>88</v>
       </c>
-      <c r="B9" s="178"/>
-      <c r="C9" s="176"/>
+      <c r="B9" s="176"/>
+      <c r="C9" s="174"/>
       <c r="D9" s="66">
         <f>SUMPRODUCT(($A$10:$A$241="Innovative")*(D$10:D$241="Completed"))+SUMPRODUCT(($A$10:$A$241="Innovative")*(D$10:D$241="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$241="Innovative")*(D$10:D$241="Partial"))</f>
         <v>0</v>
@@ -20833,10 +20832,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="172" t="s">
+      <c r="A10" s="177" t="s">
         <v>811</v>
       </c>
-      <c r="B10" s="173"/>
+      <c r="B10" s="178"/>
       <c r="C10" s="8" t="s">
         <v>864</v>
       </c>
@@ -20923,10 +20922,10 @@
       <c r="F14" s="60"/>
     </row>
     <row r="15" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="172" t="s">
+      <c r="A15" s="177" t="s">
         <v>250</v>
       </c>
-      <c r="B15" s="173"/>
+      <c r="B15" s="178"/>
       <c r="C15" s="8" t="s">
         <v>89</v>
       </c>
@@ -21067,10 +21066,10 @@
       <c r="F22" s="60"/>
     </row>
     <row r="23" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="172" t="s">
+      <c r="A23" s="177" t="s">
         <v>258</v>
       </c>
-      <c r="B23" s="173"/>
+      <c r="B23" s="178"/>
       <c r="C23" s="8" t="s">
         <v>89</v>
       </c>
@@ -21211,10 +21210,10 @@
       <c r="F30" s="60"/>
     </row>
     <row r="31" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="172" t="s">
+      <c r="A31" s="177" t="s">
         <v>263</v>
       </c>
-      <c r="B31" s="173"/>
+      <c r="B31" s="178"/>
       <c r="C31" s="8" t="s">
         <v>89</v>
       </c>
@@ -21679,10 +21678,10 @@
       <c r="F56" s="60"/>
     </row>
     <row r="57" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="172" t="s">
+      <c r="A57" s="177" t="s">
         <v>289</v>
       </c>
-      <c r="B57" s="173"/>
+      <c r="B57" s="178"/>
       <c r="C57" s="73" t="s">
         <v>833</v>
       </c>
@@ -22057,10 +22056,10 @@
       <c r="F77" s="60"/>
     </row>
     <row r="78" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="172" t="s">
+      <c r="A78" s="177" t="s">
         <v>302</v>
       </c>
-      <c r="B78" s="173"/>
+      <c r="B78" s="178"/>
       <c r="C78" s="8" t="s">
         <v>89</v>
       </c>
@@ -23065,7 +23064,7 @@
       <c r="B2" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="174" t="s">
+      <c r="C2" s="172" t="s">
         <v>831</v>
       </c>
       <c r="D2" s="66">
@@ -23088,7 +23087,7 @@
       <c r="B3" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="175"/>
+      <c r="C3" s="173"/>
       <c r="D3" s="66">
         <f>SUMPRODUCT(($A$10:$A$177="Basic")*(D$10:D$177="Missing"))+0.5*SUMPRODUCT(($A$10:$A$177="Basic")*(D$10:D$177="Partial"))</f>
         <v>0</v>
@@ -23109,7 +23108,7 @@
       <c r="B4" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="175"/>
+      <c r="C4" s="173"/>
       <c r="D4" s="66">
         <f>SUMPRODUCT(($A$10:$A$177="Intermediate")*(D$10:D$177="Missing"))+0.5*SUMPRODUCT(($A$10:$A$177="Intermediate")*(D$10:D$177="Partial"))</f>
         <v>0</v>
@@ -23130,7 +23129,7 @@
       <c r="B5" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="175"/>
+      <c r="C5" s="173"/>
       <c r="D5" s="66">
         <f>SUMPRODUCT(($A$10:$A$177="Intermediate")*(D$10:D$177="Completed"))+SUMPRODUCT(($A$10:$A$177="Intermediate")*(D$10:D$177="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$177="Intermediate")*(D$10:D$177="Partial"))</f>
         <v>0</v>
@@ -23151,7 +23150,7 @@
       <c r="B6" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="175"/>
+      <c r="C6" s="173"/>
       <c r="D6" s="66">
         <f>SUMPRODUCT(($A$10:$A$177="Advanced")*(D$10:D$177="Missing"))+0.5*SUMPRODUCT(($A$10:$A$177="Advanced")*(D$10:D$177="Partial"))</f>
         <v>0</v>
@@ -23172,7 +23171,7 @@
       <c r="B7" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="175"/>
+      <c r="C7" s="173"/>
       <c r="D7" s="66">
         <f>SUMPRODUCT(($A$10:$A$177="Advanced")*(D$10:D$177="Completed"))+SUMPRODUCT(($A$10:$A$177="Advanced")*(D$10:D$177="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$177="Advanced")*(D$10:D$177="Partial"))</f>
         <v>0</v>
@@ -23193,7 +23192,7 @@
       <c r="B8" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="175"/>
+      <c r="C8" s="173"/>
       <c r="D8" s="66">
         <f>SUMPRODUCT(($A$10:$A$177="Professional")*(D$10:D$177="Completed"))+SUMPRODUCT(($A$10:$A$177="Professional")*(D$10:D$177="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$177="Professional")*(D$10:D$177="Partial"))</f>
         <v>0</v>
@@ -23208,11 +23207,11 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="177" t="s">
+      <c r="A9" s="175" t="s">
         <v>88</v>
       </c>
-      <c r="B9" s="178"/>
-      <c r="C9" s="176"/>
+      <c r="B9" s="176"/>
+      <c r="C9" s="174"/>
       <c r="D9" s="66">
         <f>SUMPRODUCT(($A$10:$A$177="Innovative")*(D$10:D$177="Completed"))+SUMPRODUCT(($A$10:$A$177="Innovative")*(D$10:D$177="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$177="Innovative")*(D$10:D$177="Partial"))</f>
         <v>0</v>
@@ -23227,10 +23226,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="172" t="s">
+      <c r="A10" s="177" t="s">
         <v>238</v>
       </c>
-      <c r="B10" s="173"/>
+      <c r="B10" s="178"/>
       <c r="C10" s="8" t="s">
         <v>89</v>
       </c>
@@ -23443,10 +23442,10 @@
       <c r="F21" s="60"/>
     </row>
     <row r="22" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="172" t="s">
+      <c r="A22" s="177" t="s">
         <v>535</v>
       </c>
-      <c r="B22" s="173"/>
+      <c r="B22" s="178"/>
       <c r="C22" s="8" t="s">
         <v>89</v>
       </c>
@@ -23605,10 +23604,10 @@
       <c r="F30" s="60"/>
     </row>
     <row r="31" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="172" t="s">
+      <c r="A31" s="177" t="s">
         <v>551</v>
       </c>
-      <c r="B31" s="173"/>
+      <c r="B31" s="178"/>
       <c r="C31" s="8" t="s">
         <v>89</v>
       </c>
@@ -23821,10 +23820,10 @@
       <c r="F42" s="60"/>
     </row>
     <row r="43" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="172" t="s">
+      <c r="A43" s="177" t="s">
         <v>662</v>
       </c>
-      <c r="B43" s="173"/>
+      <c r="B43" s="178"/>
       <c r="C43" s="8" t="s">
         <v>89</v>
       </c>
@@ -24113,7 +24112,7 @@
       <c r="B2" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="174" t="s">
+      <c r="C2" s="172" t="s">
         <v>385</v>
       </c>
       <c r="D2" s="66">
@@ -24136,7 +24135,7 @@
       <c r="B3" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="175"/>
+      <c r="C3" s="173"/>
       <c r="D3" s="66">
         <f>SUMPRODUCT(($A$10:$A$248="Basic")*(D$10:D$248="Missing"))+0.5*SUMPRODUCT(($A$10:$A$248="Basic")*(D$10:D$248="Partial"))</f>
         <v>0</v>
@@ -24157,7 +24156,7 @@
       <c r="B4" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="175"/>
+      <c r="C4" s="173"/>
       <c r="D4" s="66">
         <f>SUMPRODUCT(($A$10:$A$248="Intermediate")*(D$10:D$248="Missing"))+0.5*SUMPRODUCT(($A$10:$A$248="Intermediate")*(D$10:D$248="Partial"))</f>
         <v>0</v>
@@ -24178,7 +24177,7 @@
       <c r="B5" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="175"/>
+      <c r="C5" s="173"/>
       <c r="D5" s="66">
         <f>SUMPRODUCT(($A$10:$A$248="Intermediate")*(D$10:D$248="Completed"))+SUMPRODUCT(($A$10:$A$248="Intermediate")*(D$10:D$248="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$248="Intermediate")*(D$10:D$248="Partial"))</f>
         <v>0</v>
@@ -24199,7 +24198,7 @@
       <c r="B6" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="175"/>
+      <c r="C6" s="173"/>
       <c r="D6" s="66">
         <f>SUMPRODUCT(($A$10:$A$248="Advanced")*(D$10:D$248="Missing"))+0.5*SUMPRODUCT(($A$10:$A$248="Advanced")*(D$10:D$248="Partial"))</f>
         <v>0</v>
@@ -24220,7 +24219,7 @@
       <c r="B7" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="175"/>
+      <c r="C7" s="173"/>
       <c r="D7" s="66">
         <f>SUMPRODUCT(($A$10:$A$248="Advanced")*(D$10:D$248="Completed"))+SUMPRODUCT(($A$10:$A$248="Advanced")*(D$10:D$248="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$248="Advanced")*(D$10:D$248="Partial"))</f>
         <v>0</v>
@@ -24241,7 +24240,7 @@
       <c r="B8" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="175"/>
+      <c r="C8" s="173"/>
       <c r="D8" s="66">
         <f>SUMPRODUCT(($A$10:$A$248="Professional")*(D$10:D$248="Completed"))+SUMPRODUCT(($A$10:$A$248="Professional")*(D$10:D$248="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$248="Professional")*(D$10:D$248="Partial"))</f>
         <v>0</v>
@@ -24256,11 +24255,11 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="177" t="s">
+      <c r="A9" s="175" t="s">
         <v>88</v>
       </c>
-      <c r="B9" s="178"/>
-      <c r="C9" s="176"/>
+      <c r="B9" s="176"/>
+      <c r="C9" s="174"/>
       <c r="D9" s="66">
         <f>SUMPRODUCT(($A$10:$A$248="Innovative")*(D$10:D$248="Completed"))+SUMPRODUCT(($A$10:$A$248="Innovative")*(D$10:D$248="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$248="Innovative")*(D$10:D$248="Partial"))</f>
         <v>0</v>
@@ -24275,10 +24274,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="172" t="s">
+      <c r="A10" s="177" t="s">
         <v>386</v>
       </c>
-      <c r="B10" s="173"/>
+      <c r="B10" s="178"/>
       <c r="C10" s="8" t="s">
         <v>89</v>
       </c>
@@ -24383,10 +24382,10 @@
       <c r="F15" s="60"/>
     </row>
     <row r="16" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="172" t="s">
+      <c r="A16" s="177" t="s">
         <v>397</v>
       </c>
-      <c r="B16" s="173"/>
+      <c r="B16" s="178"/>
       <c r="C16" s="8" t="s">
         <v>89</v>
       </c>
@@ -24491,10 +24490,10 @@
       <c r="F21" s="60"/>
     </row>
     <row r="22" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="172" t="s">
+      <c r="A22" s="177" t="s">
         <v>408</v>
       </c>
-      <c r="B22" s="173"/>
+      <c r="B22" s="178"/>
       <c r="C22" s="8" t="s">
         <v>827</v>
       </c>
@@ -24617,10 +24616,10 @@
       <c r="F28" s="60"/>
     </row>
     <row r="29" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="172" t="s">
+      <c r="A29" s="177" t="s">
         <v>421</v>
       </c>
-      <c r="B29" s="173"/>
+      <c r="B29" s="178"/>
       <c r="C29" s="8" t="s">
         <v>825</v>
       </c>
@@ -24761,10 +24760,10 @@
       <c r="F36" s="60"/>
     </row>
     <row r="37" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="172" t="s">
+      <c r="A37" s="177" t="s">
         <v>436</v>
       </c>
-      <c r="B37" s="173"/>
+      <c r="B37" s="178"/>
       <c r="C37" s="8" t="s">
         <v>826</v>
       </c>
@@ -24887,10 +24886,10 @@
       <c r="F43" s="60"/>
     </row>
     <row r="44" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="172" t="s">
+      <c r="A44" s="177" t="s">
         <v>449</v>
       </c>
-      <c r="B44" s="173"/>
+      <c r="B44" s="178"/>
       <c r="C44" s="8" t="s">
         <v>89</v>
       </c>
@@ -25574,7 +25573,7 @@
       <c r="B2" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="174" t="s">
+      <c r="C2" s="172" t="s">
         <v>474</v>
       </c>
       <c r="D2" s="66">
@@ -25597,7 +25596,7 @@
       <c r="B3" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="175"/>
+      <c r="C3" s="173"/>
       <c r="D3" s="66">
         <f>SUMPRODUCT(($A$10:$A$227="Basic")*(D$10:D$227="Missing"))+0.5*SUMPRODUCT(($A$10:$A$227="Basic")*(D$10:D$227="Partial"))</f>
         <v>0</v>
@@ -25618,7 +25617,7 @@
       <c r="B4" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="175"/>
+      <c r="C4" s="173"/>
       <c r="D4" s="66">
         <f>SUMPRODUCT(($A$10:$A$227="Intermediate")*(D$10:D$227="Missing"))+0.5*SUMPRODUCT(($A$10:$A$227="Intermediate")*(D$10:D$227="Partial"))</f>
         <v>0</v>
@@ -25639,7 +25638,7 @@
       <c r="B5" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="175"/>
+      <c r="C5" s="173"/>
       <c r="D5" s="66">
         <f>SUMPRODUCT(($A$10:$A$227="Intermediate")*(D$10:D$227="Completed"))+SUMPRODUCT(($A$10:$A$227="Intermediate")*(D$10:D$227="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$227="Intermediate")*(D$10:D$227="Partial"))</f>
         <v>0</v>
@@ -25660,7 +25659,7 @@
       <c r="B6" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="175"/>
+      <c r="C6" s="173"/>
       <c r="D6" s="66">
         <f>SUMPRODUCT(($A$10:$A$227="Advanced")*(D$10:D$227="Missing"))+0.5*SUMPRODUCT(($A$10:$A$227="Advanced")*(D$10:D$227="Partial"))</f>
         <v>0</v>
@@ -25681,7 +25680,7 @@
       <c r="B7" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="175"/>
+      <c r="C7" s="173"/>
       <c r="D7" s="66">
         <f>SUMPRODUCT(($A$10:$A$227="Advanced")*(D$10:D$227="Completed"))+SUMPRODUCT(($A$10:$A$227="Advanced")*(D$10:D$227="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$227="Advanced")*(D$10:D$227="Partial"))</f>
         <v>0</v>
@@ -25702,7 +25701,7 @@
       <c r="B8" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="175"/>
+      <c r="C8" s="173"/>
       <c r="D8" s="66">
         <f>SUMPRODUCT(($A$10:$A$227="Professional")*(D$10:D$227="Completed"))+SUMPRODUCT(($A$10:$A$227="Professional")*(D$10:D$227="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$227="Professional")*(D$10:D$227="Partial"))</f>
         <v>0</v>
@@ -25717,11 +25716,11 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="177" t="s">
+      <c r="A9" s="175" t="s">
         <v>88</v>
       </c>
-      <c r="B9" s="178"/>
-      <c r="C9" s="176"/>
+      <c r="B9" s="176"/>
+      <c r="C9" s="174"/>
       <c r="D9" s="66">
         <f>SUMPRODUCT(($A$10:$A$227="Innovative")*(D$10:D$227="Completed"))+SUMPRODUCT(($A$10:$A$227="Innovative")*(D$10:D$227="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$227="Innovative")*(D$10:D$227="Partial"))</f>
         <v>0</v>
@@ -25736,10 +25735,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="172" t="s">
+      <c r="A10" s="177" t="s">
         <v>475</v>
       </c>
-      <c r="B10" s="173"/>
+      <c r="B10" s="178"/>
       <c r="C10" s="8" t="s">
         <v>89</v>
       </c>
@@ -26078,10 +26077,10 @@
       <c r="F28" s="60"/>
     </row>
     <row r="29" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="172" t="s">
+      <c r="A29" s="177" t="s">
         <v>512</v>
       </c>
-      <c r="B29" s="173"/>
+      <c r="B29" s="178"/>
       <c r="C29" s="8" t="s">
         <v>822</v>
       </c>
@@ -26294,10 +26293,10 @@
       <c r="F40" s="60"/>
     </row>
     <row r="41" spans="1:6" s="26" customFormat="1" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="172" t="s">
+      <c r="A41" s="177" t="s">
         <v>114</v>
       </c>
-      <c r="B41" s="173"/>
+      <c r="B41" s="178"/>
       <c r="C41" s="8" t="s">
         <v>89</v>
       </c>
@@ -26456,10 +26455,10 @@
       <c r="F49" s="60"/>
     </row>
     <row r="50" spans="1:6" s="26" customFormat="1" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="172" t="s">
+      <c r="A50" s="177" t="s">
         <v>590</v>
       </c>
-      <c r="B50" s="173"/>
+      <c r="B50" s="178"/>
       <c r="C50" s="73" t="s">
         <v>823</v>
       </c>
@@ -27028,7 +27027,7 @@
       <c r="B2" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="174" t="s">
+      <c r="C2" s="172" t="s">
         <v>611</v>
       </c>
       <c r="D2" s="66">
@@ -27051,7 +27050,7 @@
       <c r="B3" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="175"/>
+      <c r="C3" s="173"/>
       <c r="D3" s="66">
         <f>SUMPRODUCT(($A$10:$A$240="Basic")*(D$10:D$240="Missing"))+0.5*SUMPRODUCT(($A$10:$A$240="Basic")*(D$10:D$240="Partial"))</f>
         <v>0</v>
@@ -27072,7 +27071,7 @@
       <c r="B4" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="175"/>
+      <c r="C4" s="173"/>
       <c r="D4" s="66">
         <f>SUMPRODUCT(($A$10:$A$240="Intermediate")*(D$10:D$240="Missing"))+0.5*SUMPRODUCT(($A$10:$A$240="Intermediate")*(D$10:D$240="Partial"))</f>
         <v>0</v>
@@ -27093,7 +27092,7 @@
       <c r="B5" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="175"/>
+      <c r="C5" s="173"/>
       <c r="D5" s="66">
         <f>SUMPRODUCT(($A$10:$A$240="Intermediate")*(D$10:D$240="Completed"))+SUMPRODUCT(($A$10:$A$240="Intermediate")*(D$10:D$240="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$240="Intermediate")*(D$10:D$240="Partial"))</f>
         <v>0</v>
@@ -27114,7 +27113,7 @@
       <c r="B6" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="175"/>
+      <c r="C6" s="173"/>
       <c r="D6" s="66">
         <f>SUMPRODUCT(($A$10:$A$240="Advanced")*(D$10:D$240="Missing"))+0.5*SUMPRODUCT(($A$10:$A$240="Advanced")*(D$10:D$240="Partial"))</f>
         <v>0</v>
@@ -27135,7 +27134,7 @@
       <c r="B7" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="175"/>
+      <c r="C7" s="173"/>
       <c r="D7" s="66">
         <f>SUMPRODUCT(($A$10:$A$240="Advanced")*(D$10:D$240="Completed"))+SUMPRODUCT(($A$10:$A$240="Advanced")*(D$10:D$240="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$240="Advanced")*(D$10:D$240="Partial"))</f>
         <v>0</v>
@@ -27156,7 +27155,7 @@
       <c r="B8" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="175"/>
+      <c r="C8" s="173"/>
       <c r="D8" s="66">
         <f>SUMPRODUCT(($A$10:$A$240="Professional")*(D$10:D$240="Completed"))+SUMPRODUCT(($A$10:$A$240="Professional")*(D$10:D$240="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$240="Professional")*(D$10:D$240="Partial"))</f>
         <v>0</v>
@@ -27171,11 +27170,11 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="177" t="s">
+      <c r="A9" s="175" t="s">
         <v>88</v>
       </c>
-      <c r="B9" s="178"/>
-      <c r="C9" s="176"/>
+      <c r="B9" s="176"/>
+      <c r="C9" s="174"/>
       <c r="D9" s="66">
         <f>SUMPRODUCT(($A$10:$A$240="Innovative")*(D$10:D$240="Completed"))+SUMPRODUCT(($A$10:$A$240="Innovative")*(D$10:D$240="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$240="Innovative")*(D$10:D$240="Partial"))</f>
         <v>0</v>
@@ -27190,10 +27189,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="172" t="s">
+      <c r="A10" s="177" t="s">
         <v>612</v>
       </c>
-      <c r="B10" s="173"/>
+      <c r="B10" s="178"/>
       <c r="C10" s="73" t="s">
         <v>816</v>
       </c>
@@ -27406,10 +27405,10 @@
       <c r="F21" s="60"/>
     </row>
     <row r="22" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="172" t="s">
+      <c r="A22" s="177" t="s">
         <v>635</v>
       </c>
-      <c r="B22" s="173"/>
+      <c r="B22" s="178"/>
       <c r="C22" s="8" t="s">
         <v>89</v>
       </c>
@@ -27622,10 +27621,10 @@
       <c r="F33" s="60"/>
     </row>
     <row r="34" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="172" t="s">
+      <c r="A34" s="177" t="s">
         <v>812</v>
       </c>
-      <c r="B34" s="173"/>
+      <c r="B34" s="178"/>
       <c r="C34" s="8" t="s">
         <v>817</v>
       </c>
@@ -27748,10 +27747,10 @@
       <c r="F40" s="60"/>
     </row>
     <row r="41" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="172" t="s">
+      <c r="A41" s="177" t="s">
         <v>681</v>
       </c>
-      <c r="B41" s="173"/>
+      <c r="B41" s="178"/>
       <c r="C41" s="8" t="s">
         <v>89</v>
       </c>
@@ -28179,65 +28178,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="179" t="s">
+      <c r="A1" s="189" t="s">
         <v>706</v>
       </c>
       <c r="B1" s="75"/>
-      <c r="C1" s="194" t="s">
+      <c r="C1" s="179" t="s">
         <v>690</v>
       </c>
-      <c r="D1" s="195"/>
-      <c r="E1" s="194" t="s">
+      <c r="D1" s="180"/>
+      <c r="E1" s="179" t="s">
         <v>691</v>
       </c>
-      <c r="F1" s="195"/>
-      <c r="G1" s="194" t="s">
+      <c r="F1" s="180"/>
+      <c r="G1" s="179" t="s">
         <v>692</v>
       </c>
-      <c r="H1" s="195"/>
+      <c r="H1" s="180"/>
     </row>
     <row r="2" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="180"/>
+      <c r="A2" s="190"/>
       <c r="B2" s="75"/>
-      <c r="C2" s="196" t="s">
+      <c r="C2" s="181" t="s">
         <v>689</v>
       </c>
-      <c r="D2" s="197"/>
-      <c r="E2" s="196" t="s">
+      <c r="D2" s="182"/>
+      <c r="E2" s="181" t="s">
         <v>689</v>
       </c>
-      <c r="F2" s="197"/>
-      <c r="G2" s="196" t="s">
+      <c r="F2" s="182"/>
+      <c r="G2" s="181" t="s">
         <v>689</v>
       </c>
-      <c r="H2" s="197"/>
-      <c r="J2" s="182" t="s">
+      <c r="H2" s="182"/>
+      <c r="J2" s="192" t="s">
         <v>708</v>
       </c>
-      <c r="K2" s="183"/>
-      <c r="L2" s="184"/>
+      <c r="K2" s="193"/>
+      <c r="L2" s="194"/>
     </row>
     <row r="3" spans="1:12" ht="22.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="181"/>
+      <c r="A3" s="191"/>
       <c r="B3" s="76"/>
-      <c r="C3" s="192">
+      <c r="C3" s="183">
         <f>MAX(0,MIN(1,IF((A6+C6) &lt;= 0.95, ROUND(A6+C6,2), FLOOR((0.95+(A6+C6-0.95)/5),2))))</f>
-        <v>0.66</v>
-      </c>
-      <c r="D3" s="193"/>
-      <c r="E3" s="192">
+        <v>0.68</v>
+      </c>
+      <c r="D3" s="184"/>
+      <c r="E3" s="183">
         <f>MAX(0,MIN(1,IF((A6+E6) &lt;= 0.95, ROUND(A6+E6,2), FLOOR((0.95+(A6+E6-0.95)/5),2))))</f>
-        <v>0.76</v>
-      </c>
-      <c r="F3" s="193"/>
-      <c r="G3" s="192">
+        <v>0.77</v>
+      </c>
+      <c r="F3" s="184"/>
+      <c r="G3" s="183">
         <f>MAX(0,MIN(1,IF((A6+G6) &lt;= 0.95, ROUND(A6+G6,2), FLOOR((0.95+(A6+G6-0.95)/5),2))))</f>
-        <v>0.81</v>
-      </c>
-      <c r="H3" s="193"/>
-      <c r="J3" s="185"/>
-      <c r="K3" s="186"/>
-      <c r="L3" s="187"/>
+        <v>0.82</v>
+      </c>
+      <c r="H3" s="184"/>
+      <c r="J3" s="195"/>
+      <c r="K3" s="196"/>
+      <c r="L3" s="197"/>
     </row>
     <row r="4" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
@@ -28254,19 +28253,19 @@
         <v>693</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="145" t="s">
+      <c r="C5" s="118" t="s">
         <v>694</v>
       </c>
-      <c r="D5" s="147"/>
-      <c r="E5" s="145" t="s">
+      <c r="D5" s="120"/>
+      <c r="E5" s="118" t="s">
         <v>695</v>
       </c>
-      <c r="F5" s="147"/>
-      <c r="G5" s="145" t="s">
+      <c r="F5" s="120"/>
+      <c r="G5" s="118" t="s">
         <v>696</v>
       </c>
-      <c r="H5" s="147"/>
-      <c r="J5" s="139" t="s">
+      <c r="H5" s="120"/>
+      <c r="J5" s="127" t="s">
         <v>722</v>
       </c>
       <c r="K5" s="31"/>
@@ -28280,22 +28279,22 @@
         <v>0.85</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="189">
+      <c r="C6" s="186">
         <f>D15+D24+D33+D42+D51+D60</f>
-        <v>-0.19500000000000001</v>
-      </c>
-      <c r="D6" s="190"/>
-      <c r="E6" s="189">
+        <v>-0.17499999999999999</v>
+      </c>
+      <c r="D6" s="187"/>
+      <c r="E6" s="186">
         <f>F15+F24+F33+F42+F51+F60</f>
-        <v>-9.0000000000000011E-2</v>
-      </c>
-      <c r="F6" s="190"/>
-      <c r="G6" s="189">
+        <v>-0.08</v>
+      </c>
+      <c r="F6" s="187"/>
+      <c r="G6" s="186">
         <f>H15+H24+H33+H42+H51+H60</f>
-        <v>-3.7500000000000006E-2</v>
-      </c>
-      <c r="H6" s="190"/>
-      <c r="J6" s="140"/>
+        <v>-3.2500000000000001E-2</v>
+      </c>
+      <c r="H6" s="187"/>
+      <c r="J6" s="128"/>
       <c r="K6" s="31"/>
       <c r="L6" s="104" t="s">
         <v>715</v>
@@ -28304,19 +28303,19 @@
     <row r="7" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="11"/>
-      <c r="C7" s="191" t="s">
+      <c r="C7" s="188" t="s">
         <v>697</v>
       </c>
-      <c r="D7" s="191"/>
-      <c r="E7" s="191" t="s">
+      <c r="D7" s="188"/>
+      <c r="E7" s="188" t="s">
         <v>698</v>
       </c>
-      <c r="F7" s="191"/>
-      <c r="G7" s="191" t="s">
+      <c r="F7" s="188"/>
+      <c r="G7" s="188" t="s">
         <v>699</v>
       </c>
-      <c r="H7" s="191"/>
-      <c r="J7" s="140"/>
+      <c r="H7" s="188"/>
+      <c r="J7" s="128"/>
       <c r="K7" s="105"/>
       <c r="L7" s="104" t="s">
         <v>716</v>
@@ -28347,7 +28346,7 @@
       <c r="H8" s="87" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="140"/>
+      <c r="J8" s="128"/>
       <c r="K8" s="105"/>
       <c r="L8" s="104" t="s">
         <v>717</v>
@@ -28383,7 +28382,7 @@
         <f t="shared" ref="H9:H14" si="2">B9*G9</f>
         <v>0</v>
       </c>
-      <c r="J9" s="140"/>
+      <c r="J9" s="128"/>
       <c r="K9" s="105"/>
       <c r="L9" s="104" t="s">
         <v>718</v>
@@ -28396,30 +28395,30 @@
       </c>
       <c r="B10" s="11">
         <f>TCRs!$D$3</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" s="82">
         <v>-0.02</v>
       </c>
       <c r="D10" s="97">
         <f t="shared" si="0"/>
-        <v>-0.14000000000000001</v>
+        <v>-0.12</v>
       </c>
       <c r="E10" s="84">
         <v>-0.01</v>
       </c>
       <c r="F10" s="97">
         <f t="shared" si="1"/>
-        <v>-7.0000000000000007E-2</v>
+        <v>-0.06</v>
       </c>
       <c r="G10" s="100">
         <v>-5.0000000000000001E-3</v>
       </c>
       <c r="H10" s="97">
         <f t="shared" si="2"/>
-        <v>-3.5000000000000003E-2</v>
-      </c>
-      <c r="J10" s="140"/>
+        <v>-0.03</v>
+      </c>
+      <c r="J10" s="128"/>
       <c r="K10" s="105"/>
       <c r="L10" s="104" t="s">
         <v>719</v>
@@ -28455,7 +28454,7 @@
         <f t="shared" si="2"/>
         <v>-1.7500000000000002E-2</v>
       </c>
-      <c r="J11" s="140"/>
+      <c r="J11" s="128"/>
       <c r="K11" s="105"/>
       <c r="L11" s="104" t="s">
         <v>720</v>
@@ -28491,7 +28490,7 @@
         <f t="shared" si="2"/>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="J12" s="141"/>
+      <c r="J12" s="129"/>
       <c r="K12" s="105"/>
       <c r="L12" s="103" t="s">
         <v>721</v>
@@ -28567,38 +28566,38 @@
       </c>
       <c r="D15" s="99">
         <f>SUM(D9:D14)</f>
-        <v>-0.19500000000000001</v>
+        <v>-0.17499999999999999</v>
       </c>
       <c r="E15" s="79" t="s">
         <v>16</v>
       </c>
       <c r="F15" s="99">
         <f>SUM(F9:F14)</f>
-        <v>-9.0000000000000011E-2</v>
+        <v>-0.08</v>
       </c>
       <c r="G15" s="79" t="s">
         <v>16</v>
       </c>
       <c r="H15" s="99">
         <f>SUM(H9:H14)</f>
-        <v>-3.7500000000000006E-2</v>
+        <v>-3.2500000000000001E-2</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="11"/>
-      <c r="C16" s="188" t="s">
+      <c r="C16" s="185" t="s">
         <v>697</v>
       </c>
-      <c r="D16" s="188"/>
-      <c r="E16" s="188" t="s">
+      <c r="D16" s="185"/>
+      <c r="E16" s="185" t="s">
         <v>698</v>
       </c>
-      <c r="F16" s="188"/>
-      <c r="G16" s="188" t="s">
+      <c r="F16" s="185"/>
+      <c r="G16" s="185" t="s">
         <v>699</v>
       </c>
-      <c r="H16" s="188"/>
+      <c r="H16" s="185"/>
     </row>
     <row r="17" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
@@ -28840,18 +28839,18 @@
     <row r="25" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="11"/>
-      <c r="C25" s="188" t="s">
+      <c r="C25" s="185" t="s">
         <v>697</v>
       </c>
-      <c r="D25" s="188"/>
-      <c r="E25" s="188" t="s">
+      <c r="D25" s="185"/>
+      <c r="E25" s="185" t="s">
         <v>698</v>
       </c>
-      <c r="F25" s="188"/>
-      <c r="G25" s="188" t="s">
+      <c r="F25" s="185"/>
+      <c r="G25" s="185" t="s">
         <v>699</v>
       </c>
-      <c r="H25" s="188"/>
+      <c r="H25" s="185"/>
     </row>
     <row r="26" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
@@ -29093,18 +29092,18 @@
     <row r="34" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3"/>
       <c r="B34" s="11"/>
-      <c r="C34" s="188" t="s">
+      <c r="C34" s="185" t="s">
         <v>697</v>
       </c>
-      <c r="D34" s="188"/>
-      <c r="E34" s="188" t="s">
+      <c r="D34" s="185"/>
+      <c r="E34" s="185" t="s">
         <v>698</v>
       </c>
-      <c r="F34" s="188"/>
-      <c r="G34" s="188" t="s">
+      <c r="F34" s="185"/>
+      <c r="G34" s="185" t="s">
         <v>699</v>
       </c>
-      <c r="H34" s="188"/>
+      <c r="H34" s="185"/>
     </row>
     <row r="35" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
@@ -29346,18 +29345,18 @@
     <row r="43" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3"/>
       <c r="B43" s="11"/>
-      <c r="C43" s="188" t="s">
+      <c r="C43" s="185" t="s">
         <v>697</v>
       </c>
-      <c r="D43" s="188"/>
-      <c r="E43" s="188" t="s">
+      <c r="D43" s="185"/>
+      <c r="E43" s="185" t="s">
         <v>698</v>
       </c>
-      <c r="F43" s="188"/>
-      <c r="G43" s="188" t="s">
+      <c r="F43" s="185"/>
+      <c r="G43" s="185" t="s">
         <v>699</v>
       </c>
-      <c r="H43" s="188"/>
+      <c r="H43" s="185"/>
     </row>
     <row r="44" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
@@ -29599,18 +29598,18 @@
     <row r="52" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="3"/>
       <c r="B52" s="11"/>
-      <c r="C52" s="188" t="s">
+      <c r="C52" s="185" t="s">
         <v>697</v>
       </c>
-      <c r="D52" s="188"/>
-      <c r="E52" s="188" t="s">
+      <c r="D52" s="185"/>
+      <c r="E52" s="185" t="s">
         <v>698</v>
       </c>
-      <c r="F52" s="188"/>
-      <c r="G52" s="188" t="s">
+      <c r="F52" s="185"/>
+      <c r="G52" s="185" t="s">
         <v>699</v>
       </c>
-      <c r="H52" s="188"/>
+      <c r="H52" s="185"/>
     </row>
     <row r="53" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
@@ -29851,26 +29850,6 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="J2:L3"/>
     <mergeCell ref="J5:J12"/>
@@ -29887,6 +29866,26 @@
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Working on confirmation of destructive action
</commit_message>
<xml_diff>
--- a/Rubric/GAM_Project_Rubric_EpisodePrototype.xlsx
+++ b/Rubric/GAM_Project_Rubric_EpisodePrototype.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Connor\Source\Repos\Game200-project\Rubric\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Connor\Source\Repos\Game200-Project\Rubric\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2302" uniqueCount="886">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2303" uniqueCount="887">
   <si>
     <t>GAME NAME</t>
   </si>
@@ -3320,6 +3320,9 @@
   </si>
   <si>
     <t>The quit game option on the pause menu must be labeled "Quit Game". It must use this exact wording. The “Quit Game” option must actually quit the game (i.e., shut down the application), not just return you to the main menu (you can have another option to do that, but a main menu is not even required). Note that not having a confirmation when quitting the game will cause you to fail the "Confirmation of Destructive Action" TCR, not this one.</t>
+  </si>
+  <si>
+    <t>Game is supposed to have a "pixel-y" look</t>
   </si>
 </sst>
 </file>
@@ -4318,6 +4321,87 @@
     <xf numFmtId="0" fontId="27" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4345,94 +4429,16 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4442,6 +4448,15 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4465,20 +4480,14 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -4493,42 +4502,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="22" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="22" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4557,6 +4530,36 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -14579,47 +14582,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="118" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="119"/>
-      <c r="C1" s="119"/>
-      <c r="D1" s="120"/>
+      <c r="A1" s="145" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="146"/>
+      <c r="C1" s="146"/>
+      <c r="D1" s="147"/>
       <c r="E1" s="16"/>
-      <c r="F1" s="118" t="s">
+      <c r="F1" s="145" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="119"/>
-      <c r="H1" s="119"/>
-      <c r="I1" s="120"/>
+      <c r="G1" s="146"/>
+      <c r="H1" s="146"/>
+      <c r="I1" s="147"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
       <c r="L1" s="35"/>
     </row>
     <row r="2" spans="1:12" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="121"/>
-      <c r="B2" s="122"/>
-      <c r="C2" s="122"/>
-      <c r="D2" s="123"/>
+      <c r="A2" s="148"/>
+      <c r="B2" s="149"/>
+      <c r="C2" s="149"/>
+      <c r="D2" s="150"/>
       <c r="E2" s="16"/>
-      <c r="F2" s="121"/>
-      <c r="G2" s="122"/>
-      <c r="H2" s="122"/>
-      <c r="I2" s="123"/>
+      <c r="F2" s="148"/>
+      <c r="G2" s="149"/>
+      <c r="H2" s="149"/>
+      <c r="I2" s="150"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
       <c r="L2" s="35"/>
     </row>
     <row r="3" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="124"/>
-      <c r="B3" s="125"/>
-      <c r="C3" s="125"/>
-      <c r="D3" s="126"/>
+      <c r="A3" s="151"/>
+      <c r="B3" s="152"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="153"/>
       <c r="E3" s="16"/>
-      <c r="F3" s="124"/>
-      <c r="G3" s="125"/>
-      <c r="H3" s="125"/>
-      <c r="I3" s="126"/>
+      <c r="F3" s="151"/>
+      <c r="G3" s="152"/>
+      <c r="H3" s="152"/>
+      <c r="I3" s="153"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
       <c r="L3" s="35"/>
@@ -14639,35 +14642,35 @@
       <c r="L4" s="35"/>
     </row>
     <row r="5" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="118" t="s">
+      <c r="A5" s="145" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="119"/>
-      <c r="C5" s="119"/>
-      <c r="D5" s="120"/>
+      <c r="B5" s="146"/>
+      <c r="C5" s="146"/>
+      <c r="D5" s="147"/>
       <c r="E5" s="16"/>
-      <c r="F5" s="118" t="s">
+      <c r="F5" s="145" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="119"/>
-      <c r="H5" s="119"/>
-      <c r="I5" s="120"/>
+      <c r="G5" s="146"/>
+      <c r="H5" s="146"/>
+      <c r="I5" s="147"/>
       <c r="J5" s="6"/>
       <c r="K5" s="30"/>
       <c r="L5" s="35"/>
     </row>
     <row r="6" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="130"/>
-      <c r="B6" s="131"/>
-      <c r="C6" s="131"/>
-      <c r="D6" s="132"/>
+      <c r="A6" s="142"/>
+      <c r="B6" s="143"/>
+      <c r="C6" s="143"/>
+      <c r="D6" s="144"/>
       <c r="E6" s="16"/>
-      <c r="F6" s="130"/>
-      <c r="G6" s="131"/>
-      <c r="H6" s="131"/>
-      <c r="I6" s="132"/>
+      <c r="F6" s="142"/>
+      <c r="G6" s="143"/>
+      <c r="H6" s="143"/>
+      <c r="I6" s="144"/>
       <c r="J6" s="6"/>
-      <c r="K6" s="127" t="s">
+      <c r="K6" s="139" t="s">
         <v>29</v>
       </c>
       <c r="L6" s="35"/>
@@ -14678,42 +14681,42 @@
       <c r="C7" s="5"/>
       <c r="D7" s="37"/>
       <c r="E7" s="16"/>
-      <c r="F7" s="130"/>
-      <c r="G7" s="131"/>
-      <c r="H7" s="131"/>
-      <c r="I7" s="132"/>
+      <c r="F7" s="142"/>
+      <c r="G7" s="143"/>
+      <c r="H7" s="143"/>
+      <c r="I7" s="144"/>
       <c r="J7" s="6"/>
-      <c r="K7" s="128"/>
+      <c r="K7" s="140"/>
       <c r="L7" s="35"/>
     </row>
     <row r="8" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="118" t="s">
+      <c r="A8" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="119"/>
-      <c r="C8" s="119"/>
-      <c r="D8" s="120"/>
+      <c r="B8" s="146"/>
+      <c r="C8" s="146"/>
+      <c r="D8" s="147"/>
       <c r="E8" s="16"/>
-      <c r="F8" s="130"/>
-      <c r="G8" s="131"/>
-      <c r="H8" s="131"/>
-      <c r="I8" s="132"/>
+      <c r="F8" s="142"/>
+      <c r="G8" s="143"/>
+      <c r="H8" s="143"/>
+      <c r="I8" s="144"/>
       <c r="J8" s="6"/>
-      <c r="K8" s="128"/>
+      <c r="K8" s="140"/>
       <c r="L8" s="35"/>
     </row>
     <row r="9" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="130"/>
-      <c r="B9" s="131"/>
-      <c r="C9" s="131"/>
-      <c r="D9" s="132"/>
+      <c r="A9" s="142"/>
+      <c r="B9" s="143"/>
+      <c r="C9" s="143"/>
+      <c r="D9" s="144"/>
       <c r="E9" s="16"/>
-      <c r="F9" s="130"/>
-      <c r="G9" s="131"/>
-      <c r="H9" s="131"/>
-      <c r="I9" s="132"/>
+      <c r="F9" s="142"/>
+      <c r="G9" s="143"/>
+      <c r="H9" s="143"/>
+      <c r="I9" s="144"/>
       <c r="J9" s="6"/>
-      <c r="K9" s="129"/>
+      <c r="K9" s="141"/>
       <c r="L9" s="35"/>
     </row>
     <row r="10" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -14731,17 +14734,17 @@
       <c r="L10" s="35"/>
     </row>
     <row r="11" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="118" t="s">
+      <c r="A11" s="145" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="119"/>
-      <c r="C11" s="119"/>
-      <c r="D11" s="120"/>
+      <c r="B11" s="146"/>
+      <c r="C11" s="146"/>
+      <c r="D11" s="147"/>
       <c r="E11" s="16"/>
-      <c r="F11" s="118" t="s">
+      <c r="F11" s="145" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="120"/>
+      <c r="G11" s="147"/>
       <c r="H11" s="2" t="s">
         <v>7</v>
       </c>
@@ -14780,7 +14783,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="6"/>
-      <c r="K12" s="127" t="s">
+      <c r="K12" s="139" t="s">
         <v>8</v>
       </c>
       <c r="L12" s="35"/>
@@ -14804,7 +14807,7 @@
         <v>0</v>
       </c>
       <c r="J13" s="47"/>
-      <c r="K13" s="128"/>
+      <c r="K13" s="140"/>
       <c r="L13" s="48"/>
     </row>
     <row r="14" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -14825,7 +14828,7 @@
         <v>0</v>
       </c>
       <c r="J14" s="12"/>
-      <c r="K14" s="129"/>
+      <c r="K14" s="141"/>
       <c r="L14" s="52"/>
     </row>
     <row r="15" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -14867,10 +14870,10 @@
       <c r="C17" s="45"/>
       <c r="D17" s="46"/>
       <c r="E17" s="6"/>
-      <c r="F17" s="118" t="s">
+      <c r="F17" s="145" t="s">
         <v>17</v>
       </c>
-      <c r="G17" s="120"/>
+      <c r="G17" s="147"/>
       <c r="H17" s="2"/>
       <c r="I17" s="38">
         <v>0.75</v>
@@ -14888,16 +14891,16 @@
       <c r="F18" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="133" t="s">
+      <c r="G18" s="123" t="s">
         <v>20</v>
       </c>
-      <c r="H18" s="134"/>
+      <c r="H18" s="125"/>
       <c r="I18" s="43">
         <f>IF(LEFT(G18,6)="Entire",0,IF(LEFT(G18,6)="Custom",-0.05,-0.1))</f>
         <v>0</v>
       </c>
       <c r="J18" s="54"/>
-      <c r="K18" s="127" t="s">
+      <c r="K18" s="139" t="s">
         <v>18</v>
       </c>
       <c r="L18" s="35"/>
@@ -14911,16 +14914,16 @@
       <c r="F19" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="G19" s="135" t="s">
+      <c r="G19" s="129" t="s">
         <v>22</v>
       </c>
-      <c r="H19" s="136"/>
+      <c r="H19" s="131"/>
       <c r="I19" s="51">
         <f>IF(G19="2D Graphics and 2D Gameplay",IF(I11=0.15,-0.05,0),IF(G19="3D Graphics but 2D Gameplay",IF(I11=0.15,-0.02,-0.3),IF(I11=0.15,0,-0.3)))</f>
         <v>0</v>
       </c>
       <c r="J19" s="6"/>
-      <c r="K19" s="129"/>
+      <c r="K19" s="141"/>
       <c r="L19" s="35"/>
     </row>
     <row r="20" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -14948,7 +14951,7 @@
       <c r="C21" s="45"/>
       <c r="D21" s="46"/>
       <c r="E21" s="6"/>
-      <c r="F21" s="151" t="s">
+      <c r="F21" s="136" t="s">
         <v>23</v>
       </c>
       <c r="G21" s="55"/>
@@ -14964,17 +14967,17 @@
       <c r="C22" s="45"/>
       <c r="D22" s="46"/>
       <c r="E22" s="6"/>
-      <c r="F22" s="152"/>
+      <c r="F22" s="137"/>
       <c r="G22" s="55"/>
       <c r="H22" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="I22" s="137">
+      <c r="I22" s="118">
         <f>I20+I15</f>
         <v>0.85</v>
       </c>
       <c r="J22" s="6"/>
-      <c r="K22" s="139" t="s">
+      <c r="K22" s="120" t="s">
         <v>26</v>
       </c>
       <c r="L22" s="35"/>
@@ -14985,14 +14988,14 @@
       <c r="C23" s="45"/>
       <c r="D23" s="46"/>
       <c r="E23" s="6"/>
-      <c r="F23" s="152"/>
+      <c r="F23" s="137"/>
       <c r="G23" s="55"/>
       <c r="H23" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="I23" s="138"/>
+      <c r="I23" s="119"/>
       <c r="J23" s="6"/>
-      <c r="K23" s="140"/>
+      <c r="K23" s="121"/>
       <c r="L23" s="35"/>
     </row>
     <row r="24" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -15001,7 +15004,7 @@
       <c r="C24" s="45"/>
       <c r="D24" s="46"/>
       <c r="E24" s="6"/>
-      <c r="F24" s="153"/>
+      <c r="F24" s="138"/>
       <c r="G24" s="55"/>
       <c r="H24" s="55"/>
       <c r="I24" s="55"/>
@@ -15029,12 +15032,12 @@
       <c r="C26" s="45"/>
       <c r="D26" s="46"/>
       <c r="E26" s="16"/>
-      <c r="F26" s="141" t="s">
+      <c r="F26" s="122" t="s">
         <v>27</v>
       </c>
-      <c r="G26" s="141"/>
-      <c r="H26" s="141"/>
-      <c r="I26" s="141"/>
+      <c r="G26" s="122"/>
+      <c r="H26" s="122"/>
+      <c r="I26" s="122"/>
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
       <c r="L26" s="35"/>
@@ -15045,12 +15048,12 @@
       <c r="C27" s="45"/>
       <c r="D27" s="46"/>
       <c r="E27" s="16"/>
-      <c r="F27" s="133" t="s">
+      <c r="F27" s="123" t="s">
         <v>28</v>
       </c>
-      <c r="G27" s="142"/>
-      <c r="H27" s="142"/>
-      <c r="I27" s="134"/>
+      <c r="G27" s="124"/>
+      <c r="H27" s="124"/>
+      <c r="I27" s="125"/>
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
       <c r="L27" s="35"/>
@@ -15061,10 +15064,10 @@
       <c r="C28" s="45"/>
       <c r="D28" s="46"/>
       <c r="E28" s="16"/>
-      <c r="F28" s="143"/>
-      <c r="G28" s="144"/>
-      <c r="H28" s="144"/>
-      <c r="I28" s="145"/>
+      <c r="F28" s="126"/>
+      <c r="G28" s="127"/>
+      <c r="H28" s="127"/>
+      <c r="I28" s="128"/>
       <c r="J28" s="6"/>
       <c r="K28" s="6"/>
       <c r="L28" s="35"/>
@@ -15075,10 +15078,10 @@
       <c r="C29" s="45"/>
       <c r="D29" s="46"/>
       <c r="E29" s="16"/>
-      <c r="F29" s="143"/>
-      <c r="G29" s="144"/>
-      <c r="H29" s="144"/>
-      <c r="I29" s="145"/>
+      <c r="F29" s="126"/>
+      <c r="G29" s="127"/>
+      <c r="H29" s="127"/>
+      <c r="I29" s="128"/>
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
       <c r="L29" s="35"/>
@@ -15089,26 +15092,26 @@
       <c r="C30" s="45"/>
       <c r="D30" s="46"/>
       <c r="E30" s="16"/>
-      <c r="F30" s="143"/>
-      <c r="G30" s="144"/>
-      <c r="H30" s="144"/>
-      <c r="I30" s="145"/>
+      <c r="F30" s="126"/>
+      <c r="G30" s="127"/>
+      <c r="H30" s="127"/>
+      <c r="I30" s="128"/>
       <c r="J30" s="6"/>
       <c r="K30" s="6"/>
       <c r="L30" s="35"/>
     </row>
     <row r="31" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="147" t="s">
+      <c r="A31" s="132" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="148"/>
-      <c r="C31" s="149"/>
-      <c r="D31" s="150"/>
+      <c r="B31" s="133"/>
+      <c r="C31" s="134"/>
+      <c r="D31" s="135"/>
       <c r="E31" s="6"/>
-      <c r="F31" s="135"/>
-      <c r="G31" s="146"/>
-      <c r="H31" s="146"/>
-      <c r="I31" s="136"/>
+      <c r="F31" s="129"/>
+      <c r="G31" s="130"/>
+      <c r="H31" s="130"/>
+      <c r="I31" s="131"/>
       <c r="J31" s="6"/>
       <c r="K31" s="6"/>
       <c r="L31" s="35"/>
@@ -15129,13 +15132,12 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="F27:I31"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="F21:F24"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="A2:D3"/>
+    <mergeCell ref="F2:I3"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="F5:I5"/>
     <mergeCell ref="K12:K14"/>
     <mergeCell ref="K18:K19"/>
     <mergeCell ref="A6:D6"/>
@@ -15151,12 +15153,13 @@
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="G19:H19"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="A2:D3"/>
-    <mergeCell ref="F2:I3"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="F27:I31"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="F21:F24"/>
   </mergeCells>
   <dataValidations count="9">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A6:D6">
@@ -15213,65 +15216,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="189" t="s">
+      <c r="A1" s="179" t="s">
         <v>706</v>
       </c>
       <c r="B1" s="75"/>
-      <c r="C1" s="179" t="s">
+      <c r="C1" s="194" t="s">
         <v>689</v>
       </c>
-      <c r="D1" s="180"/>
-      <c r="E1" s="179" t="s">
+      <c r="D1" s="195"/>
+      <c r="E1" s="194" t="s">
         <v>690</v>
       </c>
-      <c r="F1" s="180"/>
-      <c r="G1" s="179" t="s">
+      <c r="F1" s="195"/>
+      <c r="G1" s="194" t="s">
         <v>691</v>
       </c>
-      <c r="H1" s="180"/>
+      <c r="H1" s="195"/>
     </row>
     <row r="2" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="190"/>
+      <c r="A2" s="180"/>
       <c r="B2" s="75"/>
-      <c r="C2" s="181" t="s">
+      <c r="C2" s="196" t="s">
         <v>688</v>
       </c>
-      <c r="D2" s="182"/>
-      <c r="E2" s="181" t="s">
+      <c r="D2" s="197"/>
+      <c r="E2" s="196" t="s">
         <v>688</v>
       </c>
-      <c r="F2" s="182"/>
-      <c r="G2" s="181" t="s">
+      <c r="F2" s="197"/>
+      <c r="G2" s="196" t="s">
         <v>688</v>
       </c>
-      <c r="H2" s="182"/>
-      <c r="J2" s="192" t="s">
+      <c r="H2" s="197"/>
+      <c r="J2" s="182" t="s">
         <v>707</v>
       </c>
-      <c r="K2" s="193"/>
-      <c r="L2" s="194"/>
+      <c r="K2" s="183"/>
+      <c r="L2" s="184"/>
     </row>
     <row r="3" spans="1:12" ht="22.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="191"/>
+      <c r="A3" s="181"/>
       <c r="B3" s="76"/>
-      <c r="C3" s="183">
+      <c r="C3" s="192">
         <f>MAX(0,MIN(1,IF((A6+C6+L6) &lt;= 0.95, ROUND(A6+C6+L6,2), FLOOR((0.95+(A6+C6+L6-0.95)/5),2))))</f>
         <v>0.85</v>
       </c>
-      <c r="D3" s="184"/>
-      <c r="E3" s="183">
+      <c r="D3" s="193"/>
+      <c r="E3" s="192">
         <f>MAX(0,MIN(1,IF((A6+E6+L6) &lt;= 0.95, ROUND(A6+E6+L6,2), FLOOR((0.95+(A6+E6+L6-0.95)/5),2))))</f>
         <v>0.85</v>
       </c>
-      <c r="F3" s="184"/>
-      <c r="G3" s="183">
+      <c r="F3" s="193"/>
+      <c r="G3" s="192">
         <f>MAX(0,MIN(1,IF((A6+G6+L6) &lt;= 0.95, ROUND(A6+G6+L6,2), FLOOR((0.95+(A6+G6+L6-0.95)/5),2))))</f>
         <v>0.85</v>
       </c>
-      <c r="H3" s="184"/>
-      <c r="J3" s="195"/>
-      <c r="K3" s="196"/>
-      <c r="L3" s="197"/>
+      <c r="H3" s="193"/>
+      <c r="J3" s="185"/>
+      <c r="K3" s="186"/>
+      <c r="L3" s="187"/>
     </row>
     <row r="4" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
@@ -15291,18 +15294,18 @@
         <v>692</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="118" t="s">
+      <c r="C5" s="145" t="s">
         <v>693</v>
       </c>
-      <c r="D5" s="120"/>
-      <c r="E5" s="118" t="s">
+      <c r="D5" s="147"/>
+      <c r="E5" s="145" t="s">
         <v>694</v>
       </c>
-      <c r="F5" s="120"/>
-      <c r="G5" s="118" t="s">
+      <c r="F5" s="147"/>
+      <c r="G5" s="145" t="s">
         <v>695</v>
       </c>
-      <c r="H5" s="120"/>
+      <c r="H5" s="147"/>
       <c r="J5" s="77" t="s">
         <v>708</v>
       </c>
@@ -15317,24 +15320,24 @@
         <v>0.85</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="186">
+      <c r="C6" s="189">
         <f>D15+D24+D33+D42+D51+D60</f>
         <v>0</v>
       </c>
-      <c r="D6" s="187"/>
-      <c r="E6" s="186">
+      <c r="D6" s="190"/>
+      <c r="E6" s="189">
         <f>F15+F24+F33+F42+F51+F60</f>
         <v>0</v>
       </c>
-      <c r="F6" s="187"/>
-      <c r="G6" s="186">
+      <c r="F6" s="190"/>
+      <c r="G6" s="189">
         <f>H15+H24+H33+H42+H51+H60</f>
         <v>0</v>
       </c>
-      <c r="H6" s="187"/>
+      <c r="H6" s="190"/>
       <c r="J6" s="92">
         <f>ABS('Student Grade'!$F$15+'Student Grade'!$D$24+'Student Grade'!$H$33+'Student Grade'!$F$42+'Student Grade'!$F$51+'Student Grade'!$F$60-$F$15-$D$24-$D$33-$H$42-$F$51-$F$60)</f>
-        <v>0.13500000000000001</v>
+        <v>0.125</v>
       </c>
       <c r="K6" s="3"/>
       <c r="L6" s="90">
@@ -15345,18 +15348,18 @@
     <row r="7" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="11"/>
-      <c r="C7" s="188" t="s">
+      <c r="C7" s="191" t="s">
         <v>696</v>
       </c>
-      <c r="D7" s="188"/>
-      <c r="E7" s="188" t="s">
+      <c r="D7" s="191"/>
+      <c r="E7" s="191" t="s">
         <v>697</v>
       </c>
-      <c r="F7" s="188"/>
-      <c r="G7" s="188" t="s">
+      <c r="F7" s="191"/>
+      <c r="G7" s="191" t="s">
         <v>698</v>
       </c>
-      <c r="H7" s="188"/>
+      <c r="H7" s="191"/>
       <c r="J7" s="91"/>
       <c r="K7" s="3"/>
       <c r="L7" s="89"/>
@@ -15530,7 +15533,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J12" s="127" t="s">
+      <c r="J12" s="139" t="s">
         <v>721</v>
       </c>
       <c r="K12" s="31"/>
@@ -15568,7 +15571,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J13" s="128"/>
+      <c r="J13" s="140"/>
       <c r="K13" s="31"/>
       <c r="L13" s="104" t="s">
         <v>714</v>
@@ -15604,7 +15607,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J14" s="128"/>
+      <c r="J14" s="140"/>
       <c r="K14" s="105"/>
       <c r="L14" s="104" t="s">
         <v>715</v>
@@ -15634,7 +15637,7 @@
         <f>SUM(H9:H14)</f>
         <v>0</v>
       </c>
-      <c r="J15" s="128"/>
+      <c r="J15" s="140"/>
       <c r="K15" s="105"/>
       <c r="L15" s="104" t="s">
         <v>716</v>
@@ -15643,19 +15646,19 @@
     <row r="16" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="11"/>
-      <c r="C16" s="185" t="s">
+      <c r="C16" s="188" t="s">
         <v>696</v>
       </c>
-      <c r="D16" s="185"/>
-      <c r="E16" s="185" t="s">
+      <c r="D16" s="188"/>
+      <c r="E16" s="188" t="s">
         <v>697</v>
       </c>
-      <c r="F16" s="185"/>
-      <c r="G16" s="185" t="s">
+      <c r="F16" s="188"/>
+      <c r="G16" s="188" t="s">
         <v>698</v>
       </c>
-      <c r="H16" s="185"/>
-      <c r="J16" s="128"/>
+      <c r="H16" s="188"/>
+      <c r="J16" s="140"/>
       <c r="K16" s="105"/>
       <c r="L16" s="104" t="s">
         <v>717</v>
@@ -15686,7 +15689,7 @@
       <c r="H17" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="J17" s="128"/>
+      <c r="J17" s="140"/>
       <c r="K17" s="105"/>
       <c r="L17" s="104" t="s">
         <v>718</v>
@@ -15722,7 +15725,7 @@
         <f t="shared" ref="H18:H23" si="5">B18*G18</f>
         <v>0</v>
       </c>
-      <c r="J18" s="128"/>
+      <c r="J18" s="140"/>
       <c r="K18" s="105"/>
       <c r="L18" s="104" t="s">
         <v>719</v>
@@ -15758,7 +15761,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J19" s="129"/>
+      <c r="J19" s="141"/>
       <c r="K19" s="105"/>
       <c r="L19" s="103" t="s">
         <v>720</v>
@@ -15916,18 +15919,18 @@
     <row r="25" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="11"/>
-      <c r="C25" s="185" t="s">
+      <c r="C25" s="188" t="s">
         <v>696</v>
       </c>
-      <c r="D25" s="185"/>
-      <c r="E25" s="185" t="s">
+      <c r="D25" s="188"/>
+      <c r="E25" s="188" t="s">
         <v>697</v>
       </c>
-      <c r="F25" s="185"/>
-      <c r="G25" s="185" t="s">
+      <c r="F25" s="188"/>
+      <c r="G25" s="188" t="s">
         <v>698</v>
       </c>
-      <c r="H25" s="185"/>
+      <c r="H25" s="188"/>
     </row>
     <row r="26" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
@@ -16169,18 +16172,18 @@
     <row r="34" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3"/>
       <c r="B34" s="11"/>
-      <c r="C34" s="185" t="s">
+      <c r="C34" s="188" t="s">
         <v>696</v>
       </c>
-      <c r="D34" s="185"/>
-      <c r="E34" s="185" t="s">
+      <c r="D34" s="188"/>
+      <c r="E34" s="188" t="s">
         <v>697</v>
       </c>
-      <c r="F34" s="185"/>
-      <c r="G34" s="185" t="s">
+      <c r="F34" s="188"/>
+      <c r="G34" s="188" t="s">
         <v>698</v>
       </c>
-      <c r="H34" s="185"/>
+      <c r="H34" s="188"/>
     </row>
     <row r="35" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
@@ -16422,18 +16425,18 @@
     <row r="43" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3"/>
       <c r="B43" s="11"/>
-      <c r="C43" s="185" t="s">
+      <c r="C43" s="188" t="s">
         <v>696</v>
       </c>
-      <c r="D43" s="185"/>
-      <c r="E43" s="185" t="s">
+      <c r="D43" s="188"/>
+      <c r="E43" s="188" t="s">
         <v>697</v>
       </c>
-      <c r="F43" s="185"/>
-      <c r="G43" s="185" t="s">
+      <c r="F43" s="188"/>
+      <c r="G43" s="188" t="s">
         <v>698</v>
       </c>
-      <c r="H43" s="185"/>
+      <c r="H43" s="188"/>
     </row>
     <row r="44" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
@@ -16675,18 +16678,18 @@
     <row r="52" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="3"/>
       <c r="B52" s="11"/>
-      <c r="C52" s="185" t="s">
+      <c r="C52" s="188" t="s">
         <v>696</v>
       </c>
-      <c r="D52" s="185"/>
-      <c r="E52" s="185" t="s">
+      <c r="D52" s="188"/>
+      <c r="E52" s="188" t="s">
         <v>697</v>
       </c>
-      <c r="F52" s="185"/>
-      <c r="G52" s="185" t="s">
+      <c r="F52" s="188"/>
+      <c r="G52" s="188" t="s">
         <v>698</v>
       </c>
-      <c r="H52" s="185"/>
+      <c r="H52" s="188"/>
     </row>
     <row r="53" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
@@ -16927,6 +16930,27 @@
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
     <mergeCell ref="C52:D52"/>
     <mergeCell ref="E52:F52"/>
     <mergeCell ref="G52:H52"/>
@@ -16943,27 +16967,6 @@
     <mergeCell ref="E43:F43"/>
     <mergeCell ref="G43:H43"/>
     <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -16990,54 +16993,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="157" t="s">
+      <c r="A1" s="158" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="158"/>
-      <c r="C1" s="158"/>
-      <c r="D1" s="158"/>
-      <c r="E1" s="158"/>
-      <c r="F1" s="159"/>
+      <c r="B1" s="159"/>
+      <c r="C1" s="159"/>
+      <c r="D1" s="159"/>
+      <c r="E1" s="159"/>
+      <c r="F1" s="160"/>
     </row>
     <row r="2" spans="1:6" ht="43.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="154" t="s">
+      <c r="A2" s="161" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="155"/>
-      <c r="C2" s="155"/>
-      <c r="D2" s="155"/>
-      <c r="E2" s="155"/>
-      <c r="F2" s="156"/>
+      <c r="B2" s="162"/>
+      <c r="C2" s="162"/>
+      <c r="D2" s="162"/>
+      <c r="E2" s="162"/>
+      <c r="F2" s="163"/>
     </row>
     <row r="3" spans="1:6" ht="43.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="160" t="s">
+      <c r="A3" s="164" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="161"/>
-      <c r="C3" s="161"/>
-      <c r="D3" s="161"/>
-      <c r="E3" s="161"/>
-      <c r="F3" s="162"/>
+      <c r="B3" s="165"/>
+      <c r="C3" s="165"/>
+      <c r="D3" s="165"/>
+      <c r="E3" s="165"/>
+      <c r="F3" s="166"/>
     </row>
     <row r="4" spans="1:6" ht="28.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="154" t="s">
+      <c r="A4" s="161" t="s">
         <v>725</v>
       </c>
-      <c r="B4" s="155"/>
-      <c r="C4" s="155"/>
-      <c r="D4" s="155"/>
-      <c r="E4" s="155"/>
-      <c r="F4" s="156"/>
+      <c r="B4" s="162"/>
+      <c r="C4" s="162"/>
+      <c r="D4" s="162"/>
+      <c r="E4" s="162"/>
+      <c r="F4" s="163"/>
     </row>
     <row r="5" spans="1:6" ht="28.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="163" t="s">
+      <c r="A5" s="167" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="164"/>
-      <c r="C5" s="164"/>
-      <c r="D5" s="164"/>
-      <c r="E5" s="164"/>
-      <c r="F5" s="165"/>
+      <c r="B5" s="168"/>
+      <c r="C5" s="168"/>
+      <c r="D5" s="168"/>
+      <c r="E5" s="168"/>
+      <c r="F5" s="169"/>
     </row>
     <row r="6" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6"/>
@@ -17066,10 +17069,10 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="160" t="s">
+      <c r="A8" s="164" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="161"/>
+      <c r="B8" s="165"/>
       <c r="C8" s="17">
         <v>0</v>
       </c>
@@ -17085,10 +17088,10 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="167" t="s">
+      <c r="A9" s="154" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="168"/>
+      <c r="B9" s="155"/>
       <c r="C9" s="12">
         <v>0</v>
       </c>
@@ -17104,10 +17107,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="169" t="s">
+      <c r="A10" s="171" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="169"/>
+      <c r="B10" s="171"/>
       <c r="C10" s="12">
         <v>0</v>
       </c>
@@ -17123,10 +17126,10 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="169" t="s">
+      <c r="A11" s="171" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="169"/>
+      <c r="B11" s="171"/>
       <c r="C11" s="12">
         <v>0</v>
       </c>
@@ -17142,10 +17145,10 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="169" t="s">
+      <c r="A12" s="171" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="169"/>
+      <c r="B12" s="171"/>
       <c r="C12" s="12">
         <v>0</v>
       </c>
@@ -17161,10 +17164,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="167" t="s">
+      <c r="A13" s="154" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="168"/>
+      <c r="B13" s="155"/>
       <c r="C13" s="12">
         <v>0</v>
       </c>
@@ -17180,10 +17183,10 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="167" t="s">
+      <c r="A14" s="154" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="168"/>
+      <c r="B14" s="155"/>
       <c r="C14" s="12">
         <v>0</v>
       </c>
@@ -17199,10 +17202,10 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="170" t="s">
+      <c r="A15" s="156" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="171"/>
+      <c r="B15" s="157"/>
       <c r="C15" s="19">
         <v>0</v>
       </c>
@@ -17219,11 +17222,11 @@
     </row>
     <row r="16" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
-      <c r="B16" s="166" t="s">
+      <c r="B16" s="170" t="s">
         <v>50</v>
       </c>
-      <c r="C16" s="166"/>
-      <c r="D16" s="166"/>
+      <c r="C16" s="170"/>
+      <c r="D16" s="170"/>
       <c r="E16" s="108">
         <f>SUM(E8:E15)</f>
         <v>0</v>
@@ -17242,93 +17245,88 @@
       <c r="A18" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="157" t="s">
+      <c r="B18" s="158" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="158"/>
-      <c r="D18" s="158"/>
-      <c r="E18" s="158"/>
-      <c r="F18" s="159"/>
+      <c r="C18" s="159"/>
+      <c r="D18" s="159"/>
+      <c r="E18" s="159"/>
+      <c r="F18" s="160"/>
     </row>
     <row r="19" spans="1:6" ht="28.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="64" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="154" t="s">
+      <c r="B19" s="161" t="s">
         <v>69</v>
       </c>
-      <c r="C19" s="155"/>
-      <c r="D19" s="155"/>
-      <c r="E19" s="155"/>
-      <c r="F19" s="156"/>
+      <c r="C19" s="162"/>
+      <c r="D19" s="162"/>
+      <c r="E19" s="162"/>
+      <c r="F19" s="163"/>
     </row>
     <row r="20" spans="1:6" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="64" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="154" t="s">
+      <c r="B20" s="161" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="155"/>
-      <c r="D20" s="155"/>
-      <c r="E20" s="155"/>
-      <c r="F20" s="156"/>
+      <c r="C20" s="162"/>
+      <c r="D20" s="162"/>
+      <c r="E20" s="162"/>
+      <c r="F20" s="163"/>
     </row>
     <row r="21" spans="1:6" ht="28.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="154" t="s">
+      <c r="B21" s="161" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="155"/>
-      <c r="D21" s="155"/>
-      <c r="E21" s="155"/>
-      <c r="F21" s="156"/>
+      <c r="C21" s="162"/>
+      <c r="D21" s="162"/>
+      <c r="E21" s="162"/>
+      <c r="F21" s="163"/>
     </row>
     <row r="22" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="64" t="s">
         <v>60</v>
       </c>
-      <c r="B22" s="154" t="s">
+      <c r="B22" s="161" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="155"/>
-      <c r="D22" s="155"/>
-      <c r="E22" s="155"/>
-      <c r="F22" s="156"/>
+      <c r="C22" s="162"/>
+      <c r="D22" s="162"/>
+      <c r="E22" s="162"/>
+      <c r="F22" s="163"/>
     </row>
     <row r="23" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="154" t="s">
+      <c r="B23" s="161" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="155"/>
-      <c r="D23" s="155"/>
-      <c r="E23" s="155"/>
-      <c r="F23" s="156"/>
+      <c r="C23" s="162"/>
+      <c r="D23" s="162"/>
+      <c r="E23" s="162"/>
+      <c r="F23" s="163"/>
     </row>
     <row r="24" spans="1:6" ht="43.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="64" t="s">
         <v>56</v>
       </c>
-      <c r="B24" s="154" t="s">
+      <c r="B24" s="161" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="155"/>
-      <c r="D24" s="155"/>
-      <c r="E24" s="155"/>
-      <c r="F24" s="156"/>
+      <c r="C24" s="162"/>
+      <c r="D24" s="162"/>
+      <c r="E24" s="162"/>
+      <c r="F24" s="163"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B19:F19"/>
     <mergeCell ref="B24:F24"/>
     <mergeCell ref="B20:F20"/>
     <mergeCell ref="A1:F1"/>
@@ -17345,6 +17343,11 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B19:F19"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -17355,8 +17358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C93" sqref="C93"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -17398,7 +17401,7 @@
       <c r="B2" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="172" t="s">
+      <c r="C2" s="174" t="s">
         <v>881</v>
       </c>
       <c r="D2" s="66">
@@ -17421,7 +17424,7 @@
       <c r="B3" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="173"/>
+      <c r="C3" s="175"/>
       <c r="D3" s="66">
         <f>SUMPRODUCT(($A$10:$A$250="Basic")*(D$10:D$250="Missing"))+0.5*SUMPRODUCT(($A$10:$A$250="Basic")*(D$10:D$250="Partial"))</f>
         <v>6</v>
@@ -17442,10 +17445,10 @@
       <c r="B4" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="173"/>
+      <c r="C4" s="175"/>
       <c r="D4" s="66">
         <f>SUMPRODUCT(($A$10:$A$250="Intermediate")*(D$10:D$250="Missing"))+0.5*SUMPRODUCT(($A$10:$A$250="Intermediate")*(D$10:D$250="Partial"))</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E4" s="66">
         <f>SUMPRODUCT(($A$10:$A$250="Intermediate")*(E$10:E$250="Missing"))+0.5*SUMPRODUCT(($A$10:$A$250="Intermediate")*(E$10:E$250="Partial"))</f>
@@ -17463,10 +17466,10 @@
       <c r="B5" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="173"/>
+      <c r="C5" s="175"/>
       <c r="D5" s="66">
         <f>SUMPRODUCT(($A$10:$A$250="Intermediate")*(D$10:D$250="Completed"))+SUMPRODUCT(($A$10:$A$250="Intermediate")*(D$10:D$250="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$250="Intermediate")*(D$10:D$250="Partial"))</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E5" s="66">
         <f>SUMPRODUCT(($A$10:$A$250="Intermediate")*(E$10:E$250="Completed"))+SUMPRODUCT(($A$10:$A$250="Intermediate")*(E$10:E$250="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$250="Intermediate")*(E$10:E$250="Partial"))</f>
@@ -17484,7 +17487,7 @@
       <c r="B6" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="173"/>
+      <c r="C6" s="175"/>
       <c r="D6" s="66">
         <f>SUMPRODUCT(($A$10:$A$250="Advanced")*(D$10:D$250="Missing"))+0.5*SUMPRODUCT(($A$10:$A$250="Advanced")*(D$10:D$250="Partial"))</f>
         <v>3</v>
@@ -17505,7 +17508,7 @@
       <c r="B7" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="173"/>
+      <c r="C7" s="175"/>
       <c r="D7" s="66">
         <f>SUMPRODUCT(($A$10:$A$250="Advanced")*(D$10:D$250="Completed"))+SUMPRODUCT(($A$10:$A$250="Advanced")*(D$10:D$250="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$250="Advanced")*(D$10:D$250="Partial"))</f>
         <v>3</v>
@@ -17526,7 +17529,7 @@
       <c r="B8" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="173"/>
+      <c r="C8" s="175"/>
       <c r="D8" s="66">
         <f>SUMPRODUCT(($A$10:$A$250="Professional")*(D$10:D$250="Completed"))+SUMPRODUCT(($A$10:$A$250="Professional")*(D$10:D$250="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$250="Professional")*(D$10:D$250="Partial"))</f>
         <v>0</v>
@@ -17541,11 +17544,11 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="175" t="s">
+      <c r="A9" s="177" t="s">
         <v>88</v>
       </c>
-      <c r="B9" s="176"/>
-      <c r="C9" s="174"/>
+      <c r="B9" s="178"/>
+      <c r="C9" s="176"/>
       <c r="D9" s="66">
         <f>SUMPRODUCT(($A$10:$A$250="Innovative")*(D$10:D$250="Completed"))+SUMPRODUCT(($A$10:$A$250="Innovative")*(D$10:D$250="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$250="Innovative")*(D$10:D$250="Partial"))</f>
         <v>0</v>
@@ -17560,10 +17563,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="177" t="s">
+      <c r="A10" s="172" t="s">
         <v>724</v>
       </c>
-      <c r="B10" s="178"/>
+      <c r="B10" s="173"/>
       <c r="C10" s="8" t="s">
         <v>868</v>
       </c>
@@ -17686,10 +17689,10 @@
       <c r="F16" s="60"/>
     </row>
     <row r="17" spans="1:6" ht="28.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="177" t="s">
+      <c r="A17" s="172" t="s">
         <v>739</v>
       </c>
-      <c r="B17" s="178"/>
+      <c r="B17" s="173"/>
       <c r="C17" s="8" t="s">
         <v>870</v>
       </c>
@@ -17904,10 +17907,10 @@
       <c r="F28" s="60"/>
     </row>
     <row r="29" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="177" t="s">
+      <c r="A29" s="172" t="s">
         <v>740</v>
       </c>
-      <c r="B29" s="178"/>
+      <c r="B29" s="173"/>
       <c r="C29" s="8" t="s">
         <v>871</v>
       </c>
@@ -18390,10 +18393,10 @@
       <c r="F55" s="60"/>
     </row>
     <row r="56" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="177" t="s">
+      <c r="A56" s="172" t="s">
         <v>114</v>
       </c>
-      <c r="B56" s="178"/>
+      <c r="B56" s="173"/>
       <c r="C56" s="8" t="s">
         <v>89</v>
       </c>
@@ -18562,7 +18565,7 @@
         <v>127</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E65" s="8" t="s">
         <v>74</v>
@@ -18580,7 +18583,7 @@
         <v>129</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E66" s="8" t="s">
         <v>74</v>
@@ -18624,10 +18627,10 @@
       <c r="F68" s="60"/>
     </row>
     <row r="69" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="177" t="s">
+      <c r="A69" s="172" t="s">
         <v>135</v>
       </c>
-      <c r="B69" s="178"/>
+      <c r="B69" s="173"/>
       <c r="C69" s="8" t="s">
         <v>89</v>
       </c>
@@ -18788,10 +18791,10 @@
       <c r="F77" s="60"/>
     </row>
     <row r="78" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="177" t="s">
+      <c r="A78" s="172" t="s">
         <v>152</v>
       </c>
-      <c r="B78" s="178"/>
+      <c r="B78" s="173"/>
       <c r="C78" s="8" t="s">
         <v>89</v>
       </c>
@@ -18896,10 +18899,10 @@
       <c r="F83" s="60"/>
     </row>
     <row r="84" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="177" t="s">
+      <c r="A84" s="172" t="s">
         <v>163</v>
       </c>
-      <c r="B84" s="178"/>
+      <c r="B84" s="173"/>
       <c r="C84" s="8" t="s">
         <v>89</v>
       </c>
@@ -19130,10 +19133,10 @@
       <c r="F96" s="60"/>
     </row>
     <row r="97" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A97" s="177" t="s">
+      <c r="A97" s="172" t="s">
         <v>187</v>
       </c>
-      <c r="B97" s="178"/>
+      <c r="B97" s="173"/>
       <c r="C97" s="8" t="s">
         <v>89</v>
       </c>
@@ -19220,10 +19223,10 @@
       <c r="F101" s="60"/>
     </row>
     <row r="102" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A102" s="177" t="s">
+      <c r="A102" s="172" t="s">
         <v>194</v>
       </c>
-      <c r="B102" s="178"/>
+      <c r="B102" s="173"/>
       <c r="C102" s="8" t="s">
         <v>89</v>
       </c>
@@ -19366,10 +19369,10 @@
       <c r="F109" s="60"/>
     </row>
     <row r="110" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A110" s="177" t="s">
+      <c r="A110" s="172" t="s">
         <v>205</v>
       </c>
-      <c r="B110" s="178"/>
+      <c r="B110" s="173"/>
       <c r="C110" s="8" t="s">
         <v>89</v>
       </c>
@@ -19438,10 +19441,10 @@
       <c r="F113" s="60"/>
     </row>
     <row r="114" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A114" s="177" t="s">
+      <c r="A114" s="172" t="s">
         <v>212</v>
       </c>
-      <c r="B114" s="178"/>
+      <c r="B114" s="173"/>
       <c r="C114" s="8" t="s">
         <v>89</v>
       </c>
@@ -19510,10 +19513,10 @@
       <c r="F117" s="60"/>
     </row>
     <row r="118" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A118" s="177" t="s">
+      <c r="A118" s="172" t="s">
         <v>219</v>
       </c>
-      <c r="B118" s="178"/>
+      <c r="B118" s="173"/>
       <c r="C118" s="8" t="s">
         <v>823</v>
       </c>
@@ -19673,6 +19676,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C2:C9"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A56:B56"/>
     <mergeCell ref="A110:B110"/>
     <mergeCell ref="A114:B114"/>
     <mergeCell ref="A118:B118"/>
@@ -19682,11 +19690,6 @@
     <mergeCell ref="A84:B84"/>
     <mergeCell ref="A97:B97"/>
     <mergeCell ref="A102:B102"/>
-    <mergeCell ref="C2:C9"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A56:B56"/>
   </mergeCells>
   <conditionalFormatting sqref="A10 A33:A37 A39:A41 A109:A251 A95:A107 A56:A92 A14:A31">
     <cfRule type="beginsWith" dxfId="740" priority="292" stopIfTrue="1" operator="beginsWith" text="Innovative">
@@ -20670,7 +20673,7 @@
       <c r="B2" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="172" t="s">
+      <c r="C2" s="174" t="s">
         <v>862</v>
       </c>
       <c r="D2" s="66">
@@ -20693,7 +20696,7 @@
       <c r="B3" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="173"/>
+      <c r="C3" s="175"/>
       <c r="D3" s="66">
         <f>SUMPRODUCT(($A$10:$A$241="Basic")*(D$10:D$241="Missing"))+0.5*SUMPRODUCT(($A$10:$A$241="Basic")*(D$10:D$241="Partial"))</f>
         <v>0</v>
@@ -20714,7 +20717,7 @@
       <c r="B4" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="173"/>
+      <c r="C4" s="175"/>
       <c r="D4" s="66">
         <f>SUMPRODUCT(($A$10:$A$241="Intermediate")*(D$10:D$241="Missing"))+0.5*SUMPRODUCT(($A$10:$A$241="Intermediate")*(D$10:D$241="Partial"))</f>
         <v>0</v>
@@ -20735,7 +20738,7 @@
       <c r="B5" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="173"/>
+      <c r="C5" s="175"/>
       <c r="D5" s="66">
         <f>SUMPRODUCT(($A$10:$A$241="Intermediate")*(D$10:D$241="Completed"))+SUMPRODUCT(($A$10:$A$241="Intermediate")*(D$10:D$241="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$241="Intermediate")*(D$10:D$241="Partial"))</f>
         <v>0</v>
@@ -20756,7 +20759,7 @@
       <c r="B6" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="173"/>
+      <c r="C6" s="175"/>
       <c r="D6" s="66">
         <f>SUMPRODUCT(($A$10:$A$241="Advanced")*(D$10:D$241="Missing"))+0.5*SUMPRODUCT(($A$10:$A$241="Advanced")*(D$10:D$241="Partial"))</f>
         <v>0</v>
@@ -20777,7 +20780,7 @@
       <c r="B7" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="173"/>
+      <c r="C7" s="175"/>
       <c r="D7" s="66">
         <f>SUMPRODUCT(($A$10:$A$241="Advanced")*(D$10:D$241="Completed"))+SUMPRODUCT(($A$10:$A$241="Advanced")*(D$10:D$241="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$241="Advanced")*(D$10:D$241="Partial"))</f>
         <v>0</v>
@@ -20798,7 +20801,7 @@
       <c r="B8" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="173"/>
+      <c r="C8" s="175"/>
       <c r="D8" s="66">
         <f>SUMPRODUCT(($A$10:$A$241="Professional")*(D$10:D$241="Completed"))+SUMPRODUCT(($A$10:$A$241="Professional")*(D$10:D$241="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$241="Professional")*(D$10:D$241="Partial"))</f>
         <v>0</v>
@@ -20813,11 +20816,11 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="175" t="s">
+      <c r="A9" s="177" t="s">
         <v>88</v>
       </c>
-      <c r="B9" s="176"/>
-      <c r="C9" s="174"/>
+      <c r="B9" s="178"/>
+      <c r="C9" s="176"/>
       <c r="D9" s="66">
         <f>SUMPRODUCT(($A$10:$A$241="Innovative")*(D$10:D$241="Completed"))+SUMPRODUCT(($A$10:$A$241="Innovative")*(D$10:D$241="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$241="Innovative")*(D$10:D$241="Partial"))</f>
         <v>0</v>
@@ -20832,10 +20835,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="177" t="s">
+      <c r="A10" s="172" t="s">
         <v>810</v>
       </c>
-      <c r="B10" s="178"/>
+      <c r="B10" s="173"/>
       <c r="C10" s="8" t="s">
         <v>863</v>
       </c>
@@ -20922,10 +20925,10 @@
       <c r="F14" s="60"/>
     </row>
     <row r="15" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="177" t="s">
+      <c r="A15" s="172" t="s">
         <v>249</v>
       </c>
-      <c r="B15" s="178"/>
+      <c r="B15" s="173"/>
       <c r="C15" s="8" t="s">
         <v>89</v>
       </c>
@@ -21066,10 +21069,10 @@
       <c r="F22" s="60"/>
     </row>
     <row r="23" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="177" t="s">
+      <c r="A23" s="172" t="s">
         <v>257</v>
       </c>
-      <c r="B23" s="178"/>
+      <c r="B23" s="173"/>
       <c r="C23" s="8" t="s">
         <v>89</v>
       </c>
@@ -21210,10 +21213,10 @@
       <c r="F30" s="60"/>
     </row>
     <row r="31" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="177" t="s">
+      <c r="A31" s="172" t="s">
         <v>262</v>
       </c>
-      <c r="B31" s="178"/>
+      <c r="B31" s="173"/>
       <c r="C31" s="8" t="s">
         <v>89</v>
       </c>
@@ -21678,10 +21681,10 @@
       <c r="F56" s="60"/>
     </row>
     <row r="57" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="177" t="s">
+      <c r="A57" s="172" t="s">
         <v>288</v>
       </c>
-      <c r="B57" s="178"/>
+      <c r="B57" s="173"/>
       <c r="C57" s="73" t="s">
         <v>832</v>
       </c>
@@ -22056,10 +22059,10 @@
       <c r="F77" s="60"/>
     </row>
     <row r="78" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="177" t="s">
+      <c r="A78" s="172" t="s">
         <v>301</v>
       </c>
-      <c r="B78" s="178"/>
+      <c r="B78" s="173"/>
       <c r="C78" s="8" t="s">
         <v>89</v>
       </c>
@@ -23021,8 +23024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -23064,7 +23067,7 @@
       <c r="B2" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="172" t="s">
+      <c r="C2" s="174" t="s">
         <v>830</v>
       </c>
       <c r="D2" s="66">
@@ -23087,7 +23090,7 @@
       <c r="B3" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="173"/>
+      <c r="C3" s="175"/>
       <c r="D3" s="66">
         <f>SUMPRODUCT(($A$10:$A$177="Basic")*(D$10:D$177="Missing"))+0.5*SUMPRODUCT(($A$10:$A$177="Basic")*(D$10:D$177="Partial"))</f>
         <v>0</v>
@@ -23108,7 +23111,7 @@
       <c r="B4" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="173"/>
+      <c r="C4" s="175"/>
       <c r="D4" s="66">
         <f>SUMPRODUCT(($A$10:$A$177="Intermediate")*(D$10:D$177="Missing"))+0.5*SUMPRODUCT(($A$10:$A$177="Intermediate")*(D$10:D$177="Partial"))</f>
         <v>1</v>
@@ -23129,7 +23132,7 @@
       <c r="B5" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="173"/>
+      <c r="C5" s="175"/>
       <c r="D5" s="66">
         <f>SUMPRODUCT(($A$10:$A$177="Intermediate")*(D$10:D$177="Completed"))+SUMPRODUCT(($A$10:$A$177="Intermediate")*(D$10:D$177="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$177="Intermediate")*(D$10:D$177="Partial"))</f>
         <v>1</v>
@@ -23150,7 +23153,7 @@
       <c r="B6" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="173"/>
+      <c r="C6" s="175"/>
       <c r="D6" s="66">
         <f>SUMPRODUCT(($A$10:$A$177="Advanced")*(D$10:D$177="Missing"))+0.5*SUMPRODUCT(($A$10:$A$177="Advanced")*(D$10:D$177="Partial"))</f>
         <v>2</v>
@@ -23171,7 +23174,7 @@
       <c r="B7" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="173"/>
+      <c r="C7" s="175"/>
       <c r="D7" s="66">
         <f>SUMPRODUCT(($A$10:$A$177="Advanced")*(D$10:D$177="Completed"))+SUMPRODUCT(($A$10:$A$177="Advanced")*(D$10:D$177="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$177="Advanced")*(D$10:D$177="Partial"))</f>
         <v>0</v>
@@ -23192,7 +23195,7 @@
       <c r="B8" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="173"/>
+      <c r="C8" s="175"/>
       <c r="D8" s="66">
         <f>SUMPRODUCT(($A$10:$A$177="Professional")*(D$10:D$177="Completed"))+SUMPRODUCT(($A$10:$A$177="Professional")*(D$10:D$177="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$177="Professional")*(D$10:D$177="Partial"))</f>
         <v>0</v>
@@ -23207,11 +23210,11 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="175" t="s">
+      <c r="A9" s="177" t="s">
         <v>88</v>
       </c>
-      <c r="B9" s="176"/>
-      <c r="C9" s="174"/>
+      <c r="B9" s="178"/>
+      <c r="C9" s="176"/>
       <c r="D9" s="66">
         <f>SUMPRODUCT(($A$10:$A$177="Innovative")*(D$10:D$177="Completed"))+SUMPRODUCT(($A$10:$A$177="Innovative")*(D$10:D$177="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$177="Innovative")*(D$10:D$177="Partial"))</f>
         <v>0</v>
@@ -23226,10 +23229,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="177" t="s">
+      <c r="A10" s="172" t="s">
         <v>237</v>
       </c>
-      <c r="B10" s="178"/>
+      <c r="B10" s="173"/>
       <c r="C10" s="8" t="s">
         <v>89</v>
       </c>
@@ -23442,10 +23445,10 @@
       <c r="F21" s="60"/>
     </row>
     <row r="22" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="177" t="s">
+      <c r="A22" s="172" t="s">
         <v>534</v>
       </c>
-      <c r="B22" s="178"/>
+      <c r="B22" s="173"/>
       <c r="C22" s="8" t="s">
         <v>89</v>
       </c>
@@ -23604,10 +23607,10 @@
       <c r="F30" s="60"/>
     </row>
     <row r="31" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="177" t="s">
+      <c r="A31" s="172" t="s">
         <v>550</v>
       </c>
-      <c r="B31" s="178"/>
+      <c r="B31" s="173"/>
       <c r="C31" s="8" t="s">
         <v>89</v>
       </c>
@@ -23711,7 +23714,7 @@
       </c>
       <c r="F36" s="60"/>
     </row>
-    <row r="37" spans="1:6" s="26" customFormat="1" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" s="26" customFormat="1" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="70" t="s">
         <v>110</v>
       </c>
@@ -23820,10 +23823,10 @@
       <c r="F42" s="60"/>
     </row>
     <row r="43" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="177" t="s">
+      <c r="A43" s="172" t="s">
         <v>661</v>
       </c>
-      <c r="B43" s="178"/>
+      <c r="B43" s="173"/>
       <c r="C43" s="8" t="s">
         <v>89</v>
       </c>
@@ -24112,7 +24115,7 @@
       <c r="B2" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="172" t="s">
+      <c r="C2" s="174" t="s">
         <v>384</v>
       </c>
       <c r="D2" s="66">
@@ -24135,7 +24138,7 @@
       <c r="B3" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="173"/>
+      <c r="C3" s="175"/>
       <c r="D3" s="66">
         <f>SUMPRODUCT(($A$10:$A$248="Basic")*(D$10:D$248="Missing"))+0.5*SUMPRODUCT(($A$10:$A$248="Basic")*(D$10:D$248="Partial"))</f>
         <v>0</v>
@@ -24156,7 +24159,7 @@
       <c r="B4" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="173"/>
+      <c r="C4" s="175"/>
       <c r="D4" s="66">
         <f>SUMPRODUCT(($A$10:$A$248="Intermediate")*(D$10:D$248="Missing"))+0.5*SUMPRODUCT(($A$10:$A$248="Intermediate")*(D$10:D$248="Partial"))</f>
         <v>0</v>
@@ -24177,7 +24180,7 @@
       <c r="B5" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="173"/>
+      <c r="C5" s="175"/>
       <c r="D5" s="66">
         <f>SUMPRODUCT(($A$10:$A$248="Intermediate")*(D$10:D$248="Completed"))+SUMPRODUCT(($A$10:$A$248="Intermediate")*(D$10:D$248="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$248="Intermediate")*(D$10:D$248="Partial"))</f>
         <v>0</v>
@@ -24198,7 +24201,7 @@
       <c r="B6" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="173"/>
+      <c r="C6" s="175"/>
       <c r="D6" s="66">
         <f>SUMPRODUCT(($A$10:$A$248="Advanced")*(D$10:D$248="Missing"))+0.5*SUMPRODUCT(($A$10:$A$248="Advanced")*(D$10:D$248="Partial"))</f>
         <v>0</v>
@@ -24219,7 +24222,7 @@
       <c r="B7" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="173"/>
+      <c r="C7" s="175"/>
       <c r="D7" s="66">
         <f>SUMPRODUCT(($A$10:$A$248="Advanced")*(D$10:D$248="Completed"))+SUMPRODUCT(($A$10:$A$248="Advanced")*(D$10:D$248="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$248="Advanced")*(D$10:D$248="Partial"))</f>
         <v>0</v>
@@ -24240,7 +24243,7 @@
       <c r="B8" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="173"/>
+      <c r="C8" s="175"/>
       <c r="D8" s="66">
         <f>SUMPRODUCT(($A$10:$A$248="Professional")*(D$10:D$248="Completed"))+SUMPRODUCT(($A$10:$A$248="Professional")*(D$10:D$248="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$248="Professional")*(D$10:D$248="Partial"))</f>
         <v>0</v>
@@ -24255,11 +24258,11 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="175" t="s">
+      <c r="A9" s="177" t="s">
         <v>88</v>
       </c>
-      <c r="B9" s="176"/>
-      <c r="C9" s="174"/>
+      <c r="B9" s="178"/>
+      <c r="C9" s="176"/>
       <c r="D9" s="66">
         <f>SUMPRODUCT(($A$10:$A$248="Innovative")*(D$10:D$248="Completed"))+SUMPRODUCT(($A$10:$A$248="Innovative")*(D$10:D$248="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$248="Innovative")*(D$10:D$248="Partial"))</f>
         <v>0</v>
@@ -24274,10 +24277,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="177" t="s">
+      <c r="A10" s="172" t="s">
         <v>385</v>
       </c>
-      <c r="B10" s="178"/>
+      <c r="B10" s="173"/>
       <c r="C10" s="8" t="s">
         <v>89</v>
       </c>
@@ -24382,10 +24385,10 @@
       <c r="F15" s="60"/>
     </row>
     <row r="16" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="177" t="s">
+      <c r="A16" s="172" t="s">
         <v>396</v>
       </c>
-      <c r="B16" s="178"/>
+      <c r="B16" s="173"/>
       <c r="C16" s="8" t="s">
         <v>89</v>
       </c>
@@ -24490,10 +24493,10 @@
       <c r="F21" s="60"/>
     </row>
     <row r="22" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="177" t="s">
+      <c r="A22" s="172" t="s">
         <v>407</v>
       </c>
-      <c r="B22" s="178"/>
+      <c r="B22" s="173"/>
       <c r="C22" s="8" t="s">
         <v>826</v>
       </c>
@@ -24616,10 +24619,10 @@
       <c r="F28" s="60"/>
     </row>
     <row r="29" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="177" t="s">
+      <c r="A29" s="172" t="s">
         <v>420</v>
       </c>
-      <c r="B29" s="178"/>
+      <c r="B29" s="173"/>
       <c r="C29" s="8" t="s">
         <v>824</v>
       </c>
@@ -24760,10 +24763,10 @@
       <c r="F36" s="60"/>
     </row>
     <row r="37" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="177" t="s">
+      <c r="A37" s="172" t="s">
         <v>435</v>
       </c>
-      <c r="B37" s="178"/>
+      <c r="B37" s="173"/>
       <c r="C37" s="8" t="s">
         <v>825</v>
       </c>
@@ -24886,10 +24889,10 @@
       <c r="F43" s="60"/>
     </row>
     <row r="44" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="177" t="s">
+      <c r="A44" s="172" t="s">
         <v>448</v>
       </c>
-      <c r="B44" s="178"/>
+      <c r="B44" s="173"/>
       <c r="C44" s="8" t="s">
         <v>89</v>
       </c>
@@ -25530,8 +25533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F103"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -25556,7 +25559,7 @@
       </c>
       <c r="D1" s="7" t="str">
         <f>""&amp;COUNTIF(D$10:D$227,$A$2)&amp;" "&amp;$A$2</f>
-        <v>46 Untested</v>
+        <v>40 Untested</v>
       </c>
       <c r="E1" s="7" t="str">
         <f>""&amp;COUNTIF(E$10:E$227,$A$2)&amp;" "&amp;$A$2</f>
@@ -25573,7 +25576,7 @@
       <c r="B2" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="172" t="s">
+      <c r="C2" s="174" t="s">
         <v>473</v>
       </c>
       <c r="D2" s="66">
@@ -25596,7 +25599,7 @@
       <c r="B3" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="173"/>
+      <c r="C3" s="175"/>
       <c r="D3" s="66">
         <f>SUMPRODUCT(($A$10:$A$227="Basic")*(D$10:D$227="Missing"))+0.5*SUMPRODUCT(($A$10:$A$227="Basic")*(D$10:D$227="Partial"))</f>
         <v>0</v>
@@ -25617,7 +25620,7 @@
       <c r="B4" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="173"/>
+      <c r="C4" s="175"/>
       <c r="D4" s="66">
         <f>SUMPRODUCT(($A$10:$A$227="Intermediate")*(D$10:D$227="Missing"))+0.5*SUMPRODUCT(($A$10:$A$227="Intermediate")*(D$10:D$227="Partial"))</f>
         <v>0</v>
@@ -25638,10 +25641,10 @@
       <c r="B5" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="173"/>
+      <c r="C5" s="175"/>
       <c r="D5" s="66">
         <f>SUMPRODUCT(($A$10:$A$227="Intermediate")*(D$10:D$227="Completed"))+SUMPRODUCT(($A$10:$A$227="Intermediate")*(D$10:D$227="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$227="Intermediate")*(D$10:D$227="Partial"))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E5" s="66">
         <f>SUMPRODUCT(($A$10:$A$227="Intermediate")*(E$10:E$227="Completed"))+SUMPRODUCT(($A$10:$A$227="Intermediate")*(E$10:E$227="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$227="Intermediate")*(E$10:E$227="Partial"))</f>
@@ -25659,7 +25662,7 @@
       <c r="B6" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="173"/>
+      <c r="C6" s="175"/>
       <c r="D6" s="66">
         <f>SUMPRODUCT(($A$10:$A$227="Advanced")*(D$10:D$227="Missing"))+0.5*SUMPRODUCT(($A$10:$A$227="Advanced")*(D$10:D$227="Partial"))</f>
         <v>0</v>
@@ -25680,7 +25683,7 @@
       <c r="B7" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="173"/>
+      <c r="C7" s="175"/>
       <c r="D7" s="66">
         <f>SUMPRODUCT(($A$10:$A$227="Advanced")*(D$10:D$227="Completed"))+SUMPRODUCT(($A$10:$A$227="Advanced")*(D$10:D$227="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$227="Advanced")*(D$10:D$227="Partial"))</f>
         <v>0</v>
@@ -25701,7 +25704,7 @@
       <c r="B8" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="173"/>
+      <c r="C8" s="175"/>
       <c r="D8" s="66">
         <f>SUMPRODUCT(($A$10:$A$227="Professional")*(D$10:D$227="Completed"))+SUMPRODUCT(($A$10:$A$227="Professional")*(D$10:D$227="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$227="Professional")*(D$10:D$227="Partial"))</f>
         <v>0</v>
@@ -25716,11 +25719,11 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="175" t="s">
+      <c r="A9" s="177" t="s">
         <v>88</v>
       </c>
-      <c r="B9" s="176"/>
-      <c r="C9" s="174"/>
+      <c r="B9" s="178"/>
+      <c r="C9" s="176"/>
       <c r="D9" s="66">
         <f>SUMPRODUCT(($A$10:$A$227="Innovative")*(D$10:D$227="Completed"))+SUMPRODUCT(($A$10:$A$227="Innovative")*(D$10:D$227="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$227="Innovative")*(D$10:D$227="Partial"))</f>
         <v>0</v>
@@ -25735,10 +25738,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="177" t="s">
+      <c r="A10" s="172" t="s">
         <v>474</v>
       </c>
-      <c r="B10" s="178"/>
+      <c r="B10" s="173"/>
       <c r="C10" s="8" t="s">
         <v>89</v>
       </c>
@@ -25763,7 +25766,7 @@
         <v>476</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>74</v>
@@ -25781,7 +25784,7 @@
         <v>480</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>74</v>
@@ -25799,14 +25802,14 @@
         <v>478</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>74</v>
       </c>
       <c r="F13" s="60"/>
     </row>
-    <row r="14" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="68" t="s">
         <v>96</v>
       </c>
@@ -25817,12 +25820,14 @@
         <v>484</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="F14" s="60"/>
+      <c r="F14" s="60" t="s">
+        <v>886</v>
+      </c>
     </row>
     <row r="15" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="70" t="s">
@@ -25853,7 +25858,7 @@
         <v>486</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>74</v>
@@ -25871,7 +25876,7 @@
         <v>488</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>74</v>
@@ -26077,10 +26082,10 @@
       <c r="F28" s="60"/>
     </row>
     <row r="29" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="177" t="s">
+      <c r="A29" s="172" t="s">
         <v>511</v>
       </c>
-      <c r="B29" s="178"/>
+      <c r="B29" s="173"/>
       <c r="C29" s="8" t="s">
         <v>821</v>
       </c>
@@ -26293,10 +26298,10 @@
       <c r="F40" s="60"/>
     </row>
     <row r="41" spans="1:6" s="26" customFormat="1" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="177" t="s">
+      <c r="A41" s="172" t="s">
         <v>114</v>
       </c>
-      <c r="B41" s="178"/>
+      <c r="B41" s="173"/>
       <c r="C41" s="8" t="s">
         <v>89</v>
       </c>
@@ -26455,10 +26460,10 @@
       <c r="F49" s="60"/>
     </row>
     <row r="50" spans="1:6" s="26" customFormat="1" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="177" t="s">
+      <c r="A50" s="172" t="s">
         <v>589</v>
       </c>
-      <c r="B50" s="178"/>
+      <c r="B50" s="173"/>
       <c r="C50" s="73" t="s">
         <v>822</v>
       </c>
@@ -26544,7 +26549,7 @@
       </c>
       <c r="F54" s="60"/>
     </row>
-    <row r="55" spans="1:6" s="26" customFormat="1" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" s="26" customFormat="1" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="69" t="s">
         <v>98</v>
       </c>
@@ -27027,7 +27032,7 @@
       <c r="B2" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="172" t="s">
+      <c r="C2" s="174" t="s">
         <v>610</v>
       </c>
       <c r="D2" s="66">
@@ -27050,7 +27055,7 @@
       <c r="B3" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="173"/>
+      <c r="C3" s="175"/>
       <c r="D3" s="66">
         <f>SUMPRODUCT(($A$10:$A$240="Basic")*(D$10:D$240="Missing"))+0.5*SUMPRODUCT(($A$10:$A$240="Basic")*(D$10:D$240="Partial"))</f>
         <v>0</v>
@@ -27071,7 +27076,7 @@
       <c r="B4" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="173"/>
+      <c r="C4" s="175"/>
       <c r="D4" s="66">
         <f>SUMPRODUCT(($A$10:$A$240="Intermediate")*(D$10:D$240="Missing"))+0.5*SUMPRODUCT(($A$10:$A$240="Intermediate")*(D$10:D$240="Partial"))</f>
         <v>0</v>
@@ -27092,7 +27097,7 @@
       <c r="B5" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="173"/>
+      <c r="C5" s="175"/>
       <c r="D5" s="66">
         <f>SUMPRODUCT(($A$10:$A$240="Intermediate")*(D$10:D$240="Completed"))+SUMPRODUCT(($A$10:$A$240="Intermediate")*(D$10:D$240="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$240="Intermediate")*(D$10:D$240="Partial"))</f>
         <v>0</v>
@@ -27113,7 +27118,7 @@
       <c r="B6" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="173"/>
+      <c r="C6" s="175"/>
       <c r="D6" s="66">
         <f>SUMPRODUCT(($A$10:$A$240="Advanced")*(D$10:D$240="Missing"))+0.5*SUMPRODUCT(($A$10:$A$240="Advanced")*(D$10:D$240="Partial"))</f>
         <v>0</v>
@@ -27134,7 +27139,7 @@
       <c r="B7" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="173"/>
+      <c r="C7" s="175"/>
       <c r="D7" s="66">
         <f>SUMPRODUCT(($A$10:$A$240="Advanced")*(D$10:D$240="Completed"))+SUMPRODUCT(($A$10:$A$240="Advanced")*(D$10:D$240="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$240="Advanced")*(D$10:D$240="Partial"))</f>
         <v>0</v>
@@ -27155,7 +27160,7 @@
       <c r="B8" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="173"/>
+      <c r="C8" s="175"/>
       <c r="D8" s="66">
         <f>SUMPRODUCT(($A$10:$A$240="Professional")*(D$10:D$240="Completed"))+SUMPRODUCT(($A$10:$A$240="Professional")*(D$10:D$240="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$240="Professional")*(D$10:D$240="Partial"))</f>
         <v>0</v>
@@ -27170,11 +27175,11 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="175" t="s">
+      <c r="A9" s="177" t="s">
         <v>88</v>
       </c>
-      <c r="B9" s="176"/>
-      <c r="C9" s="174"/>
+      <c r="B9" s="178"/>
+      <c r="C9" s="176"/>
       <c r="D9" s="66">
         <f>SUMPRODUCT(($A$10:$A$240="Innovative")*(D$10:D$240="Completed"))+SUMPRODUCT(($A$10:$A$240="Innovative")*(D$10:D$240="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$240="Innovative")*(D$10:D$240="Partial"))</f>
         <v>0</v>
@@ -27189,10 +27194,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="177" t="s">
+      <c r="A10" s="172" t="s">
         <v>611</v>
       </c>
-      <c r="B10" s="178"/>
+      <c r="B10" s="173"/>
       <c r="C10" s="73" t="s">
         <v>815</v>
       </c>
@@ -27405,10 +27410,10 @@
       <c r="F21" s="60"/>
     </row>
     <row r="22" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="177" t="s">
+      <c r="A22" s="172" t="s">
         <v>634</v>
       </c>
-      <c r="B22" s="178"/>
+      <c r="B22" s="173"/>
       <c r="C22" s="8" t="s">
         <v>89</v>
       </c>
@@ -27621,10 +27626,10 @@
       <c r="F33" s="60"/>
     </row>
     <row r="34" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="177" t="s">
+      <c r="A34" s="172" t="s">
         <v>811</v>
       </c>
-      <c r="B34" s="178"/>
+      <c r="B34" s="173"/>
       <c r="C34" s="8" t="s">
         <v>816</v>
       </c>
@@ -27747,10 +27752,10 @@
       <c r="F40" s="60"/>
     </row>
     <row r="41" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="177" t="s">
+      <c r="A41" s="172" t="s">
         <v>680</v>
       </c>
-      <c r="B41" s="178"/>
+      <c r="B41" s="173"/>
       <c r="C41" s="8" t="s">
         <v>89</v>
       </c>
@@ -28162,7 +28167,7 @@
   <dimension ref="A1:L60"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -28178,65 +28183,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="189" t="s">
+      <c r="A1" s="179" t="s">
         <v>705</v>
       </c>
       <c r="B1" s="75"/>
-      <c r="C1" s="179" t="s">
+      <c r="C1" s="194" t="s">
         <v>689</v>
       </c>
-      <c r="D1" s="180"/>
-      <c r="E1" s="179" t="s">
+      <c r="D1" s="195"/>
+      <c r="E1" s="194" t="s">
         <v>690</v>
       </c>
-      <c r="F1" s="180"/>
-      <c r="G1" s="179" t="s">
+      <c r="F1" s="195"/>
+      <c r="G1" s="194" t="s">
         <v>691</v>
       </c>
-      <c r="H1" s="180"/>
+      <c r="H1" s="195"/>
     </row>
     <row r="2" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="190"/>
+      <c r="A2" s="180"/>
       <c r="B2" s="75"/>
-      <c r="C2" s="181" t="s">
+      <c r="C2" s="196" t="s">
         <v>688</v>
       </c>
-      <c r="D2" s="182"/>
-      <c r="E2" s="181" t="s">
+      <c r="D2" s="197"/>
+      <c r="E2" s="196" t="s">
         <v>688</v>
       </c>
-      <c r="F2" s="182"/>
-      <c r="G2" s="181" t="s">
+      <c r="F2" s="197"/>
+      <c r="G2" s="196" t="s">
         <v>688</v>
       </c>
-      <c r="H2" s="182"/>
-      <c r="J2" s="192" t="s">
+      <c r="H2" s="197"/>
+      <c r="J2" s="182" t="s">
         <v>707</v>
       </c>
-      <c r="K2" s="193"/>
-      <c r="L2" s="194"/>
+      <c r="K2" s="183"/>
+      <c r="L2" s="184"/>
     </row>
     <row r="3" spans="1:12" ht="22.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="191"/>
+      <c r="A3" s="181"/>
       <c r="B3" s="76"/>
-      <c r="C3" s="183">
+      <c r="C3" s="192">
         <f>MAX(0,MIN(1,IF((A6+C6) &lt;= 0.95, ROUND(A6+C6,2), FLOOR((0.95+(A6+C6-0.95)/5),2))))</f>
-        <v>0.62</v>
-      </c>
-      <c r="D3" s="184"/>
-      <c r="E3" s="183">
+        <v>0.64</v>
+      </c>
+      <c r="D3" s="193"/>
+      <c r="E3" s="192">
         <f>MAX(0,MIN(1,IF((A6+E6) &lt;= 0.95, ROUND(A6+E6,2), FLOOR((0.95+(A6+E6-0.95)/5),2))))</f>
-        <v>0.66</v>
-      </c>
-      <c r="F3" s="184"/>
-      <c r="G3" s="183">
+        <v>0.67</v>
+      </c>
+      <c r="F3" s="193"/>
+      <c r="G3" s="192">
         <f>MAX(0,MIN(1,IF((A6+G6) &lt;= 0.95, ROUND(A6+G6,2), FLOOR((0.95+(A6+G6-0.95)/5),2))))</f>
-        <v>0.76</v>
-      </c>
-      <c r="H3" s="184"/>
-      <c r="J3" s="195"/>
-      <c r="K3" s="196"/>
-      <c r="L3" s="197"/>
+        <v>0.77</v>
+      </c>
+      <c r="H3" s="193"/>
+      <c r="J3" s="185"/>
+      <c r="K3" s="186"/>
+      <c r="L3" s="187"/>
     </row>
     <row r="4" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
@@ -28253,19 +28258,19 @@
         <v>692</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="118" t="s">
+      <c r="C5" s="145" t="s">
         <v>693</v>
       </c>
-      <c r="D5" s="120"/>
-      <c r="E5" s="118" t="s">
+      <c r="D5" s="147"/>
+      <c r="E5" s="145" t="s">
         <v>694</v>
       </c>
-      <c r="F5" s="120"/>
-      <c r="G5" s="118" t="s">
+      <c r="F5" s="147"/>
+      <c r="G5" s="145" t="s">
         <v>695</v>
       </c>
-      <c r="H5" s="120"/>
-      <c r="J5" s="127" t="s">
+      <c r="H5" s="147"/>
+      <c r="J5" s="139" t="s">
         <v>721</v>
       </c>
       <c r="K5" s="31"/>
@@ -28279,22 +28284,22 @@
         <v>0.85</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="186">
+      <c r="C6" s="189">
         <f>D15+D24+D33+D42+D51+D60</f>
-        <v>-0.22999999999999998</v>
-      </c>
-      <c r="D6" s="187"/>
-      <c r="E6" s="186">
+        <v>-0.20999999999999996</v>
+      </c>
+      <c r="D6" s="190"/>
+      <c r="E6" s="189">
         <f>F15+F24+F33+F42+F51+F60</f>
-        <v>-0.19</v>
-      </c>
-      <c r="F6" s="187"/>
-      <c r="G6" s="186">
+        <v>-0.18</v>
+      </c>
+      <c r="F6" s="190"/>
+      <c r="G6" s="189">
         <f>H15+H24+H33+H42+H51+H60</f>
-        <v>-8.7499999999999994E-2</v>
-      </c>
-      <c r="H6" s="187"/>
-      <c r="J6" s="128"/>
+        <v>-8.249999999999999E-2</v>
+      </c>
+      <c r="H6" s="190"/>
+      <c r="J6" s="140"/>
       <c r="K6" s="31"/>
       <c r="L6" s="104" t="s">
         <v>714</v>
@@ -28303,19 +28308,19 @@
     <row r="7" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="11"/>
-      <c r="C7" s="188" t="s">
+      <c r="C7" s="191" t="s">
         <v>696</v>
       </c>
-      <c r="D7" s="188"/>
-      <c r="E7" s="188" t="s">
+      <c r="D7" s="191"/>
+      <c r="E7" s="191" t="s">
         <v>697</v>
       </c>
-      <c r="F7" s="188"/>
-      <c r="G7" s="188" t="s">
+      <c r="F7" s="191"/>
+      <c r="G7" s="191" t="s">
         <v>698</v>
       </c>
-      <c r="H7" s="188"/>
-      <c r="J7" s="128"/>
+      <c r="H7" s="191"/>
+      <c r="J7" s="140"/>
       <c r="K7" s="105"/>
       <c r="L7" s="104" t="s">
         <v>715</v>
@@ -28346,7 +28351,7 @@
       <c r="H8" s="87" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="128"/>
+      <c r="J8" s="140"/>
       <c r="K8" s="105"/>
       <c r="L8" s="104" t="s">
         <v>716</v>
@@ -28382,7 +28387,7 @@
         <f t="shared" ref="H9:H14" si="2">B9*G9</f>
         <v>0</v>
       </c>
-      <c r="J9" s="128"/>
+      <c r="J9" s="140"/>
       <c r="K9" s="105"/>
       <c r="L9" s="104" t="s">
         <v>717</v>
@@ -28418,7 +28423,7 @@
         <f t="shared" si="2"/>
         <v>-0.03</v>
       </c>
-      <c r="J10" s="128"/>
+      <c r="J10" s="140"/>
       <c r="K10" s="105"/>
       <c r="L10" s="104" t="s">
         <v>718</v>
@@ -28431,30 +28436,30 @@
       </c>
       <c r="B11" s="11">
         <f>TCRs!$D$4</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C11" s="82">
         <v>-0.01</v>
       </c>
       <c r="D11" s="97">
         <f t="shared" si="0"/>
-        <v>-7.0000000000000007E-2</v>
+        <v>-0.05</v>
       </c>
       <c r="E11" s="100">
         <v>-5.0000000000000001E-3</v>
       </c>
       <c r="F11" s="97">
         <f t="shared" si="1"/>
-        <v>-3.5000000000000003E-2</v>
+        <v>-2.5000000000000001E-2</v>
       </c>
       <c r="G11" s="80">
         <v>-2.5000000000000001E-3</v>
       </c>
       <c r="H11" s="97">
         <f t="shared" si="2"/>
-        <v>-1.7500000000000002E-2</v>
-      </c>
-      <c r="J11" s="128"/>
+        <v>-1.2500000000000001E-2</v>
+      </c>
+      <c r="J11" s="140"/>
       <c r="K11" s="105"/>
       <c r="L11" s="104" t="s">
         <v>719</v>
@@ -28490,7 +28495,7 @@
         <f t="shared" si="2"/>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="J12" s="129"/>
+      <c r="J12" s="141"/>
       <c r="K12" s="105"/>
       <c r="L12" s="103" t="s">
         <v>720</v>
@@ -28566,38 +28571,38 @@
       </c>
       <c r="D15" s="99">
         <f>SUM(D9:D14)</f>
-        <v>-0.17499999999999999</v>
+        <v>-0.15499999999999997</v>
       </c>
       <c r="E15" s="79" t="s">
         <v>16</v>
       </c>
       <c r="F15" s="99">
         <f>SUM(F9:F14)</f>
-        <v>-0.08</v>
+        <v>-6.9999999999999993E-2</v>
       </c>
       <c r="G15" s="79" t="s">
         <v>16</v>
       </c>
       <c r="H15" s="99">
         <f>SUM(H9:H14)</f>
-        <v>-3.2500000000000001E-2</v>
+        <v>-2.7499999999999997E-2</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="11"/>
-      <c r="C16" s="185" t="s">
+      <c r="C16" s="188" t="s">
         <v>696</v>
       </c>
-      <c r="D16" s="185"/>
-      <c r="E16" s="185" t="s">
+      <c r="D16" s="188"/>
+      <c r="E16" s="188" t="s">
         <v>697</v>
       </c>
-      <c r="F16" s="185"/>
-      <c r="G16" s="185" t="s">
+      <c r="F16" s="188"/>
+      <c r="G16" s="188" t="s">
         <v>698</v>
       </c>
-      <c r="H16" s="185"/>
+      <c r="H16" s="188"/>
     </row>
     <row r="17" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
@@ -28839,18 +28844,18 @@
     <row r="25" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="11"/>
-      <c r="C25" s="185" t="s">
+      <c r="C25" s="188" t="s">
         <v>696</v>
       </c>
-      <c r="D25" s="185"/>
-      <c r="E25" s="185" t="s">
+      <c r="D25" s="188"/>
+      <c r="E25" s="188" t="s">
         <v>697</v>
       </c>
-      <c r="F25" s="185"/>
-      <c r="G25" s="185" t="s">
+      <c r="F25" s="188"/>
+      <c r="G25" s="188" t="s">
         <v>698</v>
       </c>
-      <c r="H25" s="185"/>
+      <c r="H25" s="188"/>
     </row>
     <row r="26" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
@@ -29092,18 +29097,18 @@
     <row r="34" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3"/>
       <c r="B34" s="11"/>
-      <c r="C34" s="185" t="s">
+      <c r="C34" s="188" t="s">
         <v>696</v>
       </c>
-      <c r="D34" s="185"/>
-      <c r="E34" s="185" t="s">
+      <c r="D34" s="188"/>
+      <c r="E34" s="188" t="s">
         <v>697</v>
       </c>
-      <c r="F34" s="185"/>
-      <c r="G34" s="185" t="s">
+      <c r="F34" s="188"/>
+      <c r="G34" s="188" t="s">
         <v>698</v>
       </c>
-      <c r="H34" s="185"/>
+      <c r="H34" s="188"/>
     </row>
     <row r="35" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
@@ -29345,18 +29350,18 @@
     <row r="43" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3"/>
       <c r="B43" s="11"/>
-      <c r="C43" s="185" t="s">
+      <c r="C43" s="188" t="s">
         <v>696</v>
       </c>
-      <c r="D43" s="185"/>
-      <c r="E43" s="185" t="s">
+      <c r="D43" s="188"/>
+      <c r="E43" s="188" t="s">
         <v>697</v>
       </c>
-      <c r="F43" s="185"/>
-      <c r="G43" s="185" t="s">
+      <c r="F43" s="188"/>
+      <c r="G43" s="188" t="s">
         <v>698</v>
       </c>
-      <c r="H43" s="185"/>
+      <c r="H43" s="188"/>
     </row>
     <row r="44" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
@@ -29598,18 +29603,18 @@
     <row r="52" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="3"/>
       <c r="B52" s="11"/>
-      <c r="C52" s="185" t="s">
+      <c r="C52" s="188" t="s">
         <v>696</v>
       </c>
-      <c r="D52" s="185"/>
-      <c r="E52" s="185" t="s">
+      <c r="D52" s="188"/>
+      <c r="E52" s="188" t="s">
         <v>697</v>
       </c>
-      <c r="F52" s="185"/>
-      <c r="G52" s="185" t="s">
+      <c r="F52" s="188"/>
+      <c r="G52" s="188" t="s">
         <v>698</v>
       </c>
-      <c r="H52" s="185"/>
+      <c r="H52" s="188"/>
     </row>
     <row r="53" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
@@ -29850,6 +29855,26 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="J2:L3"/>
     <mergeCell ref="J5:J12"/>
@@ -29866,26 +29891,6 @@
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Worked on credits, finished fullscreen
</commit_message>
<xml_diff>
--- a/Rubric/GAM_Project_Rubric_EpisodePrototype.xlsx
+++ b/Rubric/GAM_Project_Rubric_EpisodePrototype.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Connor\Source\Repos\Game200-Project\Rubric\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Connor\Source\Repos\Game200-project\Rubric\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -4324,6 +4324,87 @@
     <xf numFmtId="0" fontId="27" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4351,94 +4432,16 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4448,6 +4451,15 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4471,20 +4483,14 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -4499,42 +4505,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="22" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="22" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4563,6 +4533,36 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -14585,47 +14585,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="118" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="119"/>
-      <c r="C1" s="119"/>
-      <c r="D1" s="120"/>
+      <c r="A1" s="145" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="146"/>
+      <c r="C1" s="146"/>
+      <c r="D1" s="147"/>
       <c r="E1" s="16"/>
-      <c r="F1" s="118" t="s">
+      <c r="F1" s="145" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="119"/>
-      <c r="H1" s="119"/>
-      <c r="I1" s="120"/>
+      <c r="G1" s="146"/>
+      <c r="H1" s="146"/>
+      <c r="I1" s="147"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
       <c r="L1" s="35"/>
     </row>
     <row r="2" spans="1:12" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="121"/>
-      <c r="B2" s="122"/>
-      <c r="C2" s="122"/>
-      <c r="D2" s="123"/>
+      <c r="A2" s="148"/>
+      <c r="B2" s="149"/>
+      <c r="C2" s="149"/>
+      <c r="D2" s="150"/>
       <c r="E2" s="16"/>
-      <c r="F2" s="121"/>
-      <c r="G2" s="122"/>
-      <c r="H2" s="122"/>
-      <c r="I2" s="123"/>
+      <c r="F2" s="148"/>
+      <c r="G2" s="149"/>
+      <c r="H2" s="149"/>
+      <c r="I2" s="150"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
       <c r="L2" s="35"/>
     </row>
     <row r="3" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="124"/>
-      <c r="B3" s="125"/>
-      <c r="C3" s="125"/>
-      <c r="D3" s="126"/>
+      <c r="A3" s="151"/>
+      <c r="B3" s="152"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="153"/>
       <c r="E3" s="16"/>
-      <c r="F3" s="124"/>
-      <c r="G3" s="125"/>
-      <c r="H3" s="125"/>
-      <c r="I3" s="126"/>
+      <c r="F3" s="151"/>
+      <c r="G3" s="152"/>
+      <c r="H3" s="152"/>
+      <c r="I3" s="153"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
       <c r="L3" s="35"/>
@@ -14645,35 +14645,35 @@
       <c r="L4" s="35"/>
     </row>
     <row r="5" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="118" t="s">
+      <c r="A5" s="145" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="119"/>
-      <c r="C5" s="119"/>
-      <c r="D5" s="120"/>
+      <c r="B5" s="146"/>
+      <c r="C5" s="146"/>
+      <c r="D5" s="147"/>
       <c r="E5" s="16"/>
-      <c r="F5" s="118" t="s">
+      <c r="F5" s="145" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="119"/>
-      <c r="H5" s="119"/>
-      <c r="I5" s="120"/>
+      <c r="G5" s="146"/>
+      <c r="H5" s="146"/>
+      <c r="I5" s="147"/>
       <c r="J5" s="6"/>
       <c r="K5" s="30"/>
       <c r="L5" s="35"/>
     </row>
     <row r="6" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="130"/>
-      <c r="B6" s="131"/>
-      <c r="C6" s="131"/>
-      <c r="D6" s="132"/>
+      <c r="A6" s="142"/>
+      <c r="B6" s="143"/>
+      <c r="C6" s="143"/>
+      <c r="D6" s="144"/>
       <c r="E6" s="16"/>
-      <c r="F6" s="130"/>
-      <c r="G6" s="131"/>
-      <c r="H6" s="131"/>
-      <c r="I6" s="132"/>
+      <c r="F6" s="142"/>
+      <c r="G6" s="143"/>
+      <c r="H6" s="143"/>
+      <c r="I6" s="144"/>
       <c r="J6" s="6"/>
-      <c r="K6" s="127" t="s">
+      <c r="K6" s="139" t="s">
         <v>29</v>
       </c>
       <c r="L6" s="35"/>
@@ -14684,42 +14684,42 @@
       <c r="C7" s="5"/>
       <c r="D7" s="37"/>
       <c r="E7" s="16"/>
-      <c r="F7" s="130"/>
-      <c r="G7" s="131"/>
-      <c r="H7" s="131"/>
-      <c r="I7" s="132"/>
+      <c r="F7" s="142"/>
+      <c r="G7" s="143"/>
+      <c r="H7" s="143"/>
+      <c r="I7" s="144"/>
       <c r="J7" s="6"/>
-      <c r="K7" s="128"/>
+      <c r="K7" s="140"/>
       <c r="L7" s="35"/>
     </row>
     <row r="8" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="118" t="s">
+      <c r="A8" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="119"/>
-      <c r="C8" s="119"/>
-      <c r="D8" s="120"/>
+      <c r="B8" s="146"/>
+      <c r="C8" s="146"/>
+      <c r="D8" s="147"/>
       <c r="E8" s="16"/>
-      <c r="F8" s="130"/>
-      <c r="G8" s="131"/>
-      <c r="H8" s="131"/>
-      <c r="I8" s="132"/>
+      <c r="F8" s="142"/>
+      <c r="G8" s="143"/>
+      <c r="H8" s="143"/>
+      <c r="I8" s="144"/>
       <c r="J8" s="6"/>
-      <c r="K8" s="128"/>
+      <c r="K8" s="140"/>
       <c r="L8" s="35"/>
     </row>
     <row r="9" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="130"/>
-      <c r="B9" s="131"/>
-      <c r="C9" s="131"/>
-      <c r="D9" s="132"/>
+      <c r="A9" s="142"/>
+      <c r="B9" s="143"/>
+      <c r="C9" s="143"/>
+      <c r="D9" s="144"/>
       <c r="E9" s="16"/>
-      <c r="F9" s="130"/>
-      <c r="G9" s="131"/>
-      <c r="H9" s="131"/>
-      <c r="I9" s="132"/>
+      <c r="F9" s="142"/>
+      <c r="G9" s="143"/>
+      <c r="H9" s="143"/>
+      <c r="I9" s="144"/>
       <c r="J9" s="6"/>
-      <c r="K9" s="129"/>
+      <c r="K9" s="141"/>
       <c r="L9" s="35"/>
     </row>
     <row r="10" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -14737,17 +14737,17 @@
       <c r="L10" s="35"/>
     </row>
     <row r="11" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="118" t="s">
+      <c r="A11" s="145" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="119"/>
-      <c r="C11" s="119"/>
-      <c r="D11" s="120"/>
+      <c r="B11" s="146"/>
+      <c r="C11" s="146"/>
+      <c r="D11" s="147"/>
       <c r="E11" s="16"/>
-      <c r="F11" s="118" t="s">
+      <c r="F11" s="145" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="120"/>
+      <c r="G11" s="147"/>
       <c r="H11" s="2" t="s">
         <v>7</v>
       </c>
@@ -14786,7 +14786,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="6"/>
-      <c r="K12" s="127" t="s">
+      <c r="K12" s="139" t="s">
         <v>8</v>
       </c>
       <c r="L12" s="35"/>
@@ -14810,7 +14810,7 @@
         <v>0</v>
       </c>
       <c r="J13" s="47"/>
-      <c r="K13" s="128"/>
+      <c r="K13" s="140"/>
       <c r="L13" s="48"/>
     </row>
     <row r="14" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -14831,7 +14831,7 @@
         <v>0</v>
       </c>
       <c r="J14" s="12"/>
-      <c r="K14" s="129"/>
+      <c r="K14" s="141"/>
       <c r="L14" s="52"/>
     </row>
     <row r="15" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -14873,10 +14873,10 @@
       <c r="C17" s="45"/>
       <c r="D17" s="46"/>
       <c r="E17" s="6"/>
-      <c r="F17" s="118" t="s">
+      <c r="F17" s="145" t="s">
         <v>17</v>
       </c>
-      <c r="G17" s="120"/>
+      <c r="G17" s="147"/>
       <c r="H17" s="2"/>
       <c r="I17" s="38">
         <v>0.75</v>
@@ -14894,16 +14894,16 @@
       <c r="F18" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="133" t="s">
+      <c r="G18" s="123" t="s">
         <v>20</v>
       </c>
-      <c r="H18" s="134"/>
+      <c r="H18" s="125"/>
       <c r="I18" s="43">
         <f>IF(LEFT(G18,6)="Entire",0,IF(LEFT(G18,6)="Custom",-0.05,-0.1))</f>
         <v>0</v>
       </c>
       <c r="J18" s="54"/>
-      <c r="K18" s="127" t="s">
+      <c r="K18" s="139" t="s">
         <v>18</v>
       </c>
       <c r="L18" s="35"/>
@@ -14917,16 +14917,16 @@
       <c r="F19" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="G19" s="135" t="s">
+      <c r="G19" s="129" t="s">
         <v>22</v>
       </c>
-      <c r="H19" s="136"/>
+      <c r="H19" s="131"/>
       <c r="I19" s="51">
         <f>IF(G19="2D Graphics and 2D Gameplay",IF(I11=0.15,-0.05,0),IF(G19="3D Graphics but 2D Gameplay",IF(I11=0.15,-0.02,-0.3),IF(I11=0.15,0,-0.3)))</f>
         <v>0</v>
       </c>
       <c r="J19" s="6"/>
-      <c r="K19" s="129"/>
+      <c r="K19" s="141"/>
       <c r="L19" s="35"/>
     </row>
     <row r="20" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -14954,7 +14954,7 @@
       <c r="C21" s="45"/>
       <c r="D21" s="46"/>
       <c r="E21" s="6"/>
-      <c r="F21" s="151" t="s">
+      <c r="F21" s="136" t="s">
         <v>23</v>
       </c>
       <c r="G21" s="55"/>
@@ -14970,17 +14970,17 @@
       <c r="C22" s="45"/>
       <c r="D22" s="46"/>
       <c r="E22" s="6"/>
-      <c r="F22" s="152"/>
+      <c r="F22" s="137"/>
       <c r="G22" s="55"/>
       <c r="H22" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="I22" s="137">
+      <c r="I22" s="118">
         <f>I20+I15</f>
         <v>0.85</v>
       </c>
       <c r="J22" s="6"/>
-      <c r="K22" s="139" t="s">
+      <c r="K22" s="120" t="s">
         <v>26</v>
       </c>
       <c r="L22" s="35"/>
@@ -14991,14 +14991,14 @@
       <c r="C23" s="45"/>
       <c r="D23" s="46"/>
       <c r="E23" s="6"/>
-      <c r="F23" s="152"/>
+      <c r="F23" s="137"/>
       <c r="G23" s="55"/>
       <c r="H23" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="I23" s="138"/>
+      <c r="I23" s="119"/>
       <c r="J23" s="6"/>
-      <c r="K23" s="140"/>
+      <c r="K23" s="121"/>
       <c r="L23" s="35"/>
     </row>
     <row r="24" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -15007,7 +15007,7 @@
       <c r="C24" s="45"/>
       <c r="D24" s="46"/>
       <c r="E24" s="6"/>
-      <c r="F24" s="153"/>
+      <c r="F24" s="138"/>
       <c r="G24" s="55"/>
       <c r="H24" s="55"/>
       <c r="I24" s="55"/>
@@ -15035,12 +15035,12 @@
       <c r="C26" s="45"/>
       <c r="D26" s="46"/>
       <c r="E26" s="16"/>
-      <c r="F26" s="141" t="s">
+      <c r="F26" s="122" t="s">
         <v>27</v>
       </c>
-      <c r="G26" s="141"/>
-      <c r="H26" s="141"/>
-      <c r="I26" s="141"/>
+      <c r="G26" s="122"/>
+      <c r="H26" s="122"/>
+      <c r="I26" s="122"/>
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
       <c r="L26" s="35"/>
@@ -15051,12 +15051,12 @@
       <c r="C27" s="45"/>
       <c r="D27" s="46"/>
       <c r="E27" s="16"/>
-      <c r="F27" s="133" t="s">
+      <c r="F27" s="123" t="s">
         <v>28</v>
       </c>
-      <c r="G27" s="142"/>
-      <c r="H27" s="142"/>
-      <c r="I27" s="134"/>
+      <c r="G27" s="124"/>
+      <c r="H27" s="124"/>
+      <c r="I27" s="125"/>
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
       <c r="L27" s="35"/>
@@ -15067,10 +15067,10 @@
       <c r="C28" s="45"/>
       <c r="D28" s="46"/>
       <c r="E28" s="16"/>
-      <c r="F28" s="143"/>
-      <c r="G28" s="144"/>
-      <c r="H28" s="144"/>
-      <c r="I28" s="145"/>
+      <c r="F28" s="126"/>
+      <c r="G28" s="127"/>
+      <c r="H28" s="127"/>
+      <c r="I28" s="128"/>
       <c r="J28" s="6"/>
       <c r="K28" s="6"/>
       <c r="L28" s="35"/>
@@ -15081,10 +15081,10 @@
       <c r="C29" s="45"/>
       <c r="D29" s="46"/>
       <c r="E29" s="16"/>
-      <c r="F29" s="143"/>
-      <c r="G29" s="144"/>
-      <c r="H29" s="144"/>
-      <c r="I29" s="145"/>
+      <c r="F29" s="126"/>
+      <c r="G29" s="127"/>
+      <c r="H29" s="127"/>
+      <c r="I29" s="128"/>
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
       <c r="L29" s="35"/>
@@ -15095,26 +15095,26 @@
       <c r="C30" s="45"/>
       <c r="D30" s="46"/>
       <c r="E30" s="16"/>
-      <c r="F30" s="143"/>
-      <c r="G30" s="144"/>
-      <c r="H30" s="144"/>
-      <c r="I30" s="145"/>
+      <c r="F30" s="126"/>
+      <c r="G30" s="127"/>
+      <c r="H30" s="127"/>
+      <c r="I30" s="128"/>
       <c r="J30" s="6"/>
       <c r="K30" s="6"/>
       <c r="L30" s="35"/>
     </row>
     <row r="31" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="147" t="s">
+      <c r="A31" s="132" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="148"/>
-      <c r="C31" s="149"/>
-      <c r="D31" s="150"/>
+      <c r="B31" s="133"/>
+      <c r="C31" s="134"/>
+      <c r="D31" s="135"/>
       <c r="E31" s="6"/>
-      <c r="F31" s="135"/>
-      <c r="G31" s="146"/>
-      <c r="H31" s="146"/>
-      <c r="I31" s="136"/>
+      <c r="F31" s="129"/>
+      <c r="G31" s="130"/>
+      <c r="H31" s="130"/>
+      <c r="I31" s="131"/>
       <c r="J31" s="6"/>
       <c r="K31" s="6"/>
       <c r="L31" s="35"/>
@@ -15135,13 +15135,12 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="F27:I31"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="F21:F24"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="A2:D3"/>
+    <mergeCell ref="F2:I3"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="F5:I5"/>
     <mergeCell ref="K12:K14"/>
     <mergeCell ref="K18:K19"/>
     <mergeCell ref="A6:D6"/>
@@ -15157,12 +15156,13 @@
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="G19:H19"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="A2:D3"/>
-    <mergeCell ref="F2:I3"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="F27:I31"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="F21:F24"/>
   </mergeCells>
   <dataValidations count="9">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A6:D6">
@@ -15219,65 +15219,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="189" t="s">
+      <c r="A1" s="179" t="s">
         <v>706</v>
       </c>
       <c r="B1" s="75"/>
-      <c r="C1" s="179" t="s">
+      <c r="C1" s="194" t="s">
         <v>689</v>
       </c>
-      <c r="D1" s="180"/>
-      <c r="E1" s="179" t="s">
+      <c r="D1" s="195"/>
+      <c r="E1" s="194" t="s">
         <v>690</v>
       </c>
-      <c r="F1" s="180"/>
-      <c r="G1" s="179" t="s">
+      <c r="F1" s="195"/>
+      <c r="G1" s="194" t="s">
         <v>691</v>
       </c>
-      <c r="H1" s="180"/>
+      <c r="H1" s="195"/>
     </row>
     <row r="2" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="190"/>
+      <c r="A2" s="180"/>
       <c r="B2" s="75"/>
-      <c r="C2" s="181" t="s">
+      <c r="C2" s="196" t="s">
         <v>688</v>
       </c>
-      <c r="D2" s="182"/>
-      <c r="E2" s="181" t="s">
+      <c r="D2" s="197"/>
+      <c r="E2" s="196" t="s">
         <v>688</v>
       </c>
-      <c r="F2" s="182"/>
-      <c r="G2" s="181" t="s">
+      <c r="F2" s="197"/>
+      <c r="G2" s="196" t="s">
         <v>688</v>
       </c>
-      <c r="H2" s="182"/>
-      <c r="J2" s="192" t="s">
+      <c r="H2" s="197"/>
+      <c r="J2" s="182" t="s">
         <v>707</v>
       </c>
-      <c r="K2" s="193"/>
-      <c r="L2" s="194"/>
+      <c r="K2" s="183"/>
+      <c r="L2" s="184"/>
     </row>
     <row r="3" spans="1:12" ht="22.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="191"/>
+      <c r="A3" s="181"/>
       <c r="B3" s="76"/>
-      <c r="C3" s="183">
+      <c r="C3" s="192">
         <f>MAX(0,MIN(1,IF((A6+C6+L6) &lt;= 0.95, ROUND(A6+C6+L6,2), FLOOR((0.95+(A6+C6+L6-0.95)/5),2))))</f>
         <v>0.85</v>
       </c>
-      <c r="D3" s="184"/>
-      <c r="E3" s="183">
+      <c r="D3" s="193"/>
+      <c r="E3" s="192">
         <f>MAX(0,MIN(1,IF((A6+E6+L6) &lt;= 0.95, ROUND(A6+E6+L6,2), FLOOR((0.95+(A6+E6+L6-0.95)/5),2))))</f>
         <v>0.85</v>
       </c>
-      <c r="F3" s="184"/>
-      <c r="G3" s="183">
+      <c r="F3" s="193"/>
+      <c r="G3" s="192">
         <f>MAX(0,MIN(1,IF((A6+G6+L6) &lt;= 0.95, ROUND(A6+G6+L6,2), FLOOR((0.95+(A6+G6+L6-0.95)/5),2))))</f>
         <v>0.85</v>
       </c>
-      <c r="H3" s="184"/>
-      <c r="J3" s="195"/>
-      <c r="K3" s="196"/>
-      <c r="L3" s="197"/>
+      <c r="H3" s="193"/>
+      <c r="J3" s="185"/>
+      <c r="K3" s="186"/>
+      <c r="L3" s="187"/>
     </row>
     <row r="4" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
@@ -15297,18 +15297,18 @@
         <v>692</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="118" t="s">
+      <c r="C5" s="145" t="s">
         <v>693</v>
       </c>
-      <c r="D5" s="120"/>
-      <c r="E5" s="118" t="s">
+      <c r="D5" s="147"/>
+      <c r="E5" s="145" t="s">
         <v>694</v>
       </c>
-      <c r="F5" s="120"/>
-      <c r="G5" s="118" t="s">
+      <c r="F5" s="147"/>
+      <c r="G5" s="145" t="s">
         <v>695</v>
       </c>
-      <c r="H5" s="120"/>
+      <c r="H5" s="147"/>
       <c r="J5" s="77" t="s">
         <v>708</v>
       </c>
@@ -15323,24 +15323,24 @@
         <v>0.85</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="186">
+      <c r="C6" s="189">
         <f>D15+D24+D33+D42+D51+D60</f>
         <v>0</v>
       </c>
-      <c r="D6" s="187"/>
-      <c r="E6" s="186">
+      <c r="D6" s="190"/>
+      <c r="E6" s="189">
         <f>F15+F24+F33+F42+F51+F60</f>
         <v>0</v>
       </c>
-      <c r="F6" s="187"/>
-      <c r="G6" s="186">
+      <c r="F6" s="190"/>
+      <c r="G6" s="189">
         <f>H15+H24+H33+H42+H51+H60</f>
         <v>0</v>
       </c>
-      <c r="H6" s="187"/>
+      <c r="H6" s="190"/>
       <c r="J6" s="92">
         <f>ABS('Student Grade'!$F$15+'Student Grade'!$D$24+'Student Grade'!$H$33+'Student Grade'!$F$42+'Student Grade'!$F$51+'Student Grade'!$F$60-$F$15-$D$24-$D$33-$H$42-$F$51-$F$60)</f>
-        <v>0.64749999999999996</v>
+        <v>0.62250000000000005</v>
       </c>
       <c r="K6" s="3"/>
       <c r="L6" s="90">
@@ -15351,18 +15351,18 @@
     <row r="7" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="11"/>
-      <c r="C7" s="188" t="s">
+      <c r="C7" s="191" t="s">
         <v>696</v>
       </c>
-      <c r="D7" s="188"/>
-      <c r="E7" s="188" t="s">
+      <c r="D7" s="191"/>
+      <c r="E7" s="191" t="s">
         <v>697</v>
       </c>
-      <c r="F7" s="188"/>
-      <c r="G7" s="188" t="s">
+      <c r="F7" s="191"/>
+      <c r="G7" s="191" t="s">
         <v>698</v>
       </c>
-      <c r="H7" s="188"/>
+      <c r="H7" s="191"/>
       <c r="J7" s="91"/>
       <c r="K7" s="3"/>
       <c r="L7" s="89"/>
@@ -15536,7 +15536,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J12" s="127" t="s">
+      <c r="J12" s="139" t="s">
         <v>721</v>
       </c>
       <c r="K12" s="31"/>
@@ -15574,7 +15574,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J13" s="128"/>
+      <c r="J13" s="140"/>
       <c r="K13" s="31"/>
       <c r="L13" s="104" t="s">
         <v>714</v>
@@ -15610,7 +15610,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J14" s="128"/>
+      <c r="J14" s="140"/>
       <c r="K14" s="105"/>
       <c r="L14" s="104" t="s">
         <v>715</v>
@@ -15640,7 +15640,7 @@
         <f>SUM(H9:H14)</f>
         <v>0</v>
       </c>
-      <c r="J15" s="128"/>
+      <c r="J15" s="140"/>
       <c r="K15" s="105"/>
       <c r="L15" s="104" t="s">
         <v>716</v>
@@ -15649,19 +15649,19 @@
     <row r="16" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="11"/>
-      <c r="C16" s="185" t="s">
+      <c r="C16" s="188" t="s">
         <v>696</v>
       </c>
-      <c r="D16" s="185"/>
-      <c r="E16" s="185" t="s">
+      <c r="D16" s="188"/>
+      <c r="E16" s="188" t="s">
         <v>697</v>
       </c>
-      <c r="F16" s="185"/>
-      <c r="G16" s="185" t="s">
+      <c r="F16" s="188"/>
+      <c r="G16" s="188" t="s">
         <v>698</v>
       </c>
-      <c r="H16" s="185"/>
-      <c r="J16" s="128"/>
+      <c r="H16" s="188"/>
+      <c r="J16" s="140"/>
       <c r="K16" s="105"/>
       <c r="L16" s="104" t="s">
         <v>717</v>
@@ -15692,7 +15692,7 @@
       <c r="H17" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="J17" s="128"/>
+      <c r="J17" s="140"/>
       <c r="K17" s="105"/>
       <c r="L17" s="104" t="s">
         <v>718</v>
@@ -15728,7 +15728,7 @@
         <f t="shared" ref="H18:H23" si="5">B18*G18</f>
         <v>0</v>
       </c>
-      <c r="J18" s="128"/>
+      <c r="J18" s="140"/>
       <c r="K18" s="105"/>
       <c r="L18" s="104" t="s">
         <v>719</v>
@@ -15764,7 +15764,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J19" s="129"/>
+      <c r="J19" s="141"/>
       <c r="K19" s="105"/>
       <c r="L19" s="103" t="s">
         <v>720</v>
@@ -15922,18 +15922,18 @@
     <row r="25" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="11"/>
-      <c r="C25" s="185" t="s">
+      <c r="C25" s="188" t="s">
         <v>696</v>
       </c>
-      <c r="D25" s="185"/>
-      <c r="E25" s="185" t="s">
+      <c r="D25" s="188"/>
+      <c r="E25" s="188" t="s">
         <v>697</v>
       </c>
-      <c r="F25" s="185"/>
-      <c r="G25" s="185" t="s">
+      <c r="F25" s="188"/>
+      <c r="G25" s="188" t="s">
         <v>698</v>
       </c>
-      <c r="H25" s="185"/>
+      <c r="H25" s="188"/>
     </row>
     <row r="26" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
@@ -16175,18 +16175,18 @@
     <row r="34" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3"/>
       <c r="B34" s="11"/>
-      <c r="C34" s="185" t="s">
+      <c r="C34" s="188" t="s">
         <v>696</v>
       </c>
-      <c r="D34" s="185"/>
-      <c r="E34" s="185" t="s">
+      <c r="D34" s="188"/>
+      <c r="E34" s="188" t="s">
         <v>697</v>
       </c>
-      <c r="F34" s="185"/>
-      <c r="G34" s="185" t="s">
+      <c r="F34" s="188"/>
+      <c r="G34" s="188" t="s">
         <v>698</v>
       </c>
-      <c r="H34" s="185"/>
+      <c r="H34" s="188"/>
     </row>
     <row r="35" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
@@ -16428,18 +16428,18 @@
     <row r="43" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3"/>
       <c r="B43" s="11"/>
-      <c r="C43" s="185" t="s">
+      <c r="C43" s="188" t="s">
         <v>696</v>
       </c>
-      <c r="D43" s="185"/>
-      <c r="E43" s="185" t="s">
+      <c r="D43" s="188"/>
+      <c r="E43" s="188" t="s">
         <v>697</v>
       </c>
-      <c r="F43" s="185"/>
-      <c r="G43" s="185" t="s">
+      <c r="F43" s="188"/>
+      <c r="G43" s="188" t="s">
         <v>698</v>
       </c>
-      <c r="H43" s="185"/>
+      <c r="H43" s="188"/>
     </row>
     <row r="44" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
@@ -16681,18 +16681,18 @@
     <row r="52" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="3"/>
       <c r="B52" s="11"/>
-      <c r="C52" s="185" t="s">
+      <c r="C52" s="188" t="s">
         <v>696</v>
       </c>
-      <c r="D52" s="185"/>
-      <c r="E52" s="185" t="s">
+      <c r="D52" s="188"/>
+      <c r="E52" s="188" t="s">
         <v>697</v>
       </c>
-      <c r="F52" s="185"/>
-      <c r="G52" s="185" t="s">
+      <c r="F52" s="188"/>
+      <c r="G52" s="188" t="s">
         <v>698</v>
       </c>
-      <c r="H52" s="185"/>
+      <c r="H52" s="188"/>
     </row>
     <row r="53" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
@@ -16933,6 +16933,27 @@
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
     <mergeCell ref="C52:D52"/>
     <mergeCell ref="E52:F52"/>
     <mergeCell ref="G52:H52"/>
@@ -16949,27 +16970,6 @@
     <mergeCell ref="E43:F43"/>
     <mergeCell ref="G43:H43"/>
     <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -16996,54 +16996,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="157" t="s">
+      <c r="A1" s="158" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="158"/>
-      <c r="C1" s="158"/>
-      <c r="D1" s="158"/>
-      <c r="E1" s="158"/>
-      <c r="F1" s="159"/>
+      <c r="B1" s="159"/>
+      <c r="C1" s="159"/>
+      <c r="D1" s="159"/>
+      <c r="E1" s="159"/>
+      <c r="F1" s="160"/>
     </row>
     <row r="2" spans="1:6" ht="43.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="154" t="s">
+      <c r="A2" s="161" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="155"/>
-      <c r="C2" s="155"/>
-      <c r="D2" s="155"/>
-      <c r="E2" s="155"/>
-      <c r="F2" s="156"/>
+      <c r="B2" s="162"/>
+      <c r="C2" s="162"/>
+      <c r="D2" s="162"/>
+      <c r="E2" s="162"/>
+      <c r="F2" s="163"/>
     </row>
     <row r="3" spans="1:6" ht="43.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="160" t="s">
+      <c r="A3" s="164" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="161"/>
-      <c r="C3" s="161"/>
-      <c r="D3" s="161"/>
-      <c r="E3" s="161"/>
-      <c r="F3" s="162"/>
+      <c r="B3" s="165"/>
+      <c r="C3" s="165"/>
+      <c r="D3" s="165"/>
+      <c r="E3" s="165"/>
+      <c r="F3" s="166"/>
     </row>
     <row r="4" spans="1:6" ht="28.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="154" t="s">
+      <c r="A4" s="161" t="s">
         <v>725</v>
       </c>
-      <c r="B4" s="155"/>
-      <c r="C4" s="155"/>
-      <c r="D4" s="155"/>
-      <c r="E4" s="155"/>
-      <c r="F4" s="156"/>
+      <c r="B4" s="162"/>
+      <c r="C4" s="162"/>
+      <c r="D4" s="162"/>
+      <c r="E4" s="162"/>
+      <c r="F4" s="163"/>
     </row>
     <row r="5" spans="1:6" ht="28.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="163" t="s">
+      <c r="A5" s="167" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="164"/>
-      <c r="C5" s="164"/>
-      <c r="D5" s="164"/>
-      <c r="E5" s="164"/>
-      <c r="F5" s="165"/>
+      <c r="B5" s="168"/>
+      <c r="C5" s="168"/>
+      <c r="D5" s="168"/>
+      <c r="E5" s="168"/>
+      <c r="F5" s="169"/>
     </row>
     <row r="6" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6"/>
@@ -17072,10 +17072,10 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="160" t="s">
+      <c r="A8" s="164" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="161"/>
+      <c r="B8" s="165"/>
       <c r="C8" s="17">
         <v>0</v>
       </c>
@@ -17091,10 +17091,10 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="167" t="s">
+      <c r="A9" s="154" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="168"/>
+      <c r="B9" s="155"/>
       <c r="C9" s="12">
         <v>0</v>
       </c>
@@ -17110,10 +17110,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="169" t="s">
+      <c r="A10" s="171" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="169"/>
+      <c r="B10" s="171"/>
       <c r="C10" s="12">
         <v>0</v>
       </c>
@@ -17129,10 +17129,10 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="169" t="s">
+      <c r="A11" s="171" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="169"/>
+      <c r="B11" s="171"/>
       <c r="C11" s="12">
         <v>0</v>
       </c>
@@ -17148,10 +17148,10 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="169" t="s">
+      <c r="A12" s="171" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="169"/>
+      <c r="B12" s="171"/>
       <c r="C12" s="12">
         <v>0</v>
       </c>
@@ -17167,10 +17167,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="167" t="s">
+      <c r="A13" s="154" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="168"/>
+      <c r="B13" s="155"/>
       <c r="C13" s="12">
         <v>0</v>
       </c>
@@ -17186,10 +17186,10 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="167" t="s">
+      <c r="A14" s="154" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="168"/>
+      <c r="B14" s="155"/>
       <c r="C14" s="12">
         <v>0</v>
       </c>
@@ -17205,10 +17205,10 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="170" t="s">
+      <c r="A15" s="156" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="171"/>
+      <c r="B15" s="157"/>
       <c r="C15" s="19">
         <v>0</v>
       </c>
@@ -17225,11 +17225,11 @@
     </row>
     <row r="16" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
-      <c r="B16" s="166" t="s">
+      <c r="B16" s="170" t="s">
         <v>50</v>
       </c>
-      <c r="C16" s="166"/>
-      <c r="D16" s="166"/>
+      <c r="C16" s="170"/>
+      <c r="D16" s="170"/>
       <c r="E16" s="108">
         <f>SUM(E8:E15)</f>
         <v>0</v>
@@ -17248,93 +17248,88 @@
       <c r="A18" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="157" t="s">
+      <c r="B18" s="158" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="158"/>
-      <c r="D18" s="158"/>
-      <c r="E18" s="158"/>
-      <c r="F18" s="159"/>
+      <c r="C18" s="159"/>
+      <c r="D18" s="159"/>
+      <c r="E18" s="159"/>
+      <c r="F18" s="160"/>
     </row>
     <row r="19" spans="1:6" ht="28.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="64" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="154" t="s">
+      <c r="B19" s="161" t="s">
         <v>69</v>
       </c>
-      <c r="C19" s="155"/>
-      <c r="D19" s="155"/>
-      <c r="E19" s="155"/>
-      <c r="F19" s="156"/>
+      <c r="C19" s="162"/>
+      <c r="D19" s="162"/>
+      <c r="E19" s="162"/>
+      <c r="F19" s="163"/>
     </row>
     <row r="20" spans="1:6" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="64" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="154" t="s">
+      <c r="B20" s="161" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="155"/>
-      <c r="D20" s="155"/>
-      <c r="E20" s="155"/>
-      <c r="F20" s="156"/>
+      <c r="C20" s="162"/>
+      <c r="D20" s="162"/>
+      <c r="E20" s="162"/>
+      <c r="F20" s="163"/>
     </row>
     <row r="21" spans="1:6" ht="28.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="154" t="s">
+      <c r="B21" s="161" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="155"/>
-      <c r="D21" s="155"/>
-      <c r="E21" s="155"/>
-      <c r="F21" s="156"/>
+      <c r="C21" s="162"/>
+      <c r="D21" s="162"/>
+      <c r="E21" s="162"/>
+      <c r="F21" s="163"/>
     </row>
     <row r="22" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="64" t="s">
         <v>60</v>
       </c>
-      <c r="B22" s="154" t="s">
+      <c r="B22" s="161" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="155"/>
-      <c r="D22" s="155"/>
-      <c r="E22" s="155"/>
-      <c r="F22" s="156"/>
+      <c r="C22" s="162"/>
+      <c r="D22" s="162"/>
+      <c r="E22" s="162"/>
+      <c r="F22" s="163"/>
     </row>
     <row r="23" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="154" t="s">
+      <c r="B23" s="161" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="155"/>
-      <c r="D23" s="155"/>
-      <c r="E23" s="155"/>
-      <c r="F23" s="156"/>
+      <c r="C23" s="162"/>
+      <c r="D23" s="162"/>
+      <c r="E23" s="162"/>
+      <c r="F23" s="163"/>
     </row>
     <row r="24" spans="1:6" ht="43.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="64" t="s">
         <v>56</v>
       </c>
-      <c r="B24" s="154" t="s">
+      <c r="B24" s="161" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="155"/>
-      <c r="D24" s="155"/>
-      <c r="E24" s="155"/>
-      <c r="F24" s="156"/>
+      <c r="C24" s="162"/>
+      <c r="D24" s="162"/>
+      <c r="E24" s="162"/>
+      <c r="F24" s="163"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B19:F19"/>
     <mergeCell ref="B24:F24"/>
     <mergeCell ref="B20:F20"/>
     <mergeCell ref="A1:F1"/>
@@ -17351,6 +17346,11 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B19:F19"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -17361,8 +17361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C91" sqref="C91"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -17404,7 +17404,7 @@
       <c r="B2" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="172" t="s">
+      <c r="C2" s="174" t="s">
         <v>881</v>
       </c>
       <c r="D2" s="66">
@@ -17427,10 +17427,10 @@
       <c r="B3" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="173"/>
+      <c r="C3" s="175"/>
       <c r="D3" s="66">
         <f>SUMPRODUCT(($A$10:$A$250="Basic")*(D$10:D$250="Missing"))+0.5*SUMPRODUCT(($A$10:$A$250="Basic")*(D$10:D$250="Partial"))</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E3" s="66">
         <f>SUMPRODUCT(($A$10:$A$250="Basic")*(E$10:E$250="Missing"))+0.5*SUMPRODUCT(($A$10:$A$250="Basic")*(E$10:E$250="Partial"))</f>
@@ -17448,10 +17448,10 @@
       <c r="B4" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="173"/>
+      <c r="C4" s="175"/>
       <c r="D4" s="66">
         <f>SUMPRODUCT(($A$10:$A$250="Intermediate")*(D$10:D$250="Missing"))+0.5*SUMPRODUCT(($A$10:$A$250="Intermediate")*(D$10:D$250="Partial"))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E4" s="66">
         <f>SUMPRODUCT(($A$10:$A$250="Intermediate")*(E$10:E$250="Missing"))+0.5*SUMPRODUCT(($A$10:$A$250="Intermediate")*(E$10:E$250="Partial"))</f>
@@ -17469,10 +17469,10 @@
       <c r="B5" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="173"/>
+      <c r="C5" s="175"/>
       <c r="D5" s="66">
         <f>SUMPRODUCT(($A$10:$A$250="Intermediate")*(D$10:D$250="Completed"))+SUMPRODUCT(($A$10:$A$250="Intermediate")*(D$10:D$250="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$250="Intermediate")*(D$10:D$250="Partial"))</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E5" s="66">
         <f>SUMPRODUCT(($A$10:$A$250="Intermediate")*(E$10:E$250="Completed"))+SUMPRODUCT(($A$10:$A$250="Intermediate")*(E$10:E$250="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$250="Intermediate")*(E$10:E$250="Partial"))</f>
@@ -17490,7 +17490,7 @@
       <c r="B6" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="173"/>
+      <c r="C6" s="175"/>
       <c r="D6" s="66">
         <f>SUMPRODUCT(($A$10:$A$250="Advanced")*(D$10:D$250="Missing"))+0.5*SUMPRODUCT(($A$10:$A$250="Advanced")*(D$10:D$250="Partial"))</f>
         <v>2.5</v>
@@ -17511,7 +17511,7 @@
       <c r="B7" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="173"/>
+      <c r="C7" s="175"/>
       <c r="D7" s="66">
         <f>SUMPRODUCT(($A$10:$A$250="Advanced")*(D$10:D$250="Completed"))+SUMPRODUCT(($A$10:$A$250="Advanced")*(D$10:D$250="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$250="Advanced")*(D$10:D$250="Partial"))</f>
         <v>3.5</v>
@@ -17532,7 +17532,7 @@
       <c r="B8" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="173"/>
+      <c r="C8" s="175"/>
       <c r="D8" s="66">
         <f>SUMPRODUCT(($A$10:$A$250="Professional")*(D$10:D$250="Completed"))+SUMPRODUCT(($A$10:$A$250="Professional")*(D$10:D$250="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$250="Professional")*(D$10:D$250="Partial"))</f>
         <v>0</v>
@@ -17547,11 +17547,11 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="175" t="s">
+      <c r="A9" s="177" t="s">
         <v>88</v>
       </c>
-      <c r="B9" s="176"/>
-      <c r="C9" s="174"/>
+      <c r="B9" s="178"/>
+      <c r="C9" s="176"/>
       <c r="D9" s="66">
         <f>SUMPRODUCT(($A$10:$A$250="Innovative")*(D$10:D$250="Completed"))+SUMPRODUCT(($A$10:$A$250="Innovative")*(D$10:D$250="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$250="Innovative")*(D$10:D$250="Partial"))</f>
         <v>0</v>
@@ -17566,10 +17566,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="177" t="s">
+      <c r="A10" s="172" t="s">
         <v>724</v>
       </c>
-      <c r="B10" s="178"/>
+      <c r="B10" s="173"/>
       <c r="C10" s="8" t="s">
         <v>868</v>
       </c>
@@ -17692,10 +17692,10 @@
       <c r="F16" s="60"/>
     </row>
     <row r="17" spans="1:6" ht="28.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="177" t="s">
+      <c r="A17" s="172" t="s">
         <v>739</v>
       </c>
-      <c r="B17" s="178"/>
+      <c r="B17" s="173"/>
       <c r="C17" s="8" t="s">
         <v>870</v>
       </c>
@@ -17910,10 +17910,10 @@
       <c r="F28" s="60"/>
     </row>
     <row r="29" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="177" t="s">
+      <c r="A29" s="172" t="s">
         <v>740</v>
       </c>
-      <c r="B29" s="178"/>
+      <c r="B29" s="173"/>
       <c r="C29" s="8" t="s">
         <v>871</v>
       </c>
@@ -18396,10 +18396,10 @@
       <c r="F55" s="60"/>
     </row>
     <row r="56" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="177" t="s">
+      <c r="A56" s="172" t="s">
         <v>114</v>
       </c>
-      <c r="B56" s="178"/>
+      <c r="B56" s="173"/>
       <c r="C56" s="8" t="s">
         <v>89</v>
       </c>
@@ -18632,10 +18632,10 @@
       <c r="F68" s="60"/>
     </row>
     <row r="69" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="177" t="s">
+      <c r="A69" s="172" t="s">
         <v>135</v>
       </c>
-      <c r="B69" s="178"/>
+      <c r="B69" s="173"/>
       <c r="C69" s="8" t="s">
         <v>89</v>
       </c>
@@ -18796,10 +18796,10 @@
       <c r="F77" s="60"/>
     </row>
     <row r="78" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="177" t="s">
+      <c r="A78" s="172" t="s">
         <v>152</v>
       </c>
-      <c r="B78" s="178"/>
+      <c r="B78" s="173"/>
       <c r="C78" s="8" t="s">
         <v>89</v>
       </c>
@@ -18904,10 +18904,10 @@
       <c r="F83" s="60"/>
     </row>
     <row r="84" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="177" t="s">
+      <c r="A84" s="172" t="s">
         <v>163</v>
       </c>
-      <c r="B84" s="178"/>
+      <c r="B84" s="173"/>
       <c r="C84" s="8" t="s">
         <v>89</v>
       </c>
@@ -18932,7 +18932,7 @@
         <v>165</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E85" s="8" t="s">
         <v>74</v>
@@ -18950,7 +18950,7 @@
         <v>169</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E86" s="8" t="s">
         <v>74</v>
@@ -19076,7 +19076,7 @@
         <v>180</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E93" s="8" t="s">
         <v>74</v>
@@ -19138,10 +19138,10 @@
       <c r="F96" s="60"/>
     </row>
     <row r="97" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A97" s="177" t="s">
+      <c r="A97" s="172" t="s">
         <v>187</v>
       </c>
-      <c r="B97" s="178"/>
+      <c r="B97" s="173"/>
       <c r="C97" s="8" t="s">
         <v>89</v>
       </c>
@@ -19228,10 +19228,10 @@
       <c r="F101" s="60"/>
     </row>
     <row r="102" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A102" s="177" t="s">
+      <c r="A102" s="172" t="s">
         <v>194</v>
       </c>
-      <c r="B102" s="178"/>
+      <c r="B102" s="173"/>
       <c r="C102" s="8" t="s">
         <v>89</v>
       </c>
@@ -19374,10 +19374,10 @@
       <c r="F109" s="60"/>
     </row>
     <row r="110" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A110" s="177" t="s">
+      <c r="A110" s="172" t="s">
         <v>205</v>
       </c>
-      <c r="B110" s="178"/>
+      <c r="B110" s="173"/>
       <c r="C110" s="8" t="s">
         <v>89</v>
       </c>
@@ -19446,10 +19446,10 @@
       <c r="F113" s="60"/>
     </row>
     <row r="114" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A114" s="177" t="s">
+      <c r="A114" s="172" t="s">
         <v>212</v>
       </c>
-      <c r="B114" s="178"/>
+      <c r="B114" s="173"/>
       <c r="C114" s="8" t="s">
         <v>89</v>
       </c>
@@ -19518,10 +19518,10 @@
       <c r="F117" s="60"/>
     </row>
     <row r="118" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A118" s="177" t="s">
+      <c r="A118" s="172" t="s">
         <v>219</v>
       </c>
-      <c r="B118" s="178"/>
+      <c r="B118" s="173"/>
       <c r="C118" s="8" t="s">
         <v>823</v>
       </c>
@@ -19681,6 +19681,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C2:C9"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A56:B56"/>
     <mergeCell ref="A110:B110"/>
     <mergeCell ref="A114:B114"/>
     <mergeCell ref="A118:B118"/>
@@ -19690,11 +19695,6 @@
     <mergeCell ref="A84:B84"/>
     <mergeCell ref="A97:B97"/>
     <mergeCell ref="A102:B102"/>
-    <mergeCell ref="C2:C9"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A56:B56"/>
   </mergeCells>
   <conditionalFormatting sqref="A10 A33:A37 A39:A41 A109:A251 A95:A107 A56:A92 A14:A31">
     <cfRule type="beginsWith" dxfId="740" priority="292" stopIfTrue="1" operator="beginsWith" text="Innovative">
@@ -20678,7 +20678,7 @@
       <c r="B2" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="172" t="s">
+      <c r="C2" s="174" t="s">
         <v>862</v>
       </c>
       <c r="D2" s="66">
@@ -20701,7 +20701,7 @@
       <c r="B3" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="173"/>
+      <c r="C3" s="175"/>
       <c r="D3" s="66">
         <f>SUMPRODUCT(($A$10:$A$241="Basic")*(D$10:D$241="Missing"))+0.5*SUMPRODUCT(($A$10:$A$241="Basic")*(D$10:D$241="Partial"))</f>
         <v>10</v>
@@ -20722,7 +20722,7 @@
       <c r="B4" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="173"/>
+      <c r="C4" s="175"/>
       <c r="D4" s="66">
         <f>SUMPRODUCT(($A$10:$A$241="Intermediate")*(D$10:D$241="Missing"))+0.5*SUMPRODUCT(($A$10:$A$241="Intermediate")*(D$10:D$241="Partial"))</f>
         <v>10</v>
@@ -20743,7 +20743,7 @@
       <c r="B5" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="173"/>
+      <c r="C5" s="175"/>
       <c r="D5" s="66">
         <f>SUMPRODUCT(($A$10:$A$241="Intermediate")*(D$10:D$241="Completed"))+SUMPRODUCT(($A$10:$A$241="Intermediate")*(D$10:D$241="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$241="Intermediate")*(D$10:D$241="Partial"))</f>
         <v>0</v>
@@ -20764,7 +20764,7 @@
       <c r="B6" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="173"/>
+      <c r="C6" s="175"/>
       <c r="D6" s="66">
         <f>SUMPRODUCT(($A$10:$A$241="Advanced")*(D$10:D$241="Missing"))+0.5*SUMPRODUCT(($A$10:$A$241="Advanced")*(D$10:D$241="Partial"))</f>
         <v>2</v>
@@ -20785,7 +20785,7 @@
       <c r="B7" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="173"/>
+      <c r="C7" s="175"/>
       <c r="D7" s="66">
         <f>SUMPRODUCT(($A$10:$A$241="Advanced")*(D$10:D$241="Completed"))+SUMPRODUCT(($A$10:$A$241="Advanced")*(D$10:D$241="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$241="Advanced")*(D$10:D$241="Partial"))</f>
         <v>1</v>
@@ -20806,7 +20806,7 @@
       <c r="B8" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="173"/>
+      <c r="C8" s="175"/>
       <c r="D8" s="66">
         <f>SUMPRODUCT(($A$10:$A$241="Professional")*(D$10:D$241="Completed"))+SUMPRODUCT(($A$10:$A$241="Professional")*(D$10:D$241="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$241="Professional")*(D$10:D$241="Partial"))</f>
         <v>0</v>
@@ -20821,11 +20821,11 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="175" t="s">
+      <c r="A9" s="177" t="s">
         <v>88</v>
       </c>
-      <c r="B9" s="176"/>
-      <c r="C9" s="174"/>
+      <c r="B9" s="178"/>
+      <c r="C9" s="176"/>
       <c r="D9" s="66">
         <f>SUMPRODUCT(($A$10:$A$241="Innovative")*(D$10:D$241="Completed"))+SUMPRODUCT(($A$10:$A$241="Innovative")*(D$10:D$241="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$241="Innovative")*(D$10:D$241="Partial"))</f>
         <v>0</v>
@@ -20840,10 +20840,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="177" t="s">
+      <c r="A10" s="172" t="s">
         <v>810</v>
       </c>
-      <c r="B10" s="178"/>
+      <c r="B10" s="173"/>
       <c r="C10" s="8" t="s">
         <v>863</v>
       </c>
@@ -20930,10 +20930,10 @@
       <c r="F14" s="60"/>
     </row>
     <row r="15" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="177" t="s">
+      <c r="A15" s="172" t="s">
         <v>249</v>
       </c>
-      <c r="B15" s="178"/>
+      <c r="B15" s="173"/>
       <c r="C15" s="8" t="s">
         <v>89</v>
       </c>
@@ -21074,10 +21074,10 @@
       <c r="F22" s="60"/>
     </row>
     <row r="23" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="177" t="s">
+      <c r="A23" s="172" t="s">
         <v>257</v>
       </c>
-      <c r="B23" s="178"/>
+      <c r="B23" s="173"/>
       <c r="C23" s="8" t="s">
         <v>89</v>
       </c>
@@ -21218,10 +21218,10 @@
       <c r="F30" s="60"/>
     </row>
     <row r="31" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="177" t="s">
+      <c r="A31" s="172" t="s">
         <v>262</v>
       </c>
-      <c r="B31" s="178"/>
+      <c r="B31" s="173"/>
       <c r="C31" s="8" t="s">
         <v>89</v>
       </c>
@@ -21686,10 +21686,10 @@
       <c r="F56" s="60"/>
     </row>
     <row r="57" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="177" t="s">
+      <c r="A57" s="172" t="s">
         <v>288</v>
       </c>
-      <c r="B57" s="178"/>
+      <c r="B57" s="173"/>
       <c r="C57" s="73" t="s">
         <v>832</v>
       </c>
@@ -22064,10 +22064,10 @@
       <c r="F77" s="60"/>
     </row>
     <row r="78" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="177" t="s">
+      <c r="A78" s="172" t="s">
         <v>301</v>
       </c>
-      <c r="B78" s="178"/>
+      <c r="B78" s="173"/>
       <c r="C78" s="8" t="s">
         <v>89</v>
       </c>
@@ -23072,7 +23072,7 @@
       <c r="B2" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="172" t="s">
+      <c r="C2" s="174" t="s">
         <v>830</v>
       </c>
       <c r="D2" s="66">
@@ -23095,7 +23095,7 @@
       <c r="B3" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="173"/>
+      <c r="C3" s="175"/>
       <c r="D3" s="66">
         <f>SUMPRODUCT(($A$10:$A$177="Basic")*(D$10:D$177="Missing"))+0.5*SUMPRODUCT(($A$10:$A$177="Basic")*(D$10:D$177="Partial"))</f>
         <v>2</v>
@@ -23116,7 +23116,7 @@
       <c r="B4" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="173"/>
+      <c r="C4" s="175"/>
       <c r="D4" s="66">
         <f>SUMPRODUCT(($A$10:$A$177="Intermediate")*(D$10:D$177="Missing"))+0.5*SUMPRODUCT(($A$10:$A$177="Intermediate")*(D$10:D$177="Partial"))</f>
         <v>2</v>
@@ -23137,7 +23137,7 @@
       <c r="B5" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="173"/>
+      <c r="C5" s="175"/>
       <c r="D5" s="66">
         <f>SUMPRODUCT(($A$10:$A$177="Intermediate")*(D$10:D$177="Completed"))+SUMPRODUCT(($A$10:$A$177="Intermediate")*(D$10:D$177="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$177="Intermediate")*(D$10:D$177="Partial"))</f>
         <v>1</v>
@@ -23158,7 +23158,7 @@
       <c r="B6" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="173"/>
+      <c r="C6" s="175"/>
       <c r="D6" s="66">
         <f>SUMPRODUCT(($A$10:$A$177="Advanced")*(D$10:D$177="Missing"))+0.5*SUMPRODUCT(($A$10:$A$177="Advanced")*(D$10:D$177="Partial"))</f>
         <v>0</v>
@@ -23179,7 +23179,7 @@
       <c r="B7" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="173"/>
+      <c r="C7" s="175"/>
       <c r="D7" s="66">
         <f>SUMPRODUCT(($A$10:$A$177="Advanced")*(D$10:D$177="Completed"))+SUMPRODUCT(($A$10:$A$177="Advanced")*(D$10:D$177="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$177="Advanced")*(D$10:D$177="Partial"))</f>
         <v>0</v>
@@ -23200,7 +23200,7 @@
       <c r="B8" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="173"/>
+      <c r="C8" s="175"/>
       <c r="D8" s="66">
         <f>SUMPRODUCT(($A$10:$A$177="Professional")*(D$10:D$177="Completed"))+SUMPRODUCT(($A$10:$A$177="Professional")*(D$10:D$177="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$177="Professional")*(D$10:D$177="Partial"))</f>
         <v>0</v>
@@ -23215,11 +23215,11 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="175" t="s">
+      <c r="A9" s="177" t="s">
         <v>88</v>
       </c>
-      <c r="B9" s="176"/>
-      <c r="C9" s="174"/>
+      <c r="B9" s="178"/>
+      <c r="C9" s="176"/>
       <c r="D9" s="66">
         <f>SUMPRODUCT(($A$10:$A$177="Innovative")*(D$10:D$177="Completed"))+SUMPRODUCT(($A$10:$A$177="Innovative")*(D$10:D$177="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$177="Innovative")*(D$10:D$177="Partial"))</f>
         <v>0</v>
@@ -23234,10 +23234,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="177" t="s">
+      <c r="A10" s="172" t="s">
         <v>237</v>
       </c>
-      <c r="B10" s="178"/>
+      <c r="B10" s="173"/>
       <c r="C10" s="8" t="s">
         <v>89</v>
       </c>
@@ -23450,10 +23450,10 @@
       <c r="F21" s="60"/>
     </row>
     <row r="22" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="177" t="s">
+      <c r="A22" s="172" t="s">
         <v>534</v>
       </c>
-      <c r="B22" s="178"/>
+      <c r="B22" s="173"/>
       <c r="C22" s="8" t="s">
         <v>89</v>
       </c>
@@ -23612,10 +23612,10 @@
       <c r="F30" s="60"/>
     </row>
     <row r="31" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="177" t="s">
+      <c r="A31" s="172" t="s">
         <v>550</v>
       </c>
-      <c r="B31" s="178"/>
+      <c r="B31" s="173"/>
       <c r="C31" s="8" t="s">
         <v>89</v>
       </c>
@@ -23828,10 +23828,10 @@
       <c r="F42" s="60"/>
     </row>
     <row r="43" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="177" t="s">
+      <c r="A43" s="172" t="s">
         <v>661</v>
       </c>
-      <c r="B43" s="178"/>
+      <c r="B43" s="173"/>
       <c r="C43" s="8" t="s">
         <v>89</v>
       </c>
@@ -24120,7 +24120,7 @@
       <c r="B2" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="172" t="s">
+      <c r="C2" s="174" t="s">
         <v>384</v>
       </c>
       <c r="D2" s="66">
@@ -24143,7 +24143,7 @@
       <c r="B3" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="173"/>
+      <c r="C3" s="175"/>
       <c r="D3" s="66">
         <f>SUMPRODUCT(($A$10:$A$248="Basic")*(D$10:D$248="Missing"))+0.5*SUMPRODUCT(($A$10:$A$248="Basic")*(D$10:D$248="Partial"))</f>
         <v>0</v>
@@ -24164,7 +24164,7 @@
       <c r="B4" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="173"/>
+      <c r="C4" s="175"/>
       <c r="D4" s="66">
         <f>SUMPRODUCT(($A$10:$A$248="Intermediate")*(D$10:D$248="Missing"))+0.5*SUMPRODUCT(($A$10:$A$248="Intermediate")*(D$10:D$248="Partial"))</f>
         <v>0</v>
@@ -24185,7 +24185,7 @@
       <c r="B5" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="173"/>
+      <c r="C5" s="175"/>
       <c r="D5" s="66">
         <f>SUMPRODUCT(($A$10:$A$248="Intermediate")*(D$10:D$248="Completed"))+SUMPRODUCT(($A$10:$A$248="Intermediate")*(D$10:D$248="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$248="Intermediate")*(D$10:D$248="Partial"))</f>
         <v>1</v>
@@ -24206,7 +24206,7 @@
       <c r="B6" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="173"/>
+      <c r="C6" s="175"/>
       <c r="D6" s="66">
         <f>SUMPRODUCT(($A$10:$A$248="Advanced")*(D$10:D$248="Missing"))+0.5*SUMPRODUCT(($A$10:$A$248="Advanced")*(D$10:D$248="Partial"))</f>
         <v>0</v>
@@ -24227,7 +24227,7 @@
       <c r="B7" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="173"/>
+      <c r="C7" s="175"/>
       <c r="D7" s="66">
         <f>SUMPRODUCT(($A$10:$A$248="Advanced")*(D$10:D$248="Completed"))+SUMPRODUCT(($A$10:$A$248="Advanced")*(D$10:D$248="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$248="Advanced")*(D$10:D$248="Partial"))</f>
         <v>0</v>
@@ -24248,7 +24248,7 @@
       <c r="B8" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="173"/>
+      <c r="C8" s="175"/>
       <c r="D8" s="66">
         <f>SUMPRODUCT(($A$10:$A$248="Professional")*(D$10:D$248="Completed"))+SUMPRODUCT(($A$10:$A$248="Professional")*(D$10:D$248="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$248="Professional")*(D$10:D$248="Partial"))</f>
         <v>0</v>
@@ -24263,11 +24263,11 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="175" t="s">
+      <c r="A9" s="177" t="s">
         <v>88</v>
       </c>
-      <c r="B9" s="176"/>
-      <c r="C9" s="174"/>
+      <c r="B9" s="178"/>
+      <c r="C9" s="176"/>
       <c r="D9" s="66">
         <f>SUMPRODUCT(($A$10:$A$248="Innovative")*(D$10:D$248="Completed"))+SUMPRODUCT(($A$10:$A$248="Innovative")*(D$10:D$248="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$248="Innovative")*(D$10:D$248="Partial"))</f>
         <v>0</v>
@@ -24282,10 +24282,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="177" t="s">
+      <c r="A10" s="172" t="s">
         <v>385</v>
       </c>
-      <c r="B10" s="178"/>
+      <c r="B10" s="173"/>
       <c r="C10" s="8" t="s">
         <v>89</v>
       </c>
@@ -24390,10 +24390,10 @@
       <c r="F15" s="60"/>
     </row>
     <row r="16" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="177" t="s">
+      <c r="A16" s="172" t="s">
         <v>396</v>
       </c>
-      <c r="B16" s="178"/>
+      <c r="B16" s="173"/>
       <c r="C16" s="8" t="s">
         <v>89</v>
       </c>
@@ -24498,10 +24498,10 @@
       <c r="F21" s="60"/>
     </row>
     <row r="22" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="177" t="s">
+      <c r="A22" s="172" t="s">
         <v>407</v>
       </c>
-      <c r="B22" s="178"/>
+      <c r="B22" s="173"/>
       <c r="C22" s="8" t="s">
         <v>826</v>
       </c>
@@ -24624,10 +24624,10 @@
       <c r="F28" s="60"/>
     </row>
     <row r="29" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="177" t="s">
+      <c r="A29" s="172" t="s">
         <v>420</v>
       </c>
-      <c r="B29" s="178"/>
+      <c r="B29" s="173"/>
       <c r="C29" s="8" t="s">
         <v>824</v>
       </c>
@@ -24768,10 +24768,10 @@
       <c r="F36" s="60"/>
     </row>
     <row r="37" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="177" t="s">
+      <c r="A37" s="172" t="s">
         <v>435</v>
       </c>
-      <c r="B37" s="178"/>
+      <c r="B37" s="173"/>
       <c r="C37" s="8" t="s">
         <v>825</v>
       </c>
@@ -24894,10 +24894,10 @@
       <c r="F43" s="60"/>
     </row>
     <row r="44" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="177" t="s">
+      <c r="A44" s="172" t="s">
         <v>448</v>
       </c>
-      <c r="B44" s="178"/>
+      <c r="B44" s="173"/>
       <c r="C44" s="8" t="s">
         <v>89</v>
       </c>
@@ -25581,7 +25581,7 @@
       <c r="B2" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="172" t="s">
+      <c r="C2" s="174" t="s">
         <v>473</v>
       </c>
       <c r="D2" s="66">
@@ -25604,7 +25604,7 @@
       <c r="B3" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="173"/>
+      <c r="C3" s="175"/>
       <c r="D3" s="66">
         <f>SUMPRODUCT(($A$10:$A$227="Basic")*(D$10:D$227="Missing"))+0.5*SUMPRODUCT(($A$10:$A$227="Basic")*(D$10:D$227="Partial"))</f>
         <v>1</v>
@@ -25625,7 +25625,7 @@
       <c r="B4" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="173"/>
+      <c r="C4" s="175"/>
       <c r="D4" s="66">
         <f>SUMPRODUCT(($A$10:$A$227="Intermediate")*(D$10:D$227="Missing"))+0.5*SUMPRODUCT(($A$10:$A$227="Intermediate")*(D$10:D$227="Partial"))</f>
         <v>2</v>
@@ -25646,7 +25646,7 @@
       <c r="B5" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="173"/>
+      <c r="C5" s="175"/>
       <c r="D5" s="66">
         <f>SUMPRODUCT(($A$10:$A$227="Intermediate")*(D$10:D$227="Completed"))+SUMPRODUCT(($A$10:$A$227="Intermediate")*(D$10:D$227="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$227="Intermediate")*(D$10:D$227="Partial"))</f>
         <v>6</v>
@@ -25667,7 +25667,7 @@
       <c r="B6" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="173"/>
+      <c r="C6" s="175"/>
       <c r="D6" s="66">
         <f>SUMPRODUCT(($A$10:$A$227="Advanced")*(D$10:D$227="Missing"))+0.5*SUMPRODUCT(($A$10:$A$227="Advanced")*(D$10:D$227="Partial"))</f>
         <v>0</v>
@@ -25688,7 +25688,7 @@
       <c r="B7" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="173"/>
+      <c r="C7" s="175"/>
       <c r="D7" s="66">
         <f>SUMPRODUCT(($A$10:$A$227="Advanced")*(D$10:D$227="Completed"))+SUMPRODUCT(($A$10:$A$227="Advanced")*(D$10:D$227="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$227="Advanced")*(D$10:D$227="Partial"))</f>
         <v>0</v>
@@ -25709,7 +25709,7 @@
       <c r="B8" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="173"/>
+      <c r="C8" s="175"/>
       <c r="D8" s="66">
         <f>SUMPRODUCT(($A$10:$A$227="Professional")*(D$10:D$227="Completed"))+SUMPRODUCT(($A$10:$A$227="Professional")*(D$10:D$227="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$227="Professional")*(D$10:D$227="Partial"))</f>
         <v>0</v>
@@ -25724,11 +25724,11 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="175" t="s">
+      <c r="A9" s="177" t="s">
         <v>88</v>
       </c>
-      <c r="B9" s="176"/>
-      <c r="C9" s="174"/>
+      <c r="B9" s="178"/>
+      <c r="C9" s="176"/>
       <c r="D9" s="66">
         <f>SUMPRODUCT(($A$10:$A$227="Innovative")*(D$10:D$227="Completed"))+SUMPRODUCT(($A$10:$A$227="Innovative")*(D$10:D$227="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$227="Innovative")*(D$10:D$227="Partial"))</f>
         <v>0</v>
@@ -25743,10 +25743,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="177" t="s">
+      <c r="A10" s="172" t="s">
         <v>474</v>
       </c>
-      <c r="B10" s="178"/>
+      <c r="B10" s="173"/>
       <c r="C10" s="8" t="s">
         <v>89</v>
       </c>
@@ -26087,10 +26087,10 @@
       <c r="F28" s="60"/>
     </row>
     <row r="29" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="177" t="s">
+      <c r="A29" s="172" t="s">
         <v>511</v>
       </c>
-      <c r="B29" s="178"/>
+      <c r="B29" s="173"/>
       <c r="C29" s="8" t="s">
         <v>821</v>
       </c>
@@ -26303,10 +26303,10 @@
       <c r="F40" s="60"/>
     </row>
     <row r="41" spans="1:6" s="26" customFormat="1" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="177" t="s">
+      <c r="A41" s="172" t="s">
         <v>114</v>
       </c>
-      <c r="B41" s="178"/>
+      <c r="B41" s="173"/>
       <c r="C41" s="8" t="s">
         <v>89</v>
       </c>
@@ -26465,10 +26465,10 @@
       <c r="F49" s="60"/>
     </row>
     <row r="50" spans="1:6" s="26" customFormat="1" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="177" t="s">
+      <c r="A50" s="172" t="s">
         <v>589</v>
       </c>
-      <c r="B50" s="178"/>
+      <c r="B50" s="173"/>
       <c r="C50" s="73" t="s">
         <v>822</v>
       </c>
@@ -26554,7 +26554,7 @@
       </c>
       <c r="F54" s="60"/>
     </row>
-    <row r="55" spans="1:6" s="26" customFormat="1" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" s="26" customFormat="1" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="69" t="s">
         <v>98</v>
       </c>
@@ -27037,7 +27037,7 @@
       <c r="B2" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="172" t="s">
+      <c r="C2" s="174" t="s">
         <v>610</v>
       </c>
       <c r="D2" s="66">
@@ -27060,7 +27060,7 @@
       <c r="B3" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="173"/>
+      <c r="C3" s="175"/>
       <c r="D3" s="66">
         <f>SUMPRODUCT(($A$10:$A$240="Basic")*(D$10:D$240="Missing"))+0.5*SUMPRODUCT(($A$10:$A$240="Basic")*(D$10:D$240="Partial"))</f>
         <v>3</v>
@@ -27081,7 +27081,7 @@
       <c r="B4" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="173"/>
+      <c r="C4" s="175"/>
       <c r="D4" s="66">
         <f>SUMPRODUCT(($A$10:$A$240="Intermediate")*(D$10:D$240="Missing"))+0.5*SUMPRODUCT(($A$10:$A$240="Intermediate")*(D$10:D$240="Partial"))</f>
         <v>3</v>
@@ -27102,7 +27102,7 @@
       <c r="B5" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="173"/>
+      <c r="C5" s="175"/>
       <c r="D5" s="66">
         <f>SUMPRODUCT(($A$10:$A$240="Intermediate")*(D$10:D$240="Completed"))+SUMPRODUCT(($A$10:$A$240="Intermediate")*(D$10:D$240="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$240="Intermediate")*(D$10:D$240="Partial"))</f>
         <v>0</v>
@@ -27123,7 +27123,7 @@
       <c r="B6" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="173"/>
+      <c r="C6" s="175"/>
       <c r="D6" s="66">
         <f>SUMPRODUCT(($A$10:$A$240="Advanced")*(D$10:D$240="Missing"))+0.5*SUMPRODUCT(($A$10:$A$240="Advanced")*(D$10:D$240="Partial"))</f>
         <v>0</v>
@@ -27144,7 +27144,7 @@
       <c r="B7" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="173"/>
+      <c r="C7" s="175"/>
       <c r="D7" s="66">
         <f>SUMPRODUCT(($A$10:$A$240="Advanced")*(D$10:D$240="Completed"))+SUMPRODUCT(($A$10:$A$240="Advanced")*(D$10:D$240="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$240="Advanced")*(D$10:D$240="Partial"))</f>
         <v>0</v>
@@ -27165,7 +27165,7 @@
       <c r="B8" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="173"/>
+      <c r="C8" s="175"/>
       <c r="D8" s="66">
         <f>SUMPRODUCT(($A$10:$A$240="Professional")*(D$10:D$240="Completed"))+SUMPRODUCT(($A$10:$A$240="Professional")*(D$10:D$240="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$240="Professional")*(D$10:D$240="Partial"))</f>
         <v>0</v>
@@ -27180,11 +27180,11 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="175" t="s">
+      <c r="A9" s="177" t="s">
         <v>88</v>
       </c>
-      <c r="B9" s="176"/>
-      <c r="C9" s="174"/>
+      <c r="B9" s="178"/>
+      <c r="C9" s="176"/>
       <c r="D9" s="66">
         <f>SUMPRODUCT(($A$10:$A$240="Innovative")*(D$10:D$240="Completed"))+SUMPRODUCT(($A$10:$A$240="Innovative")*(D$10:D$240="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$240="Innovative")*(D$10:D$240="Partial"))</f>
         <v>0</v>
@@ -27199,10 +27199,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="177" t="s">
+      <c r="A10" s="172" t="s">
         <v>611</v>
       </c>
-      <c r="B10" s="178"/>
+      <c r="B10" s="173"/>
       <c r="C10" s="73" t="s">
         <v>815</v>
       </c>
@@ -27415,10 +27415,10 @@
       <c r="F21" s="60"/>
     </row>
     <row r="22" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="177" t="s">
+      <c r="A22" s="172" t="s">
         <v>634</v>
       </c>
-      <c r="B22" s="178"/>
+      <c r="B22" s="173"/>
       <c r="C22" s="8" t="s">
         <v>89</v>
       </c>
@@ -27631,10 +27631,10 @@
       <c r="F33" s="60"/>
     </row>
     <row r="34" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="177" t="s">
+      <c r="A34" s="172" t="s">
         <v>811</v>
       </c>
-      <c r="B34" s="178"/>
+      <c r="B34" s="173"/>
       <c r="C34" s="8" t="s">
         <v>816</v>
       </c>
@@ -27757,10 +27757,10 @@
       <c r="F40" s="60"/>
     </row>
     <row r="41" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="177" t="s">
+      <c r="A41" s="172" t="s">
         <v>680</v>
       </c>
-      <c r="B41" s="178"/>
+      <c r="B41" s="173"/>
       <c r="C41" s="8" t="s">
         <v>89</v>
       </c>
@@ -28188,65 +28188,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="189" t="s">
+      <c r="A1" s="179" t="s">
         <v>705</v>
       </c>
       <c r="B1" s="75"/>
-      <c r="C1" s="179" t="s">
+      <c r="C1" s="194" t="s">
         <v>689</v>
       </c>
-      <c r="D1" s="180"/>
-      <c r="E1" s="179" t="s">
+      <c r="D1" s="195"/>
+      <c r="E1" s="194" t="s">
         <v>690</v>
       </c>
-      <c r="F1" s="180"/>
-      <c r="G1" s="179" t="s">
+      <c r="F1" s="195"/>
+      <c r="G1" s="194" t="s">
         <v>691</v>
       </c>
-      <c r="H1" s="180"/>
+      <c r="H1" s="195"/>
     </row>
     <row r="2" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="190"/>
+      <c r="A2" s="180"/>
       <c r="B2" s="75"/>
-      <c r="C2" s="181" t="s">
+      <c r="C2" s="196" t="s">
         <v>688</v>
       </c>
-      <c r="D2" s="182"/>
-      <c r="E2" s="181" t="s">
+      <c r="D2" s="197"/>
+      <c r="E2" s="196" t="s">
         <v>688</v>
       </c>
-      <c r="F2" s="182"/>
-      <c r="G2" s="181" t="s">
+      <c r="F2" s="197"/>
+      <c r="G2" s="196" t="s">
         <v>688</v>
       </c>
-      <c r="H2" s="182"/>
-      <c r="J2" s="192" t="s">
+      <c r="H2" s="197"/>
+      <c r="J2" s="182" t="s">
         <v>707</v>
       </c>
-      <c r="K2" s="193"/>
-      <c r="L2" s="194"/>
+      <c r="K2" s="183"/>
+      <c r="L2" s="184"/>
     </row>
     <row r="3" spans="1:12" ht="22.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="191"/>
+      <c r="A3" s="181"/>
       <c r="B3" s="76"/>
-      <c r="C3" s="183">
+      <c r="C3" s="192">
         <f>MAX(0,MIN(1,IF((A6+C6) &lt;= 0.95, ROUND(A6+C6,2), FLOOR((0.95+(A6+C6-0.95)/5),2))))</f>
-        <v>0.13</v>
-      </c>
-      <c r="D3" s="184"/>
-      <c r="E3" s="183">
+        <v>0.18</v>
+      </c>
+      <c r="D3" s="193"/>
+      <c r="E3" s="192">
         <f>MAX(0,MIN(1,IF((A6+E6) &lt;= 0.95, ROUND(A6+E6,2), FLOOR((0.95+(A6+E6-0.95)/5),2))))</f>
         <v>0</v>
       </c>
-      <c r="F3" s="184"/>
-      <c r="G3" s="183">
+      <c r="F3" s="193"/>
+      <c r="G3" s="192">
         <f>MAX(0,MIN(1,IF((A6+G6) &lt;= 0.95, ROUND(A6+G6,2), FLOOR((0.95+(A6+G6-0.95)/5),2))))</f>
-        <v>0.22</v>
-      </c>
-      <c r="H3" s="184"/>
-      <c r="J3" s="195"/>
-      <c r="K3" s="196"/>
-      <c r="L3" s="197"/>
+        <v>0.23</v>
+      </c>
+      <c r="H3" s="193"/>
+      <c r="J3" s="185"/>
+      <c r="K3" s="186"/>
+      <c r="L3" s="187"/>
     </row>
     <row r="4" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
@@ -28263,19 +28263,19 @@
         <v>692</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="118" t="s">
+      <c r="C5" s="145" t="s">
         <v>693</v>
       </c>
-      <c r="D5" s="120"/>
-      <c r="E5" s="118" t="s">
+      <c r="D5" s="147"/>
+      <c r="E5" s="145" t="s">
         <v>694</v>
       </c>
-      <c r="F5" s="120"/>
-      <c r="G5" s="118" t="s">
+      <c r="F5" s="147"/>
+      <c r="G5" s="145" t="s">
         <v>695</v>
       </c>
-      <c r="H5" s="120"/>
-      <c r="J5" s="127" t="s">
+      <c r="H5" s="147"/>
+      <c r="J5" s="139" t="s">
         <v>721</v>
       </c>
       <c r="K5" s="31"/>
@@ -28289,22 +28289,22 @@
         <v>0.85</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="186">
+      <c r="C6" s="189">
         <f>D15+D24+D33+D42+D51+D60</f>
-        <v>-0.72250000000000003</v>
-      </c>
-      <c r="D6" s="187"/>
-      <c r="E6" s="186">
+        <v>-0.6725000000000001</v>
+      </c>
+      <c r="D6" s="190"/>
+      <c r="E6" s="189">
         <f>F15+F24+F33+F42+F51+F60</f>
-        <v>-0.97750000000000004</v>
-      </c>
-      <c r="F6" s="187"/>
-      <c r="G6" s="186">
+        <v>-0.95250000000000001</v>
+      </c>
+      <c r="F6" s="190"/>
+      <c r="G6" s="189">
         <f>H15+H24+H33+H42+H51+H60</f>
-        <v>-0.62999999999999989</v>
-      </c>
-      <c r="H6" s="187"/>
-      <c r="J6" s="128"/>
+        <v>-0.61749999999999994</v>
+      </c>
+      <c r="H6" s="190"/>
+      <c r="J6" s="140"/>
       <c r="K6" s="31"/>
       <c r="L6" s="104" t="s">
         <v>714</v>
@@ -28313,19 +28313,19 @@
     <row r="7" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="11"/>
-      <c r="C7" s="188" t="s">
+      <c r="C7" s="191" t="s">
         <v>696</v>
       </c>
-      <c r="D7" s="188"/>
-      <c r="E7" s="188" t="s">
+      <c r="D7" s="191"/>
+      <c r="E7" s="191" t="s">
         <v>697</v>
       </c>
-      <c r="F7" s="188"/>
-      <c r="G7" s="188" t="s">
+      <c r="F7" s="191"/>
+      <c r="G7" s="191" t="s">
         <v>698</v>
       </c>
-      <c r="H7" s="188"/>
-      <c r="J7" s="128"/>
+      <c r="H7" s="191"/>
+      <c r="J7" s="140"/>
       <c r="K7" s="105"/>
       <c r="L7" s="104" t="s">
         <v>715</v>
@@ -28356,7 +28356,7 @@
       <c r="H8" s="87" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="128"/>
+      <c r="J8" s="140"/>
       <c r="K8" s="105"/>
       <c r="L8" s="104" t="s">
         <v>716</v>
@@ -28392,7 +28392,7 @@
         <f t="shared" ref="H9:H14" si="2">B9*G9</f>
         <v>0</v>
       </c>
-      <c r="J9" s="128"/>
+      <c r="J9" s="140"/>
       <c r="K9" s="105"/>
       <c r="L9" s="104" t="s">
         <v>717</v>
@@ -28405,30 +28405,30 @@
       </c>
       <c r="B10" s="11">
         <f>TCRs!$D$3</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C10" s="82">
         <v>-0.02</v>
       </c>
       <c r="D10" s="97">
         <f t="shared" si="0"/>
-        <v>-0.12</v>
+        <v>-0.08</v>
       </c>
       <c r="E10" s="84">
         <v>-0.01</v>
       </c>
       <c r="F10" s="97">
         <f t="shared" si="1"/>
-        <v>-0.06</v>
+        <v>-0.04</v>
       </c>
       <c r="G10" s="100">
         <v>-5.0000000000000001E-3</v>
       </c>
       <c r="H10" s="97">
         <f t="shared" si="2"/>
-        <v>-0.03</v>
-      </c>
-      <c r="J10" s="128"/>
+        <v>-0.02</v>
+      </c>
+      <c r="J10" s="140"/>
       <c r="K10" s="105"/>
       <c r="L10" s="104" t="s">
         <v>718</v>
@@ -28441,30 +28441,30 @@
       </c>
       <c r="B11" s="11">
         <f>TCRs!$D$4</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11" s="82">
         <v>-0.01</v>
       </c>
       <c r="D11" s="97">
         <f t="shared" si="0"/>
-        <v>-0.03</v>
+        <v>-0.02</v>
       </c>
       <c r="E11" s="100">
         <v>-5.0000000000000001E-3</v>
       </c>
       <c r="F11" s="97">
         <f t="shared" si="1"/>
-        <v>-1.4999999999999999E-2</v>
+        <v>-0.01</v>
       </c>
       <c r="G11" s="80">
         <v>-2.5000000000000001E-3</v>
       </c>
       <c r="H11" s="97">
         <f t="shared" si="2"/>
-        <v>-7.4999999999999997E-3</v>
-      </c>
-      <c r="J11" s="128"/>
+        <v>-5.0000000000000001E-3</v>
+      </c>
+      <c r="J11" s="140"/>
       <c r="K11" s="105"/>
       <c r="L11" s="104" t="s">
         <v>719</v>
@@ -28500,7 +28500,7 @@
         <f t="shared" si="2"/>
         <v>1.7500000000000002E-2</v>
       </c>
-      <c r="J12" s="129"/>
+      <c r="J12" s="141"/>
       <c r="K12" s="105"/>
       <c r="L12" s="103" t="s">
         <v>720</v>
@@ -28576,38 +28576,38 @@
       </c>
       <c r="D15" s="99">
         <f>SUM(D9:D14)</f>
-        <v>-0.13250000000000001</v>
+        <v>-8.2500000000000004E-2</v>
       </c>
       <c r="E15" s="79" t="s">
         <v>16</v>
       </c>
       <c r="F15" s="99">
         <f>SUM(F9:F14)</f>
-        <v>-5.7499999999999996E-2</v>
+        <v>-3.2500000000000001E-2</v>
       </c>
       <c r="G15" s="79" t="s">
         <v>16</v>
       </c>
       <c r="H15" s="99">
         <f>SUM(H9:H14)</f>
-        <v>-1.9999999999999997E-2</v>
+        <v>-7.4999999999999997E-3</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="11"/>
-      <c r="C16" s="185" t="s">
+      <c r="C16" s="188" t="s">
         <v>696</v>
       </c>
-      <c r="D16" s="185"/>
-      <c r="E16" s="185" t="s">
+      <c r="D16" s="188"/>
+      <c r="E16" s="188" t="s">
         <v>697</v>
       </c>
-      <c r="F16" s="185"/>
-      <c r="G16" s="185" t="s">
+      <c r="F16" s="188"/>
+      <c r="G16" s="188" t="s">
         <v>698</v>
       </c>
-      <c r="H16" s="185"/>
+      <c r="H16" s="188"/>
     </row>
     <row r="17" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
@@ -28849,18 +28849,18 @@
     <row r="25" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="11"/>
-      <c r="C25" s="185" t="s">
+      <c r="C25" s="188" t="s">
         <v>696</v>
       </c>
-      <c r="D25" s="185"/>
-      <c r="E25" s="185" t="s">
+      <c r="D25" s="188"/>
+      <c r="E25" s="188" t="s">
         <v>697</v>
       </c>
-      <c r="F25" s="185"/>
-      <c r="G25" s="185" t="s">
+      <c r="F25" s="188"/>
+      <c r="G25" s="188" t="s">
         <v>698</v>
       </c>
-      <c r="H25" s="185"/>
+      <c r="H25" s="188"/>
     </row>
     <row r="26" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
@@ -29102,18 +29102,18 @@
     <row r="34" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3"/>
       <c r="B34" s="11"/>
-      <c r="C34" s="185" t="s">
+      <c r="C34" s="188" t="s">
         <v>696</v>
       </c>
-      <c r="D34" s="185"/>
-      <c r="E34" s="185" t="s">
+      <c r="D34" s="188"/>
+      <c r="E34" s="188" t="s">
         <v>697</v>
       </c>
-      <c r="F34" s="185"/>
-      <c r="G34" s="185" t="s">
+      <c r="F34" s="188"/>
+      <c r="G34" s="188" t="s">
         <v>698</v>
       </c>
-      <c r="H34" s="185"/>
+      <c r="H34" s="188"/>
     </row>
     <row r="35" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
@@ -29355,18 +29355,18 @@
     <row r="43" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3"/>
       <c r="B43" s="11"/>
-      <c r="C43" s="185" t="s">
+      <c r="C43" s="188" t="s">
         <v>696</v>
       </c>
-      <c r="D43" s="185"/>
-      <c r="E43" s="185" t="s">
+      <c r="D43" s="188"/>
+      <c r="E43" s="188" t="s">
         <v>697</v>
       </c>
-      <c r="F43" s="185"/>
-      <c r="G43" s="185" t="s">
+      <c r="F43" s="188"/>
+      <c r="G43" s="188" t="s">
         <v>698</v>
       </c>
-      <c r="H43" s="185"/>
+      <c r="H43" s="188"/>
     </row>
     <row r="44" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
@@ -29608,18 +29608,18 @@
     <row r="52" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="3"/>
       <c r="B52" s="11"/>
-      <c r="C52" s="185" t="s">
+      <c r="C52" s="188" t="s">
         <v>696</v>
       </c>
-      <c r="D52" s="185"/>
-      <c r="E52" s="185" t="s">
+      <c r="D52" s="188"/>
+      <c r="E52" s="188" t="s">
         <v>697</v>
       </c>
-      <c r="F52" s="185"/>
-      <c r="G52" s="185" t="s">
+      <c r="F52" s="188"/>
+      <c r="G52" s="188" t="s">
         <v>698</v>
       </c>
-      <c r="H52" s="185"/>
+      <c r="H52" s="188"/>
     </row>
     <row r="53" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
@@ -29860,6 +29860,26 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="J2:L3"/>
     <mergeCell ref="J5:J12"/>
@@ -29876,26 +29896,6 @@
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Updates right before pregrading!
</commit_message>
<xml_diff>
--- a/Rubric/GAM_Project_Rubric_EpisodePrototype.xlsx
+++ b/Rubric/GAM_Project_Rubric_EpisodePrototype.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Connor\Source\Repos\Game200-project\Rubric\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Connor\Source\Repos\game200-project\Rubric\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10200" tabRatio="500" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10200" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Game Data" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2304" uniqueCount="888">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2319" uniqueCount="896">
   <si>
     <t>GAME NAME</t>
   </si>
@@ -3326,6 +3326,30 @@
   </si>
   <si>
     <t>Game doesn't display any message that the player lost or one, it just dumps them to the main menu. Hopefully we can fix this before we turn it in.</t>
+  </si>
+  <si>
+    <t>GAM 200</t>
+  </si>
+  <si>
+    <t>RTIS</t>
+  </si>
+  <si>
+    <t>BSGD</t>
+  </si>
+  <si>
+    <t>Connor Hilarides</t>
+  </si>
+  <si>
+    <t>Claire (Jake) Robsahm</t>
+  </si>
+  <si>
+    <t>Leonardo Saikali</t>
+  </si>
+  <si>
+    <t>Enrique Rodriguez</t>
+  </si>
+  <si>
+    <t>Troy K. B. de Magro</t>
   </si>
 </sst>
 </file>
@@ -4324,87 +4348,6 @@
     <xf numFmtId="0" fontId="27" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4432,16 +4375,94 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4451,15 +4472,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4483,14 +4495,20 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -4505,6 +4523,42 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4533,36 +4587,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="22" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="22" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -14566,8 +14590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18:H18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -14585,47 +14609,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="145" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="146"/>
-      <c r="C1" s="146"/>
-      <c r="D1" s="147"/>
+      <c r="A1" s="118" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="120"/>
       <c r="E1" s="16"/>
-      <c r="F1" s="145" t="s">
+      <c r="F1" s="118" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="146"/>
-      <c r="H1" s="146"/>
-      <c r="I1" s="147"/>
+      <c r="G1" s="119"/>
+      <c r="H1" s="119"/>
+      <c r="I1" s="120"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
       <c r="L1" s="35"/>
     </row>
     <row r="2" spans="1:12" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="148"/>
-      <c r="B2" s="149"/>
-      <c r="C2" s="149"/>
-      <c r="D2" s="150"/>
+      <c r="A2" s="121"/>
+      <c r="B2" s="122"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="123"/>
       <c r="E2" s="16"/>
-      <c r="F2" s="148"/>
-      <c r="G2" s="149"/>
-      <c r="H2" s="149"/>
-      <c r="I2" s="150"/>
+      <c r="F2" s="121"/>
+      <c r="G2" s="122"/>
+      <c r="H2" s="122"/>
+      <c r="I2" s="123"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
       <c r="L2" s="35"/>
     </row>
     <row r="3" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="151"/>
-      <c r="B3" s="152"/>
-      <c r="C3" s="152"/>
-      <c r="D3" s="153"/>
+      <c r="A3" s="124"/>
+      <c r="B3" s="125"/>
+      <c r="C3" s="125"/>
+      <c r="D3" s="126"/>
       <c r="E3" s="16"/>
-      <c r="F3" s="151"/>
-      <c r="G3" s="152"/>
-      <c r="H3" s="152"/>
-      <c r="I3" s="153"/>
+      <c r="F3" s="124"/>
+      <c r="G3" s="125"/>
+      <c r="H3" s="125"/>
+      <c r="I3" s="126"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
       <c r="L3" s="35"/>
@@ -14645,35 +14669,35 @@
       <c r="L4" s="35"/>
     </row>
     <row r="5" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="145" t="s">
+      <c r="A5" s="118" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="146"/>
-      <c r="C5" s="146"/>
-      <c r="D5" s="147"/>
+      <c r="B5" s="119"/>
+      <c r="C5" s="119"/>
+      <c r="D5" s="120"/>
       <c r="E5" s="16"/>
-      <c r="F5" s="145" t="s">
+      <c r="F5" s="118" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="146"/>
-      <c r="H5" s="146"/>
-      <c r="I5" s="147"/>
+      <c r="G5" s="119"/>
+      <c r="H5" s="119"/>
+      <c r="I5" s="120"/>
       <c r="J5" s="6"/>
       <c r="K5" s="30"/>
       <c r="L5" s="35"/>
     </row>
     <row r="6" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="142"/>
-      <c r="B6" s="143"/>
-      <c r="C6" s="143"/>
-      <c r="D6" s="144"/>
+      <c r="A6" s="130"/>
+      <c r="B6" s="131"/>
+      <c r="C6" s="131"/>
+      <c r="D6" s="132"/>
       <c r="E6" s="16"/>
-      <c r="F6" s="142"/>
-      <c r="G6" s="143"/>
-      <c r="H6" s="143"/>
-      <c r="I6" s="144"/>
+      <c r="F6" s="130"/>
+      <c r="G6" s="131"/>
+      <c r="H6" s="131"/>
+      <c r="I6" s="132"/>
       <c r="J6" s="6"/>
-      <c r="K6" s="139" t="s">
+      <c r="K6" s="127" t="s">
         <v>29</v>
       </c>
       <c r="L6" s="35"/>
@@ -14684,42 +14708,42 @@
       <c r="C7" s="5"/>
       <c r="D7" s="37"/>
       <c r="E7" s="16"/>
-      <c r="F7" s="142"/>
-      <c r="G7" s="143"/>
-      <c r="H7" s="143"/>
-      <c r="I7" s="144"/>
+      <c r="F7" s="130"/>
+      <c r="G7" s="131"/>
+      <c r="H7" s="131"/>
+      <c r="I7" s="132"/>
       <c r="J7" s="6"/>
-      <c r="K7" s="140"/>
+      <c r="K7" s="128"/>
       <c r="L7" s="35"/>
     </row>
     <row r="8" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="145" t="s">
+      <c r="A8" s="118" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="146"/>
-      <c r="C8" s="146"/>
-      <c r="D8" s="147"/>
+      <c r="B8" s="119"/>
+      <c r="C8" s="119"/>
+      <c r="D8" s="120"/>
       <c r="E8" s="16"/>
-      <c r="F8" s="142"/>
-      <c r="G8" s="143"/>
-      <c r="H8" s="143"/>
-      <c r="I8" s="144"/>
+      <c r="F8" s="130"/>
+      <c r="G8" s="131"/>
+      <c r="H8" s="131"/>
+      <c r="I8" s="132"/>
       <c r="J8" s="6"/>
-      <c r="K8" s="140"/>
+      <c r="K8" s="128"/>
       <c r="L8" s="35"/>
     </row>
     <row r="9" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="142"/>
-      <c r="B9" s="143"/>
-      <c r="C9" s="143"/>
-      <c r="D9" s="144"/>
+      <c r="A9" s="130"/>
+      <c r="B9" s="131"/>
+      <c r="C9" s="131"/>
+      <c r="D9" s="132"/>
       <c r="E9" s="16"/>
-      <c r="F9" s="142"/>
-      <c r="G9" s="143"/>
-      <c r="H9" s="143"/>
-      <c r="I9" s="144"/>
+      <c r="F9" s="130"/>
+      <c r="G9" s="131"/>
+      <c r="H9" s="131"/>
+      <c r="I9" s="132"/>
       <c r="J9" s="6"/>
-      <c r="K9" s="141"/>
+      <c r="K9" s="129"/>
       <c r="L9" s="35"/>
     </row>
     <row r="10" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -14737,17 +14761,17 @@
       <c r="L10" s="35"/>
     </row>
     <row r="11" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="145" t="s">
+      <c r="A11" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="146"/>
-      <c r="C11" s="146"/>
-      <c r="D11" s="147"/>
+      <c r="B11" s="119"/>
+      <c r="C11" s="119"/>
+      <c r="D11" s="120"/>
       <c r="E11" s="16"/>
-      <c r="F11" s="145" t="s">
+      <c r="F11" s="118" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="147"/>
+      <c r="G11" s="120"/>
       <c r="H11" s="2" t="s">
         <v>7</v>
       </c>
@@ -14779,22 +14803,28 @@
       <c r="G12" s="6"/>
       <c r="H12" s="13">
         <f>SUMPRODUCT(($A$13:$A$30="GAM 200")*($D$13:$D$30=""))+SUMPRODUCT(($A$13:$A$30="GAM 205")*($D$13:$D$30=""))+SUMPRODUCT(($A$13:$A$30="GAM 250")*($D$13:$D$30=""))+SUMPRODUCT(($A$13:$A$30="GAM 255")*($D$13:$D$30=""))+SUMPRODUCT(($A$13:$A$30="GAM 300")*($D$13:$D$30=""))+SUMPRODUCT(($A$13:$A$30="GAM 302")*($D$13:$D$30=""))+SUMPRODUCT(($A$13:$A$30="GAM 350")*($D$13:$D$30=""))+SUMPRODUCT(($A$13:$A$30="GAM 352")*($D$13:$D$30=""))+SUMPRODUCT(($A$13:$A$30="GAM 400")*($D$13:$D$30=""))+SUMPRODUCT(($A$13:$A$30="GAM 450")*($D$13:$D$30=""))+SUMPRODUCT(($A$13:$A$30="GAM 541")*($D$13:$D$30=""))+SUMPRODUCT(($A$13:$A$30="GAM 550")*($D$13:$D$30=""))+SUMPRODUCT(($A$13:$A$30="GAM 551")*($D$13:$D$30=""))+SUMPRODUCT(($A$13:$A$30="PRJ 402")*($D$13:$D$30=""))+SUMPRODUCT(($A$13:$A$30="PRJ 452")*($D$13:$D$30=""))+SUMPRODUCT(($A$13:$A$30="GAM 200")*($D$13:$D$30="(full)"))+SUMPRODUCT(($A$13:$A$30="GAM 205")*($D$13:$D$30="(full)"))+SUMPRODUCT(($A$13:$A$30="GAM 250")*($D$13:$D$30="(full)"))+SUMPRODUCT(($A$13:$A$30="GAM 255")*($D$13:$D$30="(full)"))+SUMPRODUCT(($A$13:$A$30="GAM 300")*($D$13:$D$30="(full)"))+SUMPRODUCT(($A$13:$A$30="GAM 302")*($D$13:$D$30="(full)"))+SUMPRODUCT(($A$13:$A$30="GAM 350")*($D$13:$D$30="(full)"))+SUMPRODUCT(($A$13:$A$30="GAM 352")*($D$13:$D$30="(full)"))+SUMPRODUCT(($A$13:$A$30="GAM 400")*($D$13:$D$30="(full)"))+SUMPRODUCT(($A$13:$A$30="GAM 450")*($D$13:$D$30="(full)"))+SUMPRODUCT(($A$13:$A$30="GAM 541")*($D$13:$D$30="(full)"))+SUMPRODUCT(($A$13:$A$30="GAM 550")*($D$13:$D$30="(full)"))+SUMPRODUCT(($A$13:$A$30="GAM 551")*($D$13:$D$30="(full)"))+SUMPRODUCT(($A$13:$A$30="PRJ 402")*($D$13:$D$30="(full)"))+SUMPRODUCT(($A$13:$A$30="PRJ 452")*($D$13:$D$30="(full)"))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I12" s="43">
         <f>-H12*0.02</f>
-        <v>0</v>
+        <v>-0.1</v>
       </c>
       <c r="J12" s="6"/>
-      <c r="K12" s="139" t="s">
+      <c r="K12" s="127" t="s">
         <v>8</v>
       </c>
       <c r="L12" s="35"/>
     </row>
     <row r="13" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="44"/>
-      <c r="B13" s="44"/>
-      <c r="C13" s="45"/>
+      <c r="A13" s="44" t="s">
+        <v>888</v>
+      </c>
+      <c r="B13" s="44" t="s">
+        <v>889</v>
+      </c>
+      <c r="C13" s="45" t="s">
+        <v>891</v>
+      </c>
       <c r="D13" s="46"/>
       <c r="E13" s="6"/>
       <c r="F13" s="42" t="s">
@@ -14810,13 +14840,19 @@
         <v>0</v>
       </c>
       <c r="J13" s="47"/>
-      <c r="K13" s="140"/>
+      <c r="K13" s="128"/>
       <c r="L13" s="48"/>
     </row>
     <row r="14" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="44"/>
-      <c r="B14" s="44"/>
-      <c r="C14" s="45"/>
+      <c r="A14" s="44" t="s">
+        <v>888</v>
+      </c>
+      <c r="B14" s="44" t="s">
+        <v>890</v>
+      </c>
+      <c r="C14" s="45" t="s">
+        <v>892</v>
+      </c>
       <c r="D14" s="46"/>
       <c r="E14" s="6"/>
       <c r="F14" s="49" t="s">
@@ -14831,13 +14867,19 @@
         <v>0</v>
       </c>
       <c r="J14" s="12"/>
-      <c r="K14" s="141"/>
+      <c r="K14" s="129"/>
       <c r="L14" s="52"/>
     </row>
     <row r="15" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="44"/>
-      <c r="B15" s="44"/>
-      <c r="C15" s="45"/>
+      <c r="A15" s="44" t="s">
+        <v>888</v>
+      </c>
+      <c r="B15" s="44" t="s">
+        <v>890</v>
+      </c>
+      <c r="C15" s="45" t="s">
+        <v>893</v>
+      </c>
       <c r="D15" s="46"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
@@ -14847,16 +14889,22 @@
       </c>
       <c r="I15" s="53">
         <f>SUM(I11:I14)</f>
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="J15" s="12"/>
       <c r="K15" s="52"/>
       <c r="L15" s="52"/>
     </row>
     <row r="16" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="44"/>
-      <c r="B16" s="44"/>
-      <c r="C16" s="45"/>
+      <c r="A16" s="44" t="s">
+        <v>888</v>
+      </c>
+      <c r="B16" s="44" t="s">
+        <v>890</v>
+      </c>
+      <c r="C16" s="45" t="s">
+        <v>894</v>
+      </c>
       <c r="D16" s="46"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
@@ -14868,15 +14916,21 @@
       <c r="L16" s="52"/>
     </row>
     <row r="17" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="44"/>
-      <c r="B17" s="44"/>
-      <c r="C17" s="45"/>
+      <c r="A17" s="44" t="s">
+        <v>888</v>
+      </c>
+      <c r="B17" s="44" t="s">
+        <v>890</v>
+      </c>
+      <c r="C17" s="45" t="s">
+        <v>895</v>
+      </c>
       <c r="D17" s="46"/>
       <c r="E17" s="6"/>
-      <c r="F17" s="145" t="s">
+      <c r="F17" s="118" t="s">
         <v>17</v>
       </c>
-      <c r="G17" s="147"/>
+      <c r="G17" s="120"/>
       <c r="H17" s="2"/>
       <c r="I17" s="38">
         <v>0.75</v>
@@ -14894,16 +14948,16 @@
       <c r="F18" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="123" t="s">
+      <c r="G18" s="133" t="s">
         <v>20</v>
       </c>
-      <c r="H18" s="125"/>
+      <c r="H18" s="134"/>
       <c r="I18" s="43">
         <f>IF(LEFT(G18,6)="Entire",0,IF(LEFT(G18,6)="Custom",-0.05,-0.1))</f>
         <v>0</v>
       </c>
       <c r="J18" s="54"/>
-      <c r="K18" s="139" t="s">
+      <c r="K18" s="127" t="s">
         <v>18</v>
       </c>
       <c r="L18" s="35"/>
@@ -14917,16 +14971,16 @@
       <c r="F19" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="G19" s="129" t="s">
+      <c r="G19" s="135" t="s">
         <v>22</v>
       </c>
-      <c r="H19" s="131"/>
+      <c r="H19" s="136"/>
       <c r="I19" s="51">
         <f>IF(G19="2D Graphics and 2D Gameplay",IF(I11=0.15,-0.05,0),IF(G19="3D Graphics but 2D Gameplay",IF(I11=0.15,-0.02,-0.3),IF(I11=0.15,0,-0.3)))</f>
         <v>0</v>
       </c>
       <c r="J19" s="6"/>
-      <c r="K19" s="141"/>
+      <c r="K19" s="129"/>
       <c r="L19" s="35"/>
     </row>
     <row r="20" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -14954,7 +15008,7 @@
       <c r="C21" s="45"/>
       <c r="D21" s="46"/>
       <c r="E21" s="6"/>
-      <c r="F21" s="136" t="s">
+      <c r="F21" s="151" t="s">
         <v>23</v>
       </c>
       <c r="G21" s="55"/>
@@ -14970,17 +15024,17 @@
       <c r="C22" s="45"/>
       <c r="D22" s="46"/>
       <c r="E22" s="6"/>
-      <c r="F22" s="137"/>
+      <c r="F22" s="152"/>
       <c r="G22" s="55"/>
       <c r="H22" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="I22" s="118">
+      <c r="I22" s="137">
         <f>I20+I15</f>
-        <v>0.85</v>
+        <v>0.75</v>
       </c>
       <c r="J22" s="6"/>
-      <c r="K22" s="120" t="s">
+      <c r="K22" s="139" t="s">
         <v>26</v>
       </c>
       <c r="L22" s="35"/>
@@ -14991,14 +15045,14 @@
       <c r="C23" s="45"/>
       <c r="D23" s="46"/>
       <c r="E23" s="6"/>
-      <c r="F23" s="137"/>
+      <c r="F23" s="152"/>
       <c r="G23" s="55"/>
       <c r="H23" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="I23" s="119"/>
+      <c r="I23" s="138"/>
       <c r="J23" s="6"/>
-      <c r="K23" s="121"/>
+      <c r="K23" s="140"/>
       <c r="L23" s="35"/>
     </row>
     <row r="24" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -15007,7 +15061,7 @@
       <c r="C24" s="45"/>
       <c r="D24" s="46"/>
       <c r="E24" s="6"/>
-      <c r="F24" s="138"/>
+      <c r="F24" s="153"/>
       <c r="G24" s="55"/>
       <c r="H24" s="55"/>
       <c r="I24" s="55"/>
@@ -15035,12 +15089,12 @@
       <c r="C26" s="45"/>
       <c r="D26" s="46"/>
       <c r="E26" s="16"/>
-      <c r="F26" s="122" t="s">
+      <c r="F26" s="141" t="s">
         <v>27</v>
       </c>
-      <c r="G26" s="122"/>
-      <c r="H26" s="122"/>
-      <c r="I26" s="122"/>
+      <c r="G26" s="141"/>
+      <c r="H26" s="141"/>
+      <c r="I26" s="141"/>
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
       <c r="L26" s="35"/>
@@ -15051,12 +15105,12 @@
       <c r="C27" s="45"/>
       <c r="D27" s="46"/>
       <c r="E27" s="16"/>
-      <c r="F27" s="123" t="s">
+      <c r="F27" s="133" t="s">
         <v>28</v>
       </c>
-      <c r="G27" s="124"/>
-      <c r="H27" s="124"/>
-      <c r="I27" s="125"/>
+      <c r="G27" s="142"/>
+      <c r="H27" s="142"/>
+      <c r="I27" s="134"/>
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
       <c r="L27" s="35"/>
@@ -15067,10 +15121,10 @@
       <c r="C28" s="45"/>
       <c r="D28" s="46"/>
       <c r="E28" s="16"/>
-      <c r="F28" s="126"/>
-      <c r="G28" s="127"/>
-      <c r="H28" s="127"/>
-      <c r="I28" s="128"/>
+      <c r="F28" s="143"/>
+      <c r="G28" s="144"/>
+      <c r="H28" s="144"/>
+      <c r="I28" s="145"/>
       <c r="J28" s="6"/>
       <c r="K28" s="6"/>
       <c r="L28" s="35"/>
@@ -15081,10 +15135,10 @@
       <c r="C29" s="45"/>
       <c r="D29" s="46"/>
       <c r="E29" s="16"/>
-      <c r="F29" s="126"/>
-      <c r="G29" s="127"/>
-      <c r="H29" s="127"/>
-      <c r="I29" s="128"/>
+      <c r="F29" s="143"/>
+      <c r="G29" s="144"/>
+      <c r="H29" s="144"/>
+      <c r="I29" s="145"/>
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
       <c r="L29" s="35"/>
@@ -15095,26 +15149,26 @@
       <c r="C30" s="45"/>
       <c r="D30" s="46"/>
       <c r="E30" s="16"/>
-      <c r="F30" s="126"/>
-      <c r="G30" s="127"/>
-      <c r="H30" s="127"/>
-      <c r="I30" s="128"/>
+      <c r="F30" s="143"/>
+      <c r="G30" s="144"/>
+      <c r="H30" s="144"/>
+      <c r="I30" s="145"/>
       <c r="J30" s="6"/>
       <c r="K30" s="6"/>
       <c r="L30" s="35"/>
     </row>
     <row r="31" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="132" t="s">
+      <c r="A31" s="147" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="133"/>
-      <c r="C31" s="134"/>
-      <c r="D31" s="135"/>
+      <c r="B31" s="148"/>
+      <c r="C31" s="149"/>
+      <c r="D31" s="150"/>
       <c r="E31" s="6"/>
-      <c r="F31" s="129"/>
-      <c r="G31" s="130"/>
-      <c r="H31" s="130"/>
-      <c r="I31" s="131"/>
+      <c r="F31" s="135"/>
+      <c r="G31" s="146"/>
+      <c r="H31" s="146"/>
+      <c r="I31" s="136"/>
       <c r="J31" s="6"/>
       <c r="K31" s="6"/>
       <c r="L31" s="35"/>
@@ -15135,12 +15189,13 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="A2:D3"/>
-    <mergeCell ref="F2:I3"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="F27:I31"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="F21:F24"/>
     <mergeCell ref="K12:K14"/>
     <mergeCell ref="K18:K19"/>
     <mergeCell ref="A6:D6"/>
@@ -15156,13 +15211,12 @@
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="G19:H19"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="F27:I31"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="F21:F24"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="A2:D3"/>
+    <mergeCell ref="F2:I3"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="F5:I5"/>
   </mergeCells>
   <dataValidations count="9">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A6:D6">
@@ -15219,65 +15273,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="179" t="s">
+      <c r="A1" s="189" t="s">
         <v>706</v>
       </c>
       <c r="B1" s="75"/>
-      <c r="C1" s="194" t="s">
+      <c r="C1" s="179" t="s">
         <v>689</v>
       </c>
-      <c r="D1" s="195"/>
-      <c r="E1" s="194" t="s">
+      <c r="D1" s="180"/>
+      <c r="E1" s="179" t="s">
         <v>690</v>
       </c>
-      <c r="F1" s="195"/>
-      <c r="G1" s="194" t="s">
+      <c r="F1" s="180"/>
+      <c r="G1" s="179" t="s">
         <v>691</v>
       </c>
-      <c r="H1" s="195"/>
+      <c r="H1" s="180"/>
     </row>
     <row r="2" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="180"/>
+      <c r="A2" s="190"/>
       <c r="B2" s="75"/>
-      <c r="C2" s="196" t="s">
+      <c r="C2" s="181" t="s">
         <v>688</v>
       </c>
-      <c r="D2" s="197"/>
-      <c r="E2" s="196" t="s">
+      <c r="D2" s="182"/>
+      <c r="E2" s="181" t="s">
         <v>688</v>
       </c>
-      <c r="F2" s="197"/>
-      <c r="G2" s="196" t="s">
+      <c r="F2" s="182"/>
+      <c r="G2" s="181" t="s">
         <v>688</v>
       </c>
-      <c r="H2" s="197"/>
-      <c r="J2" s="182" t="s">
+      <c r="H2" s="182"/>
+      <c r="J2" s="192" t="s">
         <v>707</v>
       </c>
-      <c r="K2" s="183"/>
-      <c r="L2" s="184"/>
+      <c r="K2" s="193"/>
+      <c r="L2" s="194"/>
     </row>
     <row r="3" spans="1:12" ht="22.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="181"/>
+      <c r="A3" s="191"/>
       <c r="B3" s="76"/>
-      <c r="C3" s="192">
+      <c r="C3" s="183">
         <f>MAX(0,MIN(1,IF((A6+C6+L6) &lt;= 0.95, ROUND(A6+C6+L6,2), FLOOR((0.95+(A6+C6+L6-0.95)/5),2))))</f>
-        <v>0.85</v>
-      </c>
-      <c r="D3" s="193"/>
-      <c r="E3" s="192">
+        <v>0.75</v>
+      </c>
+      <c r="D3" s="184"/>
+      <c r="E3" s="183">
         <f>MAX(0,MIN(1,IF((A6+E6+L6) &lt;= 0.95, ROUND(A6+E6+L6,2), FLOOR((0.95+(A6+E6+L6-0.95)/5),2))))</f>
-        <v>0.85</v>
-      </c>
-      <c r="F3" s="193"/>
-      <c r="G3" s="192">
+        <v>0.75</v>
+      </c>
+      <c r="F3" s="184"/>
+      <c r="G3" s="183">
         <f>MAX(0,MIN(1,IF((A6+G6+L6) &lt;= 0.95, ROUND(A6+G6+L6,2), FLOOR((0.95+(A6+G6+L6-0.95)/5),2))))</f>
-        <v>0.85</v>
-      </c>
-      <c r="H3" s="193"/>
-      <c r="J3" s="185"/>
-      <c r="K3" s="186"/>
-      <c r="L3" s="187"/>
+        <v>0.75</v>
+      </c>
+      <c r="H3" s="184"/>
+      <c r="J3" s="195"/>
+      <c r="K3" s="196"/>
+      <c r="L3" s="197"/>
     </row>
     <row r="4" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
@@ -15297,18 +15351,18 @@
         <v>692</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="145" t="s">
+      <c r="C5" s="118" t="s">
         <v>693</v>
       </c>
-      <c r="D5" s="147"/>
-      <c r="E5" s="145" t="s">
+      <c r="D5" s="120"/>
+      <c r="E5" s="118" t="s">
         <v>694</v>
       </c>
-      <c r="F5" s="147"/>
-      <c r="G5" s="145" t="s">
+      <c r="F5" s="120"/>
+      <c r="G5" s="118" t="s">
         <v>695</v>
       </c>
-      <c r="H5" s="147"/>
+      <c r="H5" s="120"/>
       <c r="J5" s="77" t="s">
         <v>708</v>
       </c>
@@ -15320,27 +15374,27 @@
     <row r="6" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="78">
         <f>'Game Data'!$I$22+Submission!$E$16</f>
-        <v>0.85</v>
+        <v>0.75</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="189">
+      <c r="C6" s="186">
         <f>D15+D24+D33+D42+D51+D60</f>
         <v>0</v>
       </c>
-      <c r="D6" s="190"/>
-      <c r="E6" s="189">
+      <c r="D6" s="187"/>
+      <c r="E6" s="186">
         <f>F15+F24+F33+F42+F51+F60</f>
         <v>0</v>
       </c>
-      <c r="F6" s="190"/>
-      <c r="G6" s="189">
+      <c r="F6" s="187"/>
+      <c r="G6" s="186">
         <f>H15+H24+H33+H42+H51+H60</f>
         <v>0</v>
       </c>
-      <c r="H6" s="190"/>
+      <c r="H6" s="187"/>
       <c r="J6" s="92">
         <f>ABS('Student Grade'!$F$15+'Student Grade'!$D$24+'Student Grade'!$H$33+'Student Grade'!$F$42+'Student Grade'!$F$51+'Student Grade'!$F$60-$F$15-$D$24-$D$33-$H$42-$F$51-$F$60)</f>
-        <v>0.62250000000000005</v>
+        <v>0.49750000000000005</v>
       </c>
       <c r="K6" s="3"/>
       <c r="L6" s="90">
@@ -15351,18 +15405,18 @@
     <row r="7" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="11"/>
-      <c r="C7" s="191" t="s">
+      <c r="C7" s="188" t="s">
         <v>696</v>
       </c>
-      <c r="D7" s="191"/>
-      <c r="E7" s="191" t="s">
+      <c r="D7" s="188"/>
+      <c r="E7" s="188" t="s">
         <v>697</v>
       </c>
-      <c r="F7" s="191"/>
-      <c r="G7" s="191" t="s">
+      <c r="F7" s="188"/>
+      <c r="G7" s="188" t="s">
         <v>698</v>
       </c>
-      <c r="H7" s="191"/>
+      <c r="H7" s="188"/>
       <c r="J7" s="91"/>
       <c r="K7" s="3"/>
       <c r="L7" s="89"/>
@@ -15536,7 +15590,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J12" s="139" t="s">
+      <c r="J12" s="127" t="s">
         <v>721</v>
       </c>
       <c r="K12" s="31"/>
@@ -15574,7 +15628,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J13" s="140"/>
+      <c r="J13" s="128"/>
       <c r="K13" s="31"/>
       <c r="L13" s="104" t="s">
         <v>714</v>
@@ -15610,7 +15664,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J14" s="140"/>
+      <c r="J14" s="128"/>
       <c r="K14" s="105"/>
       <c r="L14" s="104" t="s">
         <v>715</v>
@@ -15640,7 +15694,7 @@
         <f>SUM(H9:H14)</f>
         <v>0</v>
       </c>
-      <c r="J15" s="140"/>
+      <c r="J15" s="128"/>
       <c r="K15" s="105"/>
       <c r="L15" s="104" t="s">
         <v>716</v>
@@ -15649,19 +15703,19 @@
     <row r="16" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="11"/>
-      <c r="C16" s="188" t="s">
+      <c r="C16" s="185" t="s">
         <v>696</v>
       </c>
-      <c r="D16" s="188"/>
-      <c r="E16" s="188" t="s">
+      <c r="D16" s="185"/>
+      <c r="E16" s="185" t="s">
         <v>697</v>
       </c>
-      <c r="F16" s="188"/>
-      <c r="G16" s="188" t="s">
+      <c r="F16" s="185"/>
+      <c r="G16" s="185" t="s">
         <v>698</v>
       </c>
-      <c r="H16" s="188"/>
-      <c r="J16" s="140"/>
+      <c r="H16" s="185"/>
+      <c r="J16" s="128"/>
       <c r="K16" s="105"/>
       <c r="L16" s="104" t="s">
         <v>717</v>
@@ -15692,7 +15746,7 @@
       <c r="H17" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="J17" s="140"/>
+      <c r="J17" s="128"/>
       <c r="K17" s="105"/>
       <c r="L17" s="104" t="s">
         <v>718</v>
@@ -15728,7 +15782,7 @@
         <f t="shared" ref="H18:H23" si="5">B18*G18</f>
         <v>0</v>
       </c>
-      <c r="J18" s="140"/>
+      <c r="J18" s="128"/>
       <c r="K18" s="105"/>
       <c r="L18" s="104" t="s">
         <v>719</v>
@@ -15764,7 +15818,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J19" s="141"/>
+      <c r="J19" s="129"/>
       <c r="K19" s="105"/>
       <c r="L19" s="103" t="s">
         <v>720</v>
@@ -15922,18 +15976,18 @@
     <row r="25" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="11"/>
-      <c r="C25" s="188" t="s">
+      <c r="C25" s="185" t="s">
         <v>696</v>
       </c>
-      <c r="D25" s="188"/>
-      <c r="E25" s="188" t="s">
+      <c r="D25" s="185"/>
+      <c r="E25" s="185" t="s">
         <v>697</v>
       </c>
-      <c r="F25" s="188"/>
-      <c r="G25" s="188" t="s">
+      <c r="F25" s="185"/>
+      <c r="G25" s="185" t="s">
         <v>698</v>
       </c>
-      <c r="H25" s="188"/>
+      <c r="H25" s="185"/>
     </row>
     <row r="26" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
@@ -16175,18 +16229,18 @@
     <row r="34" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3"/>
       <c r="B34" s="11"/>
-      <c r="C34" s="188" t="s">
+      <c r="C34" s="185" t="s">
         <v>696</v>
       </c>
-      <c r="D34" s="188"/>
-      <c r="E34" s="188" t="s">
+      <c r="D34" s="185"/>
+      <c r="E34" s="185" t="s">
         <v>697</v>
       </c>
-      <c r="F34" s="188"/>
-      <c r="G34" s="188" t="s">
+      <c r="F34" s="185"/>
+      <c r="G34" s="185" t="s">
         <v>698</v>
       </c>
-      <c r="H34" s="188"/>
+      <c r="H34" s="185"/>
     </row>
     <row r="35" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
@@ -16428,18 +16482,18 @@
     <row r="43" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3"/>
       <c r="B43" s="11"/>
-      <c r="C43" s="188" t="s">
+      <c r="C43" s="185" t="s">
         <v>696</v>
       </c>
-      <c r="D43" s="188"/>
-      <c r="E43" s="188" t="s">
+      <c r="D43" s="185"/>
+      <c r="E43" s="185" t="s">
         <v>697</v>
       </c>
-      <c r="F43" s="188"/>
-      <c r="G43" s="188" t="s">
+      <c r="F43" s="185"/>
+      <c r="G43" s="185" t="s">
         <v>698</v>
       </c>
-      <c r="H43" s="188"/>
+      <c r="H43" s="185"/>
     </row>
     <row r="44" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
@@ -16681,18 +16735,18 @@
     <row r="52" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="3"/>
       <c r="B52" s="11"/>
-      <c r="C52" s="188" t="s">
+      <c r="C52" s="185" t="s">
         <v>696</v>
       </c>
-      <c r="D52" s="188"/>
-      <c r="E52" s="188" t="s">
+      <c r="D52" s="185"/>
+      <c r="E52" s="185" t="s">
         <v>697</v>
       </c>
-      <c r="F52" s="188"/>
-      <c r="G52" s="188" t="s">
+      <c r="F52" s="185"/>
+      <c r="G52" s="185" t="s">
         <v>698</v>
       </c>
-      <c r="H52" s="188"/>
+      <c r="H52" s="185"/>
     </row>
     <row r="53" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
@@ -16933,27 +16987,6 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
     <mergeCell ref="C52:D52"/>
     <mergeCell ref="E52:F52"/>
     <mergeCell ref="G52:H52"/>
@@ -16970,6 +17003,27 @@
     <mergeCell ref="E43:F43"/>
     <mergeCell ref="G43:H43"/>
     <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -16996,54 +17050,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="158" t="s">
+      <c r="A1" s="157" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="159"/>
-      <c r="C1" s="159"/>
-      <c r="D1" s="159"/>
-      <c r="E1" s="159"/>
-      <c r="F1" s="160"/>
+      <c r="B1" s="158"/>
+      <c r="C1" s="158"/>
+      <c r="D1" s="158"/>
+      <c r="E1" s="158"/>
+      <c r="F1" s="159"/>
     </row>
     <row r="2" spans="1:6" ht="43.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="161" t="s">
+      <c r="A2" s="154" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="162"/>
-      <c r="C2" s="162"/>
-      <c r="D2" s="162"/>
-      <c r="E2" s="162"/>
-      <c r="F2" s="163"/>
+      <c r="B2" s="155"/>
+      <c r="C2" s="155"/>
+      <c r="D2" s="155"/>
+      <c r="E2" s="155"/>
+      <c r="F2" s="156"/>
     </row>
     <row r="3" spans="1:6" ht="43.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="164" t="s">
+      <c r="A3" s="160" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="165"/>
-      <c r="C3" s="165"/>
-      <c r="D3" s="165"/>
-      <c r="E3" s="165"/>
-      <c r="F3" s="166"/>
+      <c r="B3" s="161"/>
+      <c r="C3" s="161"/>
+      <c r="D3" s="161"/>
+      <c r="E3" s="161"/>
+      <c r="F3" s="162"/>
     </row>
     <row r="4" spans="1:6" ht="28.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="161" t="s">
+      <c r="A4" s="154" t="s">
         <v>725</v>
       </c>
-      <c r="B4" s="162"/>
-      <c r="C4" s="162"/>
-      <c r="D4" s="162"/>
-      <c r="E4" s="162"/>
-      <c r="F4" s="163"/>
+      <c r="B4" s="155"/>
+      <c r="C4" s="155"/>
+      <c r="D4" s="155"/>
+      <c r="E4" s="155"/>
+      <c r="F4" s="156"/>
     </row>
     <row r="5" spans="1:6" ht="28.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="167" t="s">
+      <c r="A5" s="163" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="168"/>
-      <c r="C5" s="168"/>
-      <c r="D5" s="168"/>
-      <c r="E5" s="168"/>
-      <c r="F5" s="169"/>
+      <c r="B5" s="164"/>
+      <c r="C5" s="164"/>
+      <c r="D5" s="164"/>
+      <c r="E5" s="164"/>
+      <c r="F5" s="165"/>
     </row>
     <row r="6" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6"/>
@@ -17072,10 +17126,10 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="164" t="s">
+      <c r="A8" s="160" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="165"/>
+      <c r="B8" s="161"/>
       <c r="C8" s="17">
         <v>0</v>
       </c>
@@ -17091,10 +17145,10 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="154" t="s">
+      <c r="A9" s="167" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="155"/>
+      <c r="B9" s="168"/>
       <c r="C9" s="12">
         <v>0</v>
       </c>
@@ -17110,10 +17164,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="171" t="s">
+      <c r="A10" s="169" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="171"/>
+      <c r="B10" s="169"/>
       <c r="C10" s="12">
         <v>0</v>
       </c>
@@ -17129,10 +17183,10 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="171" t="s">
+      <c r="A11" s="169" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="171"/>
+      <c r="B11" s="169"/>
       <c r="C11" s="12">
         <v>0</v>
       </c>
@@ -17148,10 +17202,10 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="171" t="s">
+      <c r="A12" s="169" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="171"/>
+      <c r="B12" s="169"/>
       <c r="C12" s="12">
         <v>0</v>
       </c>
@@ -17167,10 +17221,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="154" t="s">
+      <c r="A13" s="167" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="155"/>
+      <c r="B13" s="168"/>
       <c r="C13" s="12">
         <v>0</v>
       </c>
@@ -17186,10 +17240,10 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="154" t="s">
+      <c r="A14" s="167" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="155"/>
+      <c r="B14" s="168"/>
       <c r="C14" s="12">
         <v>0</v>
       </c>
@@ -17205,10 +17259,10 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="156" t="s">
+      <c r="A15" s="170" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="157"/>
+      <c r="B15" s="171"/>
       <c r="C15" s="19">
         <v>0</v>
       </c>
@@ -17225,11 +17279,11 @@
     </row>
     <row r="16" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
-      <c r="B16" s="170" t="s">
+      <c r="B16" s="166" t="s">
         <v>50</v>
       </c>
-      <c r="C16" s="170"/>
-      <c r="D16" s="170"/>
+      <c r="C16" s="166"/>
+      <c r="D16" s="166"/>
       <c r="E16" s="108">
         <f>SUM(E8:E15)</f>
         <v>0</v>
@@ -17248,88 +17302,93 @@
       <c r="A18" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="158" t="s">
+      <c r="B18" s="157" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="159"/>
-      <c r="D18" s="159"/>
-      <c r="E18" s="159"/>
-      <c r="F18" s="160"/>
+      <c r="C18" s="158"/>
+      <c r="D18" s="158"/>
+      <c r="E18" s="158"/>
+      <c r="F18" s="159"/>
     </row>
     <row r="19" spans="1:6" ht="28.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="64" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="161" t="s">
+      <c r="B19" s="154" t="s">
         <v>69</v>
       </c>
-      <c r="C19" s="162"/>
-      <c r="D19" s="162"/>
-      <c r="E19" s="162"/>
-      <c r="F19" s="163"/>
+      <c r="C19" s="155"/>
+      <c r="D19" s="155"/>
+      <c r="E19" s="155"/>
+      <c r="F19" s="156"/>
     </row>
     <row r="20" spans="1:6" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="64" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="161" t="s">
+      <c r="B20" s="154" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="162"/>
-      <c r="D20" s="162"/>
-      <c r="E20" s="162"/>
-      <c r="F20" s="163"/>
+      <c r="C20" s="155"/>
+      <c r="D20" s="155"/>
+      <c r="E20" s="155"/>
+      <c r="F20" s="156"/>
     </row>
     <row r="21" spans="1:6" ht="28.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="161" t="s">
+      <c r="B21" s="154" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="162"/>
-      <c r="D21" s="162"/>
-      <c r="E21" s="162"/>
-      <c r="F21" s="163"/>
+      <c r="C21" s="155"/>
+      <c r="D21" s="155"/>
+      <c r="E21" s="155"/>
+      <c r="F21" s="156"/>
     </row>
     <row r="22" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="64" t="s">
         <v>60</v>
       </c>
-      <c r="B22" s="161" t="s">
+      <c r="B22" s="154" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="162"/>
-      <c r="D22" s="162"/>
-      <c r="E22" s="162"/>
-      <c r="F22" s="163"/>
+      <c r="C22" s="155"/>
+      <c r="D22" s="155"/>
+      <c r="E22" s="155"/>
+      <c r="F22" s="156"/>
     </row>
     <row r="23" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="161" t="s">
+      <c r="B23" s="154" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="162"/>
-      <c r="D23" s="162"/>
-      <c r="E23" s="162"/>
-      <c r="F23" s="163"/>
+      <c r="C23" s="155"/>
+      <c r="D23" s="155"/>
+      <c r="E23" s="155"/>
+      <c r="F23" s="156"/>
     </row>
     <row r="24" spans="1:6" ht="43.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="64" t="s">
         <v>56</v>
       </c>
-      <c r="B24" s="161" t="s">
+      <c r="B24" s="154" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="162"/>
-      <c r="D24" s="162"/>
-      <c r="E24" s="162"/>
-      <c r="F24" s="163"/>
+      <c r="C24" s="155"/>
+      <c r="D24" s="155"/>
+      <c r="E24" s="155"/>
+      <c r="F24" s="156"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B19:F19"/>
     <mergeCell ref="B24:F24"/>
     <mergeCell ref="B20:F20"/>
     <mergeCell ref="A1:F1"/>
@@ -17346,11 +17405,6 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B19:F19"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -17361,8 +17415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+    <sheetView topLeftCell="A64" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -17404,7 +17458,7 @@
       <c r="B2" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="174" t="s">
+      <c r="C2" s="172" t="s">
         <v>881</v>
       </c>
       <c r="D2" s="66">
@@ -17427,10 +17481,10 @@
       <c r="B3" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="175"/>
+      <c r="C3" s="173"/>
       <c r="D3" s="66">
         <f>SUMPRODUCT(($A$10:$A$250="Basic")*(D$10:D$250="Missing"))+0.5*SUMPRODUCT(($A$10:$A$250="Basic")*(D$10:D$250="Partial"))</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E3" s="66">
         <f>SUMPRODUCT(($A$10:$A$250="Basic")*(E$10:E$250="Missing"))+0.5*SUMPRODUCT(($A$10:$A$250="Basic")*(E$10:E$250="Partial"))</f>
@@ -17448,10 +17502,10 @@
       <c r="B4" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="175"/>
+      <c r="C4" s="173"/>
       <c r="D4" s="66">
         <f>SUMPRODUCT(($A$10:$A$250="Intermediate")*(D$10:D$250="Missing"))+0.5*SUMPRODUCT(($A$10:$A$250="Intermediate")*(D$10:D$250="Partial"))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" s="66">
         <f>SUMPRODUCT(($A$10:$A$250="Intermediate")*(E$10:E$250="Missing"))+0.5*SUMPRODUCT(($A$10:$A$250="Intermediate")*(E$10:E$250="Partial"))</f>
@@ -17469,10 +17523,10 @@
       <c r="B5" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="175"/>
+      <c r="C5" s="173"/>
       <c r="D5" s="66">
         <f>SUMPRODUCT(($A$10:$A$250="Intermediate")*(D$10:D$250="Completed"))+SUMPRODUCT(($A$10:$A$250="Intermediate")*(D$10:D$250="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$250="Intermediate")*(D$10:D$250="Partial"))</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E5" s="66">
         <f>SUMPRODUCT(($A$10:$A$250="Intermediate")*(E$10:E$250="Completed"))+SUMPRODUCT(($A$10:$A$250="Intermediate")*(E$10:E$250="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$250="Intermediate")*(E$10:E$250="Partial"))</f>
@@ -17490,7 +17544,7 @@
       <c r="B6" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="175"/>
+      <c r="C6" s="173"/>
       <c r="D6" s="66">
         <f>SUMPRODUCT(($A$10:$A$250="Advanced")*(D$10:D$250="Missing"))+0.5*SUMPRODUCT(($A$10:$A$250="Advanced")*(D$10:D$250="Partial"))</f>
         <v>2.5</v>
@@ -17511,7 +17565,7 @@
       <c r="B7" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="175"/>
+      <c r="C7" s="173"/>
       <c r="D7" s="66">
         <f>SUMPRODUCT(($A$10:$A$250="Advanced")*(D$10:D$250="Completed"))+SUMPRODUCT(($A$10:$A$250="Advanced")*(D$10:D$250="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$250="Advanced")*(D$10:D$250="Partial"))</f>
         <v>3.5</v>
@@ -17532,7 +17586,7 @@
       <c r="B8" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="175"/>
+      <c r="C8" s="173"/>
       <c r="D8" s="66">
         <f>SUMPRODUCT(($A$10:$A$250="Professional")*(D$10:D$250="Completed"))+SUMPRODUCT(($A$10:$A$250="Professional")*(D$10:D$250="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$250="Professional")*(D$10:D$250="Partial"))</f>
         <v>0</v>
@@ -17547,11 +17601,11 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="177" t="s">
+      <c r="A9" s="175" t="s">
         <v>88</v>
       </c>
-      <c r="B9" s="178"/>
-      <c r="C9" s="176"/>
+      <c r="B9" s="176"/>
+      <c r="C9" s="174"/>
       <c r="D9" s="66">
         <f>SUMPRODUCT(($A$10:$A$250="Innovative")*(D$10:D$250="Completed"))+SUMPRODUCT(($A$10:$A$250="Innovative")*(D$10:D$250="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$250="Innovative")*(D$10:D$250="Partial"))</f>
         <v>0</v>
@@ -17566,10 +17620,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="172" t="s">
+      <c r="A10" s="177" t="s">
         <v>724</v>
       </c>
-      <c r="B10" s="173"/>
+      <c r="B10" s="178"/>
       <c r="C10" s="8" t="s">
         <v>868</v>
       </c>
@@ -17692,10 +17746,10 @@
       <c r="F16" s="60"/>
     </row>
     <row r="17" spans="1:6" ht="28.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="172" t="s">
+      <c r="A17" s="177" t="s">
         <v>739</v>
       </c>
-      <c r="B17" s="173"/>
+      <c r="B17" s="178"/>
       <c r="C17" s="8" t="s">
         <v>870</v>
       </c>
@@ -17848,7 +17902,7 @@
         <v>733</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>74</v>
@@ -17884,7 +17938,7 @@
         <v>112</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>74</v>
@@ -17910,10 +17964,10 @@
       <c r="F28" s="60"/>
     </row>
     <row r="29" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="172" t="s">
+      <c r="A29" s="177" t="s">
         <v>740</v>
       </c>
-      <c r="B29" s="173"/>
+      <c r="B29" s="178"/>
       <c r="C29" s="8" t="s">
         <v>871</v>
       </c>
@@ -18396,10 +18450,10 @@
       <c r="F55" s="60"/>
     </row>
     <row r="56" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="172" t="s">
+      <c r="A56" s="177" t="s">
         <v>114</v>
       </c>
-      <c r="B56" s="173"/>
+      <c r="B56" s="178"/>
       <c r="C56" s="8" t="s">
         <v>89</v>
       </c>
@@ -18514,7 +18568,7 @@
         <v>878</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E62" s="8" t="s">
         <v>74</v>
@@ -18632,10 +18686,10 @@
       <c r="F68" s="60"/>
     </row>
     <row r="69" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="172" t="s">
+      <c r="A69" s="177" t="s">
         <v>135</v>
       </c>
-      <c r="B69" s="173"/>
+      <c r="B69" s="178"/>
       <c r="C69" s="8" t="s">
         <v>89</v>
       </c>
@@ -18796,10 +18850,10 @@
       <c r="F77" s="60"/>
     </row>
     <row r="78" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="172" t="s">
+      <c r="A78" s="177" t="s">
         <v>152</v>
       </c>
-      <c r="B78" s="173"/>
+      <c r="B78" s="178"/>
       <c r="C78" s="8" t="s">
         <v>89</v>
       </c>
@@ -18904,10 +18958,10 @@
       <c r="F83" s="60"/>
     </row>
     <row r="84" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="172" t="s">
+      <c r="A84" s="177" t="s">
         <v>163</v>
       </c>
-      <c r="B84" s="173"/>
+      <c r="B84" s="178"/>
       <c r="C84" s="8" t="s">
         <v>89</v>
       </c>
@@ -19138,10 +19192,10 @@
       <c r="F96" s="60"/>
     </row>
     <row r="97" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A97" s="172" t="s">
+      <c r="A97" s="177" t="s">
         <v>187</v>
       </c>
-      <c r="B97" s="173"/>
+      <c r="B97" s="178"/>
       <c r="C97" s="8" t="s">
         <v>89</v>
       </c>
@@ -19228,10 +19282,10 @@
       <c r="F101" s="60"/>
     </row>
     <row r="102" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A102" s="172" t="s">
+      <c r="A102" s="177" t="s">
         <v>194</v>
       </c>
-      <c r="B102" s="173"/>
+      <c r="B102" s="178"/>
       <c r="C102" s="8" t="s">
         <v>89</v>
       </c>
@@ -19374,10 +19428,10 @@
       <c r="F109" s="60"/>
     </row>
     <row r="110" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A110" s="172" t="s">
+      <c r="A110" s="177" t="s">
         <v>205</v>
       </c>
-      <c r="B110" s="173"/>
+      <c r="B110" s="178"/>
       <c r="C110" s="8" t="s">
         <v>89</v>
       </c>
@@ -19446,10 +19500,10 @@
       <c r="F113" s="60"/>
     </row>
     <row r="114" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A114" s="172" t="s">
+      <c r="A114" s="177" t="s">
         <v>212</v>
       </c>
-      <c r="B114" s="173"/>
+      <c r="B114" s="178"/>
       <c r="C114" s="8" t="s">
         <v>89</v>
       </c>
@@ -19518,10 +19572,10 @@
       <c r="F117" s="60"/>
     </row>
     <row r="118" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A118" s="172" t="s">
+      <c r="A118" s="177" t="s">
         <v>219</v>
       </c>
-      <c r="B118" s="173"/>
+      <c r="B118" s="178"/>
       <c r="C118" s="8" t="s">
         <v>823</v>
       </c>
@@ -19681,11 +19735,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C2:C9"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A56:B56"/>
     <mergeCell ref="A110:B110"/>
     <mergeCell ref="A114:B114"/>
     <mergeCell ref="A118:B118"/>
@@ -19695,6 +19744,11 @@
     <mergeCell ref="A84:B84"/>
     <mergeCell ref="A97:B97"/>
     <mergeCell ref="A102:B102"/>
+    <mergeCell ref="C2:C9"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A56:B56"/>
   </mergeCells>
   <conditionalFormatting sqref="A10 A33:A37 A39:A41 A109:A251 A95:A107 A56:A92 A14:A31">
     <cfRule type="beginsWith" dxfId="740" priority="292" stopIfTrue="1" operator="beginsWith" text="Innovative">
@@ -20678,7 +20732,7 @@
       <c r="B2" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="174" t="s">
+      <c r="C2" s="172" t="s">
         <v>862</v>
       </c>
       <c r="D2" s="66">
@@ -20701,7 +20755,7 @@
       <c r="B3" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="175"/>
+      <c r="C3" s="173"/>
       <c r="D3" s="66">
         <f>SUMPRODUCT(($A$10:$A$241="Basic")*(D$10:D$241="Missing"))+0.5*SUMPRODUCT(($A$10:$A$241="Basic")*(D$10:D$241="Partial"))</f>
         <v>10</v>
@@ -20722,7 +20776,7 @@
       <c r="B4" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="175"/>
+      <c r="C4" s="173"/>
       <c r="D4" s="66">
         <f>SUMPRODUCT(($A$10:$A$241="Intermediate")*(D$10:D$241="Missing"))+0.5*SUMPRODUCT(($A$10:$A$241="Intermediate")*(D$10:D$241="Partial"))</f>
         <v>10</v>
@@ -20743,7 +20797,7 @@
       <c r="B5" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="175"/>
+      <c r="C5" s="173"/>
       <c r="D5" s="66">
         <f>SUMPRODUCT(($A$10:$A$241="Intermediate")*(D$10:D$241="Completed"))+SUMPRODUCT(($A$10:$A$241="Intermediate")*(D$10:D$241="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$241="Intermediate")*(D$10:D$241="Partial"))</f>
         <v>0</v>
@@ -20764,7 +20818,7 @@
       <c r="B6" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="175"/>
+      <c r="C6" s="173"/>
       <c r="D6" s="66">
         <f>SUMPRODUCT(($A$10:$A$241="Advanced")*(D$10:D$241="Missing"))+0.5*SUMPRODUCT(($A$10:$A$241="Advanced")*(D$10:D$241="Partial"))</f>
         <v>2</v>
@@ -20785,7 +20839,7 @@
       <c r="B7" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="175"/>
+      <c r="C7" s="173"/>
       <c r="D7" s="66">
         <f>SUMPRODUCT(($A$10:$A$241="Advanced")*(D$10:D$241="Completed"))+SUMPRODUCT(($A$10:$A$241="Advanced")*(D$10:D$241="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$241="Advanced")*(D$10:D$241="Partial"))</f>
         <v>1</v>
@@ -20806,7 +20860,7 @@
       <c r="B8" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="175"/>
+      <c r="C8" s="173"/>
       <c r="D8" s="66">
         <f>SUMPRODUCT(($A$10:$A$241="Professional")*(D$10:D$241="Completed"))+SUMPRODUCT(($A$10:$A$241="Professional")*(D$10:D$241="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$241="Professional")*(D$10:D$241="Partial"))</f>
         <v>0</v>
@@ -20821,11 +20875,11 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="177" t="s">
+      <c r="A9" s="175" t="s">
         <v>88</v>
       </c>
-      <c r="B9" s="178"/>
-      <c r="C9" s="176"/>
+      <c r="B9" s="176"/>
+      <c r="C9" s="174"/>
       <c r="D9" s="66">
         <f>SUMPRODUCT(($A$10:$A$241="Innovative")*(D$10:D$241="Completed"))+SUMPRODUCT(($A$10:$A$241="Innovative")*(D$10:D$241="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$241="Innovative")*(D$10:D$241="Partial"))</f>
         <v>0</v>
@@ -20840,10 +20894,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="172" t="s">
+      <c r="A10" s="177" t="s">
         <v>810</v>
       </c>
-      <c r="B10" s="173"/>
+      <c r="B10" s="178"/>
       <c r="C10" s="8" t="s">
         <v>863</v>
       </c>
@@ -20930,10 +20984,10 @@
       <c r="F14" s="60"/>
     </row>
     <row r="15" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="172" t="s">
+      <c r="A15" s="177" t="s">
         <v>249</v>
       </c>
-      <c r="B15" s="173"/>
+      <c r="B15" s="178"/>
       <c r="C15" s="8" t="s">
         <v>89</v>
       </c>
@@ -21074,10 +21128,10 @@
       <c r="F22" s="60"/>
     </row>
     <row r="23" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="172" t="s">
+      <c r="A23" s="177" t="s">
         <v>257</v>
       </c>
-      <c r="B23" s="173"/>
+      <c r="B23" s="178"/>
       <c r="C23" s="8" t="s">
         <v>89</v>
       </c>
@@ -21218,10 +21272,10 @@
       <c r="F30" s="60"/>
     </row>
     <row r="31" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="172" t="s">
+      <c r="A31" s="177" t="s">
         <v>262</v>
       </c>
-      <c r="B31" s="173"/>
+      <c r="B31" s="178"/>
       <c r="C31" s="8" t="s">
         <v>89</v>
       </c>
@@ -21686,10 +21740,10 @@
       <c r="F56" s="60"/>
     </row>
     <row r="57" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="172" t="s">
+      <c r="A57" s="177" t="s">
         <v>288</v>
       </c>
-      <c r="B57" s="173"/>
+      <c r="B57" s="178"/>
       <c r="C57" s="73" t="s">
         <v>832</v>
       </c>
@@ -22064,10 +22118,10 @@
       <c r="F77" s="60"/>
     </row>
     <row r="78" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="172" t="s">
+      <c r="A78" s="177" t="s">
         <v>301</v>
       </c>
-      <c r="B78" s="173"/>
+      <c r="B78" s="178"/>
       <c r="C78" s="8" t="s">
         <v>89</v>
       </c>
@@ -23072,7 +23126,7 @@
       <c r="B2" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="174" t="s">
+      <c r="C2" s="172" t="s">
         <v>830</v>
       </c>
       <c r="D2" s="66">
@@ -23095,7 +23149,7 @@
       <c r="B3" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="175"/>
+      <c r="C3" s="173"/>
       <c r="D3" s="66">
         <f>SUMPRODUCT(($A$10:$A$177="Basic")*(D$10:D$177="Missing"))+0.5*SUMPRODUCT(($A$10:$A$177="Basic")*(D$10:D$177="Partial"))</f>
         <v>2</v>
@@ -23116,7 +23170,7 @@
       <c r="B4" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="175"/>
+      <c r="C4" s="173"/>
       <c r="D4" s="66">
         <f>SUMPRODUCT(($A$10:$A$177="Intermediate")*(D$10:D$177="Missing"))+0.5*SUMPRODUCT(($A$10:$A$177="Intermediate")*(D$10:D$177="Partial"))</f>
         <v>2</v>
@@ -23137,7 +23191,7 @@
       <c r="B5" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="175"/>
+      <c r="C5" s="173"/>
       <c r="D5" s="66">
         <f>SUMPRODUCT(($A$10:$A$177="Intermediate")*(D$10:D$177="Completed"))+SUMPRODUCT(($A$10:$A$177="Intermediate")*(D$10:D$177="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$177="Intermediate")*(D$10:D$177="Partial"))</f>
         <v>1</v>
@@ -23158,7 +23212,7 @@
       <c r="B6" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="175"/>
+      <c r="C6" s="173"/>
       <c r="D6" s="66">
         <f>SUMPRODUCT(($A$10:$A$177="Advanced")*(D$10:D$177="Missing"))+0.5*SUMPRODUCT(($A$10:$A$177="Advanced")*(D$10:D$177="Partial"))</f>
         <v>0</v>
@@ -23179,7 +23233,7 @@
       <c r="B7" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="175"/>
+      <c r="C7" s="173"/>
       <c r="D7" s="66">
         <f>SUMPRODUCT(($A$10:$A$177="Advanced")*(D$10:D$177="Completed"))+SUMPRODUCT(($A$10:$A$177="Advanced")*(D$10:D$177="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$177="Advanced")*(D$10:D$177="Partial"))</f>
         <v>0</v>
@@ -23200,7 +23254,7 @@
       <c r="B8" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="175"/>
+      <c r="C8" s="173"/>
       <c r="D8" s="66">
         <f>SUMPRODUCT(($A$10:$A$177="Professional")*(D$10:D$177="Completed"))+SUMPRODUCT(($A$10:$A$177="Professional")*(D$10:D$177="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$177="Professional")*(D$10:D$177="Partial"))</f>
         <v>0</v>
@@ -23215,11 +23269,11 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="177" t="s">
+      <c r="A9" s="175" t="s">
         <v>88</v>
       </c>
-      <c r="B9" s="178"/>
-      <c r="C9" s="176"/>
+      <c r="B9" s="176"/>
+      <c r="C9" s="174"/>
       <c r="D9" s="66">
         <f>SUMPRODUCT(($A$10:$A$177="Innovative")*(D$10:D$177="Completed"))+SUMPRODUCT(($A$10:$A$177="Innovative")*(D$10:D$177="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$177="Innovative")*(D$10:D$177="Partial"))</f>
         <v>0</v>
@@ -23234,10 +23288,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="172" t="s">
+      <c r="A10" s="177" t="s">
         <v>237</v>
       </c>
-      <c r="B10" s="173"/>
+      <c r="B10" s="178"/>
       <c r="C10" s="8" t="s">
         <v>89</v>
       </c>
@@ -23450,10 +23504,10 @@
       <c r="F21" s="60"/>
     </row>
     <row r="22" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="172" t="s">
+      <c r="A22" s="177" t="s">
         <v>534</v>
       </c>
-      <c r="B22" s="173"/>
+      <c r="B22" s="178"/>
       <c r="C22" s="8" t="s">
         <v>89</v>
       </c>
@@ -23612,10 +23666,10 @@
       <c r="F30" s="60"/>
     </row>
     <row r="31" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="172" t="s">
+      <c r="A31" s="177" t="s">
         <v>550</v>
       </c>
-      <c r="B31" s="173"/>
+      <c r="B31" s="178"/>
       <c r="C31" s="8" t="s">
         <v>89</v>
       </c>
@@ -23828,10 +23882,10 @@
       <c r="F42" s="60"/>
     </row>
     <row r="43" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="172" t="s">
+      <c r="A43" s="177" t="s">
         <v>661</v>
       </c>
-      <c r="B43" s="173"/>
+      <c r="B43" s="178"/>
       <c r="C43" s="8" t="s">
         <v>89</v>
       </c>
@@ -24120,7 +24174,7 @@
       <c r="B2" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="174" t="s">
+      <c r="C2" s="172" t="s">
         <v>384</v>
       </c>
       <c r="D2" s="66">
@@ -24143,7 +24197,7 @@
       <c r="B3" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="175"/>
+      <c r="C3" s="173"/>
       <c r="D3" s="66">
         <f>SUMPRODUCT(($A$10:$A$248="Basic")*(D$10:D$248="Missing"))+0.5*SUMPRODUCT(($A$10:$A$248="Basic")*(D$10:D$248="Partial"))</f>
         <v>0</v>
@@ -24164,7 +24218,7 @@
       <c r="B4" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="175"/>
+      <c r="C4" s="173"/>
       <c r="D4" s="66">
         <f>SUMPRODUCT(($A$10:$A$248="Intermediate")*(D$10:D$248="Missing"))+0.5*SUMPRODUCT(($A$10:$A$248="Intermediate")*(D$10:D$248="Partial"))</f>
         <v>0</v>
@@ -24185,7 +24239,7 @@
       <c r="B5" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="175"/>
+      <c r="C5" s="173"/>
       <c r="D5" s="66">
         <f>SUMPRODUCT(($A$10:$A$248="Intermediate")*(D$10:D$248="Completed"))+SUMPRODUCT(($A$10:$A$248="Intermediate")*(D$10:D$248="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$248="Intermediate")*(D$10:D$248="Partial"))</f>
         <v>1</v>
@@ -24206,7 +24260,7 @@
       <c r="B6" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="175"/>
+      <c r="C6" s="173"/>
       <c r="D6" s="66">
         <f>SUMPRODUCT(($A$10:$A$248="Advanced")*(D$10:D$248="Missing"))+0.5*SUMPRODUCT(($A$10:$A$248="Advanced")*(D$10:D$248="Partial"))</f>
         <v>0</v>
@@ -24227,7 +24281,7 @@
       <c r="B7" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="175"/>
+      <c r="C7" s="173"/>
       <c r="D7" s="66">
         <f>SUMPRODUCT(($A$10:$A$248="Advanced")*(D$10:D$248="Completed"))+SUMPRODUCT(($A$10:$A$248="Advanced")*(D$10:D$248="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$248="Advanced")*(D$10:D$248="Partial"))</f>
         <v>0</v>
@@ -24248,7 +24302,7 @@
       <c r="B8" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="175"/>
+      <c r="C8" s="173"/>
       <c r="D8" s="66">
         <f>SUMPRODUCT(($A$10:$A$248="Professional")*(D$10:D$248="Completed"))+SUMPRODUCT(($A$10:$A$248="Professional")*(D$10:D$248="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$248="Professional")*(D$10:D$248="Partial"))</f>
         <v>0</v>
@@ -24263,11 +24317,11 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="177" t="s">
+      <c r="A9" s="175" t="s">
         <v>88</v>
       </c>
-      <c r="B9" s="178"/>
-      <c r="C9" s="176"/>
+      <c r="B9" s="176"/>
+      <c r="C9" s="174"/>
       <c r="D9" s="66">
         <f>SUMPRODUCT(($A$10:$A$248="Innovative")*(D$10:D$248="Completed"))+SUMPRODUCT(($A$10:$A$248="Innovative")*(D$10:D$248="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$248="Innovative")*(D$10:D$248="Partial"))</f>
         <v>0</v>
@@ -24282,10 +24336,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="172" t="s">
+      <c r="A10" s="177" t="s">
         <v>385</v>
       </c>
-      <c r="B10" s="173"/>
+      <c r="B10" s="178"/>
       <c r="C10" s="8" t="s">
         <v>89</v>
       </c>
@@ -24390,10 +24444,10 @@
       <c r="F15" s="60"/>
     </row>
     <row r="16" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="172" t="s">
+      <c r="A16" s="177" t="s">
         <v>396</v>
       </c>
-      <c r="B16" s="173"/>
+      <c r="B16" s="178"/>
       <c r="C16" s="8" t="s">
         <v>89</v>
       </c>
@@ -24498,10 +24552,10 @@
       <c r="F21" s="60"/>
     </row>
     <row r="22" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="172" t="s">
+      <c r="A22" s="177" t="s">
         <v>407</v>
       </c>
-      <c r="B22" s="173"/>
+      <c r="B22" s="178"/>
       <c r="C22" s="8" t="s">
         <v>826</v>
       </c>
@@ -24624,10 +24678,10 @@
       <c r="F28" s="60"/>
     </row>
     <row r="29" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="172" t="s">
+      <c r="A29" s="177" t="s">
         <v>420</v>
       </c>
-      <c r="B29" s="173"/>
+      <c r="B29" s="178"/>
       <c r="C29" s="8" t="s">
         <v>824</v>
       </c>
@@ -24768,10 +24822,10 @@
       <c r="F36" s="60"/>
     </row>
     <row r="37" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="172" t="s">
+      <c r="A37" s="177" t="s">
         <v>435</v>
       </c>
-      <c r="B37" s="173"/>
+      <c r="B37" s="178"/>
       <c r="C37" s="8" t="s">
         <v>825</v>
       </c>
@@ -24894,10 +24948,10 @@
       <c r="F43" s="60"/>
     </row>
     <row r="44" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="172" t="s">
+      <c r="A44" s="177" t="s">
         <v>448</v>
       </c>
-      <c r="B44" s="173"/>
+      <c r="B44" s="178"/>
       <c r="C44" s="8" t="s">
         <v>89</v>
       </c>
@@ -25581,7 +25635,7 @@
       <c r="B2" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="174" t="s">
+      <c r="C2" s="172" t="s">
         <v>473</v>
       </c>
       <c r="D2" s="66">
@@ -25604,7 +25658,7 @@
       <c r="B3" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="175"/>
+      <c r="C3" s="173"/>
       <c r="D3" s="66">
         <f>SUMPRODUCT(($A$10:$A$227="Basic")*(D$10:D$227="Missing"))+0.5*SUMPRODUCT(($A$10:$A$227="Basic")*(D$10:D$227="Partial"))</f>
         <v>1</v>
@@ -25625,7 +25679,7 @@
       <c r="B4" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="175"/>
+      <c r="C4" s="173"/>
       <c r="D4" s="66">
         <f>SUMPRODUCT(($A$10:$A$227="Intermediate")*(D$10:D$227="Missing"))+0.5*SUMPRODUCT(($A$10:$A$227="Intermediate")*(D$10:D$227="Partial"))</f>
         <v>2</v>
@@ -25646,7 +25700,7 @@
       <c r="B5" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="175"/>
+      <c r="C5" s="173"/>
       <c r="D5" s="66">
         <f>SUMPRODUCT(($A$10:$A$227="Intermediate")*(D$10:D$227="Completed"))+SUMPRODUCT(($A$10:$A$227="Intermediate")*(D$10:D$227="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$227="Intermediate")*(D$10:D$227="Partial"))</f>
         <v>6</v>
@@ -25667,7 +25721,7 @@
       <c r="B6" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="175"/>
+      <c r="C6" s="173"/>
       <c r="D6" s="66">
         <f>SUMPRODUCT(($A$10:$A$227="Advanced")*(D$10:D$227="Missing"))+0.5*SUMPRODUCT(($A$10:$A$227="Advanced")*(D$10:D$227="Partial"))</f>
         <v>0</v>
@@ -25688,7 +25742,7 @@
       <c r="B7" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="175"/>
+      <c r="C7" s="173"/>
       <c r="D7" s="66">
         <f>SUMPRODUCT(($A$10:$A$227="Advanced")*(D$10:D$227="Completed"))+SUMPRODUCT(($A$10:$A$227="Advanced")*(D$10:D$227="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$227="Advanced")*(D$10:D$227="Partial"))</f>
         <v>0</v>
@@ -25709,7 +25763,7 @@
       <c r="B8" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="175"/>
+      <c r="C8" s="173"/>
       <c r="D8" s="66">
         <f>SUMPRODUCT(($A$10:$A$227="Professional")*(D$10:D$227="Completed"))+SUMPRODUCT(($A$10:$A$227="Professional")*(D$10:D$227="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$227="Professional")*(D$10:D$227="Partial"))</f>
         <v>0</v>
@@ -25724,11 +25778,11 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="177" t="s">
+      <c r="A9" s="175" t="s">
         <v>88</v>
       </c>
-      <c r="B9" s="178"/>
-      <c r="C9" s="176"/>
+      <c r="B9" s="176"/>
+      <c r="C9" s="174"/>
       <c r="D9" s="66">
         <f>SUMPRODUCT(($A$10:$A$227="Innovative")*(D$10:D$227="Completed"))+SUMPRODUCT(($A$10:$A$227="Innovative")*(D$10:D$227="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$227="Innovative")*(D$10:D$227="Partial"))</f>
         <v>0</v>
@@ -25743,10 +25797,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="172" t="s">
+      <c r="A10" s="177" t="s">
         <v>474</v>
       </c>
-      <c r="B10" s="173"/>
+      <c r="B10" s="178"/>
       <c r="C10" s="8" t="s">
         <v>89</v>
       </c>
@@ -26087,10 +26141,10 @@
       <c r="F28" s="60"/>
     </row>
     <row r="29" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="172" t="s">
+      <c r="A29" s="177" t="s">
         <v>511</v>
       </c>
-      <c r="B29" s="173"/>
+      <c r="B29" s="178"/>
       <c r="C29" s="8" t="s">
         <v>821</v>
       </c>
@@ -26303,10 +26357,10 @@
       <c r="F40" s="60"/>
     </row>
     <row r="41" spans="1:6" s="26" customFormat="1" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="172" t="s">
+      <c r="A41" s="177" t="s">
         <v>114</v>
       </c>
-      <c r="B41" s="173"/>
+      <c r="B41" s="178"/>
       <c r="C41" s="8" t="s">
         <v>89</v>
       </c>
@@ -26465,10 +26519,10 @@
       <c r="F49" s="60"/>
     </row>
     <row r="50" spans="1:6" s="26" customFormat="1" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="172" t="s">
+      <c r="A50" s="177" t="s">
         <v>589</v>
       </c>
-      <c r="B50" s="173"/>
+      <c r="B50" s="178"/>
       <c r="C50" s="73" t="s">
         <v>822</v>
       </c>
@@ -26554,7 +26608,7 @@
       </c>
       <c r="F54" s="60"/>
     </row>
-    <row r="55" spans="1:6" s="26" customFormat="1" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" s="26" customFormat="1" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="69" t="s">
         <v>98</v>
       </c>
@@ -26994,8 +27048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F116"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView topLeftCell="A16" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -27037,12 +27091,12 @@
       <c r="B2" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="174" t="s">
+      <c r="C2" s="172" t="s">
         <v>610</v>
       </c>
       <c r="D2" s="66">
         <f>SUMPRODUCT(($A$10:$A$240="Required")*(D$10:D$240="Missing"))+0.5*SUMPRODUCT(($A$10:$A$240="Required")*(D$10:D$240="Partial"))</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E2" s="66">
         <f>SUMPRODUCT(($A$10:$A$240="Required")*(E$10:E$240="Missing"))+0.5*SUMPRODUCT(($A$10:$A$240="Required")*(E$10:E$240="Partial"))</f>
@@ -27060,7 +27114,7 @@
       <c r="B3" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="175"/>
+      <c r="C3" s="173"/>
       <c r="D3" s="66">
         <f>SUMPRODUCT(($A$10:$A$240="Basic")*(D$10:D$240="Missing"))+0.5*SUMPRODUCT(($A$10:$A$240="Basic")*(D$10:D$240="Partial"))</f>
         <v>3</v>
@@ -27081,7 +27135,7 @@
       <c r="B4" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="175"/>
+      <c r="C4" s="173"/>
       <c r="D4" s="66">
         <f>SUMPRODUCT(($A$10:$A$240="Intermediate")*(D$10:D$240="Missing"))+0.5*SUMPRODUCT(($A$10:$A$240="Intermediate")*(D$10:D$240="Partial"))</f>
         <v>3</v>
@@ -27102,7 +27156,7 @@
       <c r="B5" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="175"/>
+      <c r="C5" s="173"/>
       <c r="D5" s="66">
         <f>SUMPRODUCT(($A$10:$A$240="Intermediate")*(D$10:D$240="Completed"))+SUMPRODUCT(($A$10:$A$240="Intermediate")*(D$10:D$240="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$240="Intermediate")*(D$10:D$240="Partial"))</f>
         <v>0</v>
@@ -27123,7 +27177,7 @@
       <c r="B6" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="175"/>
+      <c r="C6" s="173"/>
       <c r="D6" s="66">
         <f>SUMPRODUCT(($A$10:$A$240="Advanced")*(D$10:D$240="Missing"))+0.5*SUMPRODUCT(($A$10:$A$240="Advanced")*(D$10:D$240="Partial"))</f>
         <v>0</v>
@@ -27144,7 +27198,7 @@
       <c r="B7" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="175"/>
+      <c r="C7" s="173"/>
       <c r="D7" s="66">
         <f>SUMPRODUCT(($A$10:$A$240="Advanced")*(D$10:D$240="Completed"))+SUMPRODUCT(($A$10:$A$240="Advanced")*(D$10:D$240="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$240="Advanced")*(D$10:D$240="Partial"))</f>
         <v>0</v>
@@ -27165,7 +27219,7 @@
       <c r="B8" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="175"/>
+      <c r="C8" s="173"/>
       <c r="D8" s="66">
         <f>SUMPRODUCT(($A$10:$A$240="Professional")*(D$10:D$240="Completed"))+SUMPRODUCT(($A$10:$A$240="Professional")*(D$10:D$240="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$240="Professional")*(D$10:D$240="Partial"))</f>
         <v>0</v>
@@ -27180,11 +27234,11 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="177" t="s">
+      <c r="A9" s="175" t="s">
         <v>88</v>
       </c>
-      <c r="B9" s="178"/>
-      <c r="C9" s="176"/>
+      <c r="B9" s="176"/>
+      <c r="C9" s="174"/>
       <c r="D9" s="66">
         <f>SUMPRODUCT(($A$10:$A$240="Innovative")*(D$10:D$240="Completed"))+SUMPRODUCT(($A$10:$A$240="Innovative")*(D$10:D$240="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$240="Innovative")*(D$10:D$240="Partial"))</f>
         <v>0</v>
@@ -27199,10 +27253,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="172" t="s">
+      <c r="A10" s="177" t="s">
         <v>611</v>
       </c>
-      <c r="B10" s="173"/>
+      <c r="B10" s="178"/>
       <c r="C10" s="73" t="s">
         <v>815</v>
       </c>
@@ -27415,10 +27469,10 @@
       <c r="F21" s="60"/>
     </row>
     <row r="22" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="172" t="s">
+      <c r="A22" s="177" t="s">
         <v>634</v>
       </c>
-      <c r="B22" s="173"/>
+      <c r="B22" s="178"/>
       <c r="C22" s="8" t="s">
         <v>89</v>
       </c>
@@ -27443,7 +27497,7 @@
         <v>636</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>74</v>
@@ -27461,7 +27515,7 @@
         <v>638</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>74</v>
@@ -27631,10 +27685,10 @@
       <c r="F33" s="60"/>
     </row>
     <row r="34" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="172" t="s">
+      <c r="A34" s="177" t="s">
         <v>811</v>
       </c>
-      <c r="B34" s="173"/>
+      <c r="B34" s="178"/>
       <c r="C34" s="8" t="s">
         <v>816</v>
       </c>
@@ -27757,10 +27811,10 @@
       <c r="F40" s="60"/>
     </row>
     <row r="41" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="172" t="s">
+      <c r="A41" s="177" t="s">
         <v>680</v>
       </c>
-      <c r="B41" s="173"/>
+      <c r="B41" s="178"/>
       <c r="C41" s="8" t="s">
         <v>89</v>
       </c>
@@ -28171,8 +28225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+    <sheetView topLeftCell="A49" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -28188,65 +28242,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="179" t="s">
+      <c r="A1" s="189" t="s">
         <v>705</v>
       </c>
       <c r="B1" s="75"/>
-      <c r="C1" s="194" t="s">
+      <c r="C1" s="179" t="s">
         <v>689</v>
       </c>
-      <c r="D1" s="195"/>
-      <c r="E1" s="194" t="s">
+      <c r="D1" s="180"/>
+      <c r="E1" s="179" t="s">
         <v>690</v>
       </c>
-      <c r="F1" s="195"/>
-      <c r="G1" s="194" t="s">
+      <c r="F1" s="180"/>
+      <c r="G1" s="179" t="s">
         <v>691</v>
       </c>
-      <c r="H1" s="195"/>
+      <c r="H1" s="180"/>
     </row>
     <row r="2" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="180"/>
+      <c r="A2" s="190"/>
       <c r="B2" s="75"/>
-      <c r="C2" s="196" t="s">
+      <c r="C2" s="181" t="s">
         <v>688</v>
       </c>
-      <c r="D2" s="197"/>
-      <c r="E2" s="196" t="s">
+      <c r="D2" s="182"/>
+      <c r="E2" s="181" t="s">
         <v>688</v>
       </c>
-      <c r="F2" s="197"/>
-      <c r="G2" s="196" t="s">
+      <c r="F2" s="182"/>
+      <c r="G2" s="181" t="s">
         <v>688</v>
       </c>
-      <c r="H2" s="197"/>
-      <c r="J2" s="182" t="s">
+      <c r="H2" s="182"/>
+      <c r="J2" s="192" t="s">
         <v>707</v>
       </c>
-      <c r="K2" s="183"/>
-      <c r="L2" s="184"/>
+      <c r="K2" s="193"/>
+      <c r="L2" s="194"/>
     </row>
     <row r="3" spans="1:12" ht="22.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="181"/>
+      <c r="A3" s="191"/>
       <c r="B3" s="76"/>
-      <c r="C3" s="192">
+      <c r="C3" s="183">
         <f>MAX(0,MIN(1,IF((A6+C6) &lt;= 0.95, ROUND(A6+C6,2), FLOOR((0.95+(A6+C6-0.95)/5),2))))</f>
-        <v>0.18</v>
-      </c>
-      <c r="D3" s="193"/>
-      <c r="E3" s="192">
+        <v>0.23</v>
+      </c>
+      <c r="D3" s="184"/>
+      <c r="E3" s="183">
         <f>MAX(0,MIN(1,IF((A6+E6) &lt;= 0.95, ROUND(A6+E6,2), FLOOR((0.95+(A6+E6-0.95)/5),2))))</f>
         <v>0</v>
       </c>
-      <c r="F3" s="193"/>
-      <c r="G3" s="192">
+      <c r="F3" s="184"/>
+      <c r="G3" s="183">
         <f>MAX(0,MIN(1,IF((A6+G6) &lt;= 0.95, ROUND(A6+G6,2), FLOOR((0.95+(A6+G6-0.95)/5),2))))</f>
-        <v>0.23</v>
-      </c>
-      <c r="H3" s="193"/>
-      <c r="J3" s="185"/>
-      <c r="K3" s="186"/>
-      <c r="L3" s="187"/>
+        <v>0.25</v>
+      </c>
+      <c r="H3" s="184"/>
+      <c r="J3" s="195"/>
+      <c r="K3" s="196"/>
+      <c r="L3" s="197"/>
     </row>
     <row r="4" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
@@ -28263,19 +28317,19 @@
         <v>692</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="145" t="s">
+      <c r="C5" s="118" t="s">
         <v>693</v>
       </c>
-      <c r="D5" s="147"/>
-      <c r="E5" s="145" t="s">
+      <c r="D5" s="120"/>
+      <c r="E5" s="118" t="s">
         <v>694</v>
       </c>
-      <c r="F5" s="147"/>
-      <c r="G5" s="145" t="s">
+      <c r="F5" s="120"/>
+      <c r="G5" s="118" t="s">
         <v>695</v>
       </c>
-      <c r="H5" s="147"/>
-      <c r="J5" s="139" t="s">
+      <c r="H5" s="120"/>
+      <c r="J5" s="127" t="s">
         <v>721</v>
       </c>
       <c r="K5" s="31"/>
@@ -28286,25 +28340,25 @@
     <row r="6" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="78">
         <f>'Game Data'!$I$22+Submission!$E$16</f>
-        <v>0.85</v>
+        <v>0.75</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="189">
+      <c r="C6" s="186">
         <f>D15+D24+D33+D42+D51+D60</f>
-        <v>-0.6725000000000001</v>
-      </c>
-      <c r="D6" s="190"/>
-      <c r="E6" s="189">
+        <v>-0.52250000000000008</v>
+      </c>
+      <c r="D6" s="187"/>
+      <c r="E6" s="186">
         <f>F15+F24+F33+F42+F51+F60</f>
-        <v>-0.95250000000000001</v>
-      </c>
-      <c r="F6" s="190"/>
-      <c r="G6" s="189">
+        <v>-0.82750000000000012</v>
+      </c>
+      <c r="F6" s="187"/>
+      <c r="G6" s="186">
         <f>H15+H24+H33+H42+H51+H60</f>
-        <v>-0.61749999999999994</v>
-      </c>
-      <c r="H6" s="190"/>
-      <c r="J6" s="140"/>
+        <v>-0.505</v>
+      </c>
+      <c r="H6" s="187"/>
+      <c r="J6" s="128"/>
       <c r="K6" s="31"/>
       <c r="L6" s="104" t="s">
         <v>714</v>
@@ -28313,19 +28367,19 @@
     <row r="7" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="11"/>
-      <c r="C7" s="191" t="s">
+      <c r="C7" s="188" t="s">
         <v>696</v>
       </c>
-      <c r="D7" s="191"/>
-      <c r="E7" s="191" t="s">
+      <c r="D7" s="188"/>
+      <c r="E7" s="188" t="s">
         <v>697</v>
       </c>
-      <c r="F7" s="191"/>
-      <c r="G7" s="191" t="s">
+      <c r="F7" s="188"/>
+      <c r="G7" s="188" t="s">
         <v>698</v>
       </c>
-      <c r="H7" s="191"/>
-      <c r="J7" s="140"/>
+      <c r="H7" s="188"/>
+      <c r="J7" s="128"/>
       <c r="K7" s="105"/>
       <c r="L7" s="104" t="s">
         <v>715</v>
@@ -28356,7 +28410,7 @@
       <c r="H8" s="87" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="140"/>
+      <c r="J8" s="128"/>
       <c r="K8" s="105"/>
       <c r="L8" s="104" t="s">
         <v>716</v>
@@ -28392,7 +28446,7 @@
         <f t="shared" ref="H9:H14" si="2">B9*G9</f>
         <v>0</v>
       </c>
-      <c r="J9" s="140"/>
+      <c r="J9" s="128"/>
       <c r="K9" s="105"/>
       <c r="L9" s="104" t="s">
         <v>717</v>
@@ -28405,30 +28459,30 @@
       </c>
       <c r="B10" s="11">
         <f>TCRs!$D$3</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C10" s="82">
         <v>-0.02</v>
       </c>
       <c r="D10" s="97">
         <f t="shared" si="0"/>
-        <v>-0.08</v>
+        <v>-0.04</v>
       </c>
       <c r="E10" s="84">
         <v>-0.01</v>
       </c>
       <c r="F10" s="97">
         <f t="shared" si="1"/>
-        <v>-0.04</v>
+        <v>-0.02</v>
       </c>
       <c r="G10" s="100">
         <v>-5.0000000000000001E-3</v>
       </c>
       <c r="H10" s="97">
         <f t="shared" si="2"/>
-        <v>-0.02</v>
-      </c>
-      <c r="J10" s="140"/>
+        <v>-0.01</v>
+      </c>
+      <c r="J10" s="128"/>
       <c r="K10" s="105"/>
       <c r="L10" s="104" t="s">
         <v>718</v>
@@ -28441,30 +28495,30 @@
       </c>
       <c r="B11" s="11">
         <f>TCRs!$D$4</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11" s="82">
         <v>-0.01</v>
       </c>
       <c r="D11" s="97">
         <f t="shared" si="0"/>
-        <v>-0.02</v>
+        <v>-0.01</v>
       </c>
       <c r="E11" s="100">
         <v>-5.0000000000000001E-3</v>
       </c>
       <c r="F11" s="97">
         <f t="shared" si="1"/>
-        <v>-0.01</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="G11" s="80">
         <v>-2.5000000000000001E-3</v>
       </c>
       <c r="H11" s="97">
         <f t="shared" si="2"/>
-        <v>-5.0000000000000001E-3</v>
-      </c>
-      <c r="J11" s="140"/>
+        <v>-2.5000000000000001E-3</v>
+      </c>
+      <c r="J11" s="128"/>
       <c r="K11" s="105"/>
       <c r="L11" s="104" t="s">
         <v>719</v>
@@ -28500,7 +28554,7 @@
         <f t="shared" si="2"/>
         <v>1.7500000000000002E-2</v>
       </c>
-      <c r="J12" s="141"/>
+      <c r="J12" s="129"/>
       <c r="K12" s="105"/>
       <c r="L12" s="103" t="s">
         <v>720</v>
@@ -28576,38 +28630,38 @@
       </c>
       <c r="D15" s="99">
         <f>SUM(D9:D14)</f>
-        <v>-8.2500000000000004E-2</v>
+        <v>-3.2500000000000001E-2</v>
       </c>
       <c r="E15" s="79" t="s">
         <v>16</v>
       </c>
       <c r="F15" s="99">
         <f>SUM(F9:F14)</f>
-        <v>-3.2500000000000001E-2</v>
+        <v>-7.4999999999999997E-3</v>
       </c>
       <c r="G15" s="79" t="s">
         <v>16</v>
       </c>
       <c r="H15" s="99">
         <f>SUM(H9:H14)</f>
-        <v>-7.4999999999999997E-3</v>
+        <v>5.000000000000001E-3</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="11"/>
-      <c r="C16" s="188" t="s">
+      <c r="C16" s="185" t="s">
         <v>696</v>
       </c>
-      <c r="D16" s="188"/>
-      <c r="E16" s="188" t="s">
+      <c r="D16" s="185"/>
+      <c r="E16" s="185" t="s">
         <v>697</v>
       </c>
-      <c r="F16" s="188"/>
-      <c r="G16" s="188" t="s">
+      <c r="F16" s="185"/>
+      <c r="G16" s="185" t="s">
         <v>698</v>
       </c>
-      <c r="H16" s="188"/>
+      <c r="H16" s="185"/>
     </row>
     <row r="17" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
@@ -28849,18 +28903,18 @@
     <row r="25" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="11"/>
-      <c r="C25" s="188" t="s">
+      <c r="C25" s="185" t="s">
         <v>696</v>
       </c>
-      <c r="D25" s="188"/>
-      <c r="E25" s="188" t="s">
+      <c r="D25" s="185"/>
+      <c r="E25" s="185" t="s">
         <v>697</v>
       </c>
-      <c r="F25" s="188"/>
-      <c r="G25" s="188" t="s">
+      <c r="F25" s="185"/>
+      <c r="G25" s="185" t="s">
         <v>698</v>
       </c>
-      <c r="H25" s="188"/>
+      <c r="H25" s="185"/>
     </row>
     <row r="26" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
@@ -29102,18 +29156,18 @@
     <row r="34" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3"/>
       <c r="B34" s="11"/>
-      <c r="C34" s="188" t="s">
+      <c r="C34" s="185" t="s">
         <v>696</v>
       </c>
-      <c r="D34" s="188"/>
-      <c r="E34" s="188" t="s">
+      <c r="D34" s="185"/>
+      <c r="E34" s="185" t="s">
         <v>697</v>
       </c>
-      <c r="F34" s="188"/>
-      <c r="G34" s="188" t="s">
+      <c r="F34" s="185"/>
+      <c r="G34" s="185" t="s">
         <v>698</v>
       </c>
-      <c r="H34" s="188"/>
+      <c r="H34" s="185"/>
     </row>
     <row r="35" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
@@ -29355,18 +29409,18 @@
     <row r="43" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3"/>
       <c r="B43" s="11"/>
-      <c r="C43" s="188" t="s">
+      <c r="C43" s="185" t="s">
         <v>696</v>
       </c>
-      <c r="D43" s="188"/>
-      <c r="E43" s="188" t="s">
+      <c r="D43" s="185"/>
+      <c r="E43" s="185" t="s">
         <v>697</v>
       </c>
-      <c r="F43" s="188"/>
-      <c r="G43" s="188" t="s">
+      <c r="F43" s="185"/>
+      <c r="G43" s="185" t="s">
         <v>698</v>
       </c>
-      <c r="H43" s="188"/>
+      <c r="H43" s="185"/>
     </row>
     <row r="44" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
@@ -29608,18 +29662,18 @@
     <row r="52" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="3"/>
       <c r="B52" s="11"/>
-      <c r="C52" s="188" t="s">
+      <c r="C52" s="185" t="s">
         <v>696</v>
       </c>
-      <c r="D52" s="188"/>
-      <c r="E52" s="188" t="s">
+      <c r="D52" s="185"/>
+      <c r="E52" s="185" t="s">
         <v>697</v>
       </c>
-      <c r="F52" s="188"/>
-      <c r="G52" s="188" t="s">
+      <c r="F52" s="185"/>
+      <c r="G52" s="185" t="s">
         <v>698</v>
       </c>
-      <c r="H52" s="188"/>
+      <c r="H52" s="185"/>
     </row>
     <row r="53" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
@@ -29654,28 +29708,28 @@
       </c>
       <c r="B54" s="57">
         <f>ACRs!$D$2</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C54" s="81">
         <v>-0.05</v>
       </c>
       <c r="D54" s="96">
         <f t="shared" ref="D54:D59" si="15">B54*C54</f>
-        <v>-0.2</v>
+        <v>-0.1</v>
       </c>
       <c r="E54" s="83">
         <v>-0.05</v>
       </c>
       <c r="F54" s="96">
         <f t="shared" ref="F54:F59" si="16">B54*E54</f>
-        <v>-0.2</v>
+        <v>-0.1</v>
       </c>
       <c r="G54" s="83">
         <v>-0.05</v>
       </c>
       <c r="H54" s="96">
         <f t="shared" ref="H54:H59" si="17">B54*G54</f>
-        <v>-0.2</v>
+        <v>-0.1</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -29841,45 +29895,25 @@
       </c>
       <c r="D60" s="99">
         <f>SUM(D54:D59)</f>
-        <v>-0.245</v>
+        <v>-0.14500000000000002</v>
       </c>
       <c r="E60" s="79" t="s">
         <v>16</v>
       </c>
       <c r="F60" s="99">
         <f>SUM(F54:F59)</f>
-        <v>-0.245</v>
+        <v>-0.14500000000000002</v>
       </c>
       <c r="G60" s="79" t="s">
         <v>16</v>
       </c>
       <c r="H60" s="99">
         <f>SUM(H54:H59)</f>
-        <v>-0.245</v>
+        <v>-0.14500000000000002</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="J2:L3"/>
     <mergeCell ref="J5:J12"/>
@@ -29896,6 +29930,26 @@
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>